<commit_message>
End of day with xlsx update
</commit_message>
<xml_diff>
--- a/Rolleston Workzones_ps_140327.xlsx
+++ b/Rolleston Workzones_ps_140327.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael Kerkow\Documents\GitHub\14002-RollestonSim\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="60" windowWidth="15360" windowHeight="8370" activeTab="4"/>
   </bookViews>
@@ -11,15 +16,16 @@
     <sheet name="SimioInputs" sheetId="7" r:id="rId2"/>
     <sheet name="Weather" sheetId="3" r:id="rId3"/>
     <sheet name="Equipment" sheetId="4" r:id="rId4"/>
-    <sheet name="ROM" sheetId="5" r:id="rId5"/>
-    <sheet name="CHF" sheetId="6" r:id="rId6"/>
+    <sheet name="Shifts" sheetId="8" r:id="rId5"/>
+    <sheet name="ROM" sheetId="5" r:id="rId6"/>
+    <sheet name="CHF" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="263">
   <si>
     <t>Work Zone</t>
   </si>
@@ -757,17 +763,70 @@
   </si>
   <si>
     <t>Hopper empty - stop outfeed</t>
+  </si>
+  <si>
+    <t>First Break Start</t>
+  </si>
+  <si>
+    <t>First break End</t>
+  </si>
+  <si>
+    <t>Second Break Start</t>
+  </si>
+  <si>
+    <t>Second break End</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>Delay</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Day Shift Staff Arrive</t>
+  </si>
+  <si>
+    <t>Excavator Stops Loading Trucks, Truck Cycles Stop</t>
+  </si>
+  <si>
+    <t>Excavator product begins, Trucks Cycles Begin</t>
+  </si>
+  <si>
+    <t>Excavator Stops Loading Trucks, Trucks Cycles Stop</t>
+  </si>
+  <si>
+    <t>Night Shift</t>
+  </si>
+  <si>
+    <t>Day Shift</t>
+  </si>
+  <si>
+    <t>Preshift Finishes, Excavator Product Begin, Trucks Cycles Begin</t>
+  </si>
+  <si>
+    <t>Night Shift Staff Arrive</t>
+  </si>
+  <si>
+    <t>Day Shift Ends</t>
+  </si>
+  <si>
+    <t>Night Shift Ends</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+  <numFmts count="6">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="[$-409]h:mm:ss\ AM/PM;@"/>
+    <numFmt numFmtId="168" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -1409,7 +1468,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="209">
+  <cellXfs count="217">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="6" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1763,6 +1822,26 @@
     <xf numFmtId="9" fontId="0" fillId="11" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Comma 11 2" xfId="8"/>
@@ -1839,7 +1918,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1874,7 +1953,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -8399,7 +8478,7 @@
   <dimension ref="A1:N55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="H9" sqref="H9:N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12324,10 +12403,655 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:G29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="7" max="7" width="58.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>250</v>
+      </c>
+      <c r="D3" t="s">
+        <v>184</v>
+      </c>
+      <c r="F3" s="196" t="s">
+        <v>258</v>
+      </c>
+      <c r="G3" s="196" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="209">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="B4" s="210" t="s">
+        <v>253</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <f>C4*60</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="214">
+        <f>A4</f>
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="G4" s="215" t="str">
+        <f>B4</f>
+        <v>Day Shift Staff Arrive</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="209">
+        <v>0.25</v>
+      </c>
+      <c r="B5" s="210"/>
+      <c r="F5" s="214"/>
+      <c r="G5" s="215"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="211">
+        <v>0.2638888888888889</v>
+      </c>
+      <c r="B6" s="210" t="s">
+        <v>259</v>
+      </c>
+      <c r="C6" s="212">
+        <f>(A6-A4)*24</f>
+        <v>0.50000000000000022</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ref="D6:D29" si="0">C6*60</f>
+        <v>30.000000000000014</v>
+      </c>
+      <c r="F6" s="214">
+        <f t="shared" ref="F6:F29" si="1">A6</f>
+        <v>0.2638888888888889</v>
+      </c>
+      <c r="G6" s="215" t="str">
+        <f t="shared" ref="G6:G29" si="2">B6</f>
+        <v>Preshift Finishes, Excavator Product Begin, Trucks Cycles Begin</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="213">
+        <v>0.41145833333333331</v>
+      </c>
+      <c r="B7" s="210" t="s">
+        <v>254</v>
+      </c>
+      <c r="C7" s="212">
+        <f>(A7-A6)*24</f>
+        <v>3.5416666666666661</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>212.49999999999997</v>
+      </c>
+      <c r="F7" s="214">
+        <f t="shared" si="1"/>
+        <v>0.41145833333333331</v>
+      </c>
+      <c r="G7" s="215" t="str">
+        <f t="shared" si="2"/>
+        <v>Excavator Stops Loading Trucks, Truck Cycles Stop</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="213">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="B8" s="210" t="s">
+        <v>246</v>
+      </c>
+      <c r="C8" s="212">
+        <f t="shared" ref="C8:C29" si="3">(A8-A7)*24</f>
+        <v>0.12500000000000089</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>7.5000000000000533</v>
+      </c>
+      <c r="E8" s="216">
+        <f>(A8-A5)*24</f>
+        <v>4</v>
+      </c>
+      <c r="F8" s="214">
+        <f t="shared" si="1"/>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="G8" s="215" t="str">
+        <f t="shared" si="2"/>
+        <v>First Break Start</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="213">
+        <v>0.4375</v>
+      </c>
+      <c r="B9" s="210" t="s">
+        <v>247</v>
+      </c>
+      <c r="C9" s="212">
+        <f t="shared" si="3"/>
+        <v>0.49999999999999956</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>29.999999999999972</v>
+      </c>
+      <c r="F9" s="214">
+        <f t="shared" si="1"/>
+        <v>0.4375</v>
+      </c>
+      <c r="G9" s="215" t="str">
+        <f t="shared" si="2"/>
+        <v>First break End</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="213">
+        <v>0.44270833333333331</v>
+      </c>
+      <c r="B10" s="210" t="s">
+        <v>255</v>
+      </c>
+      <c r="C10" s="212">
+        <f t="shared" si="3"/>
+        <v>0.12499999999999956</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>7.4999999999999734</v>
+      </c>
+      <c r="F10" s="214">
+        <f t="shared" si="1"/>
+        <v>0.44270833333333331</v>
+      </c>
+      <c r="G10" s="215" t="str">
+        <f t="shared" si="2"/>
+        <v>Excavator product begins, Trucks Cycles Begin</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="213">
+        <v>0.578125</v>
+      </c>
+      <c r="B11" s="210" t="s">
+        <v>256</v>
+      </c>
+      <c r="C11" s="212">
+        <f t="shared" si="3"/>
+        <v>3.2500000000000004</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>195.00000000000003</v>
+      </c>
+      <c r="F11" s="214">
+        <f t="shared" si="1"/>
+        <v>0.578125</v>
+      </c>
+      <c r="G11" s="215" t="str">
+        <f t="shared" si="2"/>
+        <v>Excavator Stops Loading Trucks, Trucks Cycles Stop</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="213">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="B12" s="210" t="s">
+        <v>248</v>
+      </c>
+      <c r="C12" s="212">
+        <f t="shared" si="3"/>
+        <v>0.12500000000000089</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>7.5000000000000533</v>
+      </c>
+      <c r="E12" s="216">
+        <f>(A12-A9)*24</f>
+        <v>3.5000000000000009</v>
+      </c>
+      <c r="F12" s="214">
+        <f t="shared" si="1"/>
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="G12" s="215" t="str">
+        <f t="shared" si="2"/>
+        <v>Second Break Start</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="213">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="B13" s="210" t="s">
+        <v>249</v>
+      </c>
+      <c r="C13" s="212">
+        <f t="shared" si="3"/>
+        <v>0.49999999999999822</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>29.999999999999893</v>
+      </c>
+      <c r="F13" s="214">
+        <f t="shared" si="1"/>
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="G13" s="215" t="str">
+        <f t="shared" si="2"/>
+        <v>Second break End</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="213">
+        <v>0.609375</v>
+      </c>
+      <c r="B14" s="210" t="s">
+        <v>255</v>
+      </c>
+      <c r="C14" s="212">
+        <f t="shared" si="3"/>
+        <v>0.12500000000000089</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>7.5000000000000533</v>
+      </c>
+      <c r="F14" s="214">
+        <f t="shared" si="1"/>
+        <v>0.609375</v>
+      </c>
+      <c r="G14" s="215" t="str">
+        <f t="shared" si="2"/>
+        <v>Excavator product begins, Trucks Cycles Begin</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="213">
+        <v>0.74652777777777779</v>
+      </c>
+      <c r="B15" s="210" t="s">
+        <v>256</v>
+      </c>
+      <c r="C15" s="212">
+        <f>(A15-A14)*24</f>
+        <v>3.291666666666667</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>197.50000000000003</v>
+      </c>
+      <c r="F15" s="214">
+        <f t="shared" si="1"/>
+        <v>0.74652777777777779</v>
+      </c>
+      <c r="G15" s="215" t="str">
+        <f t="shared" si="2"/>
+        <v>Excavator Stops Loading Trucks, Trucks Cycles Stop</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="213">
+        <v>0.75</v>
+      </c>
+      <c r="B16" s="210" t="s">
+        <v>261</v>
+      </c>
+      <c r="C16" s="212">
+        <f>(A16-A15)*24*60</f>
+        <v>4.9999999999999822</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>299.99999999999892</v>
+      </c>
+      <c r="E16" s="216">
+        <f>(A16-A13)*24</f>
+        <v>3.5000000000000009</v>
+      </c>
+      <c r="F16" s="214">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="G16" s="215" t="str">
+        <f t="shared" si="2"/>
+        <v>Day Shift Ends</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="213"/>
+      <c r="B17" s="210"/>
+      <c r="C17" s="212"/>
+      <c r="F17" s="196" t="s">
+        <v>257</v>
+      </c>
+      <c r="G17" s="196" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="213">
+        <v>0.74305555555555547</v>
+      </c>
+      <c r="B18" s="210" t="s">
+        <v>260</v>
+      </c>
+      <c r="C18" s="212"/>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F18" s="214">
+        <f t="shared" si="1"/>
+        <v>0.74305555555555547</v>
+      </c>
+      <c r="G18" s="215" t="str">
+        <f t="shared" si="2"/>
+        <v>Night Shift Staff Arrive</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="213">
+        <v>0.76388888888888884</v>
+      </c>
+      <c r="B19" s="210" t="s">
+        <v>259</v>
+      </c>
+      <c r="C19" s="212">
+        <f t="shared" si="3"/>
+        <v>0.50000000000000089</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>30.000000000000053</v>
+      </c>
+      <c r="F19" s="214">
+        <f t="shared" si="1"/>
+        <v>0.76388888888888884</v>
+      </c>
+      <c r="G19" s="215" t="str">
+        <f t="shared" si="2"/>
+        <v>Preshift Finishes, Excavator Product Begin, Trucks Cycles Begin</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="213">
+        <v>0.91145833333333337</v>
+      </c>
+      <c r="B20" s="210" t="s">
+        <v>254</v>
+      </c>
+      <c r="C20" s="212">
+        <f t="shared" si="3"/>
+        <v>3.5416666666666687</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>212.50000000000011</v>
+      </c>
+      <c r="F20" s="214">
+        <f t="shared" si="1"/>
+        <v>0.91145833333333337</v>
+      </c>
+      <c r="G20" s="215" t="str">
+        <f t="shared" si="2"/>
+        <v>Excavator Stops Loading Trucks, Truck Cycles Stop</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="213">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="B21" s="210" t="s">
+        <v>246</v>
+      </c>
+      <c r="C21" s="212">
+        <f t="shared" si="3"/>
+        <v>0.12499999999999822</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>7.4999999999998934</v>
+      </c>
+      <c r="F21" s="214">
+        <f t="shared" si="1"/>
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="G21" s="215" t="str">
+        <f t="shared" si="2"/>
+        <v>First Break Start</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="213">
+        <v>0.9375</v>
+      </c>
+      <c r="B22" s="210" t="s">
+        <v>247</v>
+      </c>
+      <c r="C22" s="212">
+        <f t="shared" si="3"/>
+        <v>0.50000000000000089</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>30.000000000000053</v>
+      </c>
+      <c r="F22" s="214">
+        <f t="shared" si="1"/>
+        <v>0.9375</v>
+      </c>
+      <c r="G22" s="215" t="str">
+        <f t="shared" si="2"/>
+        <v>First break End</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="213">
+        <v>0.94270833333333337</v>
+      </c>
+      <c r="B23" s="210" t="s">
+        <v>255</v>
+      </c>
+      <c r="C23" s="212">
+        <f t="shared" si="3"/>
+        <v>0.12500000000000089</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>7.5000000000000533</v>
+      </c>
+      <c r="F23" s="214">
+        <f t="shared" si="1"/>
+        <v>0.94270833333333337</v>
+      </c>
+      <c r="G23" s="215" t="str">
+        <f t="shared" si="2"/>
+        <v>Excavator product begins, Trucks Cycles Begin</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="213">
+        <v>7.8125E-2</v>
+      </c>
+      <c r="B24" s="210" t="s">
+        <v>256</v>
+      </c>
+      <c r="C24" s="212">
+        <f t="shared" si="3"/>
+        <v>-20.75</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>-1245</v>
+      </c>
+      <c r="F24" s="214">
+        <f t="shared" si="1"/>
+        <v>7.8125E-2</v>
+      </c>
+      <c r="G24" s="215" t="str">
+        <f t="shared" si="2"/>
+        <v>Excavator Stops Loading Trucks, Trucks Cycles Stop</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="213">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="B25" s="210" t="s">
+        <v>248</v>
+      </c>
+      <c r="C25" s="212">
+        <f t="shared" si="3"/>
+        <v>0.12499999999999989</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>7.4999999999999929</v>
+      </c>
+      <c r="F25" s="214">
+        <f t="shared" si="1"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G25" s="215" t="str">
+        <f t="shared" si="2"/>
+        <v>Second Break Start</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="213">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="B26" s="210" t="s">
+        <v>249</v>
+      </c>
+      <c r="C26" s="212">
+        <f t="shared" si="3"/>
+        <v>0.50000000000000022</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>30.000000000000014</v>
+      </c>
+      <c r="F26" s="214">
+        <f t="shared" si="1"/>
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="G26" s="215" t="str">
+        <f t="shared" si="2"/>
+        <v>Second break End</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="213">
+        <v>0.109375</v>
+      </c>
+      <c r="B27" s="210" t="s">
+        <v>255</v>
+      </c>
+      <c r="C27" s="212">
+        <f t="shared" si="3"/>
+        <v>0.12499999999999989</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>7.4999999999999929</v>
+      </c>
+      <c r="F27" s="214">
+        <f t="shared" si="1"/>
+        <v>0.109375</v>
+      </c>
+      <c r="G27" s="215" t="str">
+        <f t="shared" si="2"/>
+        <v>Excavator product begins, Trucks Cycles Begin</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="213">
+        <v>0.24652777777777779</v>
+      </c>
+      <c r="B28" s="210" t="s">
+        <v>256</v>
+      </c>
+      <c r="C28" s="212">
+        <f t="shared" si="3"/>
+        <v>3.291666666666667</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>197.50000000000003</v>
+      </c>
+      <c r="F28" s="214">
+        <f t="shared" si="1"/>
+        <v>0.24652777777777779</v>
+      </c>
+      <c r="G28" s="215" t="str">
+        <f t="shared" si="2"/>
+        <v>Excavator Stops Loading Trucks, Trucks Cycles Stop</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="213">
+        <v>0.25</v>
+      </c>
+      <c r="B29" s="210" t="s">
+        <v>262</v>
+      </c>
+      <c r="C29" s="212">
+        <f t="shared" si="3"/>
+        <v>8.3333333333333037E-2</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>4.9999999999999822</v>
+      </c>
+      <c r="F29" s="214">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+      <c r="G29" s="215" t="str">
+        <f t="shared" si="2"/>
+        <v>Night Shift Ends</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="B2:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
@@ -12747,7 +13471,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="B2:E29"/>

</xml_diff>

<commit_message>
End of day Pre experiement commit
</commit_message>
<xml_diff>
--- a/Rolleston Workzones_ps_140327.xlsx
+++ b/Rolleston Workzones_ps_140327.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="15360" windowHeight="8370" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="15360" windowHeight="8370" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Working Locations" sheetId="1" r:id="rId1"/>
@@ -1449,7 +1449,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1467,8 +1467,9 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="217">
+  <cellXfs count="219">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="6" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1842,8 +1843,11 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="17" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="18">
+    <cellStyle name="Comma" xfId="17" builtinId="3"/>
     <cellStyle name="Comma 11 2" xfId="8"/>
     <cellStyle name="Comma 2" xfId="15"/>
     <cellStyle name="Comma 2 19" xfId="9"/>
@@ -2165,8 +2169,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:V249"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G86" sqref="G86"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="N43" sqref="N43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2174,6 +2178,8 @@
     <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.85546875" customWidth="1"/>
+    <col min="17" max="17" width="20.140625" customWidth="1"/>
+    <col min="18" max="18" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:15" ht="22.5" x14ac:dyDescent="0.3">
@@ -2422,7 +2428,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="182"/>
       <c r="B17" s="112"/>
       <c r="C17" s="113" t="s">
@@ -2447,7 +2453,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="182"/>
       <c r="B18" s="112"/>
       <c r="C18" s="113" t="s">
@@ -2472,7 +2478,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="182"/>
       <c r="B19" s="116" t="s">
         <v>31</v>
@@ -2499,7 +2505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="182"/>
       <c r="B20" s="112"/>
       <c r="C20" s="113" t="s">
@@ -2524,7 +2530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="182"/>
       <c r="B21" s="117"/>
       <c r="C21" s="118" t="s">
@@ -2549,10 +2555,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="182"/>
     </row>
-    <row r="23" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="182"/>
       <c r="B23" s="21" t="s">
         <v>84</v>
@@ -2561,7 +2567,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="182"/>
       <c r="B24" s="43"/>
       <c r="C24" s="54"/>
@@ -2581,8 +2587,11 @@
       <c r="M24" s="34"/>
       <c r="N24" s="34"/>
       <c r="O24" s="35"/>
-    </row>
-    <row r="25" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S24">
+        <v>12000000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="182"/>
       <c r="B25" s="39"/>
       <c r="C25" s="56" t="s">
@@ -2624,8 +2633,13 @@
       <c r="O25" s="64" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q25" s="44"/>
+      <c r="R25" s="44"/>
+      <c r="S25">
+        <v>12000000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="182"/>
       <c r="B26" s="61" t="s">
         <v>38</v>
@@ -2682,7 +2696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="182"/>
       <c r="B27" s="36" t="s">
         <v>39</v>
@@ -2700,8 +2714,11 @@
       <c r="M27" s="37"/>
       <c r="N27" s="37"/>
       <c r="O27" s="38"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q27" s="212"/>
+      <c r="R27" s="212"/>
+      <c r="S27" s="212"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="182"/>
       <c r="B28" s="59" t="s">
         <v>40</v>
@@ -2752,8 +2769,27 @@
         <f>IF(I$26&gt;0,I28/I$26,0)</f>
         <v>0.10175587053099218</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P28">
+        <v>31</v>
+      </c>
+      <c r="Q28" s="217">
+        <f>($S$25/365)*P28</f>
+        <v>1019178.0821917807</v>
+      </c>
+      <c r="R28" s="212">
+        <f>I28*1000</f>
+        <v>481000</v>
+      </c>
+      <c r="S28" s="212">
+        <f>Q28-R28</f>
+        <v>538178.08219178068</v>
+      </c>
+      <c r="T28">
+        <f>S28/$S$40</f>
+        <v>7.3996711424691414E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="182"/>
       <c r="B29" s="59" t="s">
         <v>41</v>
@@ -2804,8 +2840,27 @@
         <f t="shared" si="10"/>
         <v>3.8290670615612442E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P29">
+        <v>28</v>
+      </c>
+      <c r="Q29" s="217">
+        <f t="shared" ref="Q29:Q39" si="11">($S$25/365)*P29</f>
+        <v>920547.94520547939</v>
+      </c>
+      <c r="R29" s="212">
+        <f t="shared" ref="R29:R39" si="12">I29*1000</f>
+        <v>181000</v>
+      </c>
+      <c r="S29" s="212">
+        <f t="shared" ref="S29:S39" si="13">Q29-R29</f>
+        <v>739547.94520547939</v>
+      </c>
+      <c r="T29">
+        <f t="shared" ref="T29:T39" si="14">S29/$S$40</f>
+        <v>0.10168402931465412</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="182"/>
       <c r="B30" s="59" t="s">
         <v>42</v>
@@ -2856,8 +2911,27 @@
         <f t="shared" si="10"/>
         <v>0.1191030251745293</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P30">
+        <v>31</v>
+      </c>
+      <c r="Q30" s="217">
+        <f t="shared" si="11"/>
+        <v>1019178.0821917807</v>
+      </c>
+      <c r="R30" s="212">
+        <f t="shared" si="12"/>
+        <v>563000</v>
+      </c>
+      <c r="S30" s="212">
+        <f t="shared" si="13"/>
+        <v>456178.08219178068</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="14"/>
+        <v>6.2722134221336545E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="182"/>
       <c r="B31" s="59" t="s">
         <v>43</v>
@@ -2908,8 +2982,27 @@
         <f t="shared" si="10"/>
         <v>9.1178337211762217E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P31">
+        <v>30</v>
+      </c>
+      <c r="Q31" s="217">
+        <f t="shared" si="11"/>
+        <v>986301.36986301362</v>
+      </c>
+      <c r="R31" s="212">
+        <f t="shared" si="12"/>
+        <v>431000</v>
+      </c>
+      <c r="S31" s="212">
+        <f t="shared" si="13"/>
+        <v>555301.36986301362</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="14"/>
+        <v>7.6351075190844719E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="182"/>
       <c r="B32" s="59" t="s">
         <v>17</v>
@@ -2960,8 +3053,27 @@
         <f>IF(I$26&gt;0,I32/I$26,0)</f>
         <v>6.0503490585995343E-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P32">
+        <v>31</v>
+      </c>
+      <c r="Q32" s="217">
+        <f t="shared" si="11"/>
+        <v>1019178.0821917807</v>
+      </c>
+      <c r="R32" s="212">
+        <f t="shared" si="12"/>
+        <v>286000</v>
+      </c>
+      <c r="S32" s="212">
+        <f t="shared" si="13"/>
+        <v>733178.08219178068</v>
+      </c>
+      <c r="T32">
+        <f t="shared" si="14"/>
+        <v>0.10080820599364508</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="182"/>
       <c r="B33" s="59" t="s">
         <v>44</v>
@@ -3012,8 +3124,27 @@
         <f t="shared" si="10"/>
         <v>0.11296805584937593</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P33">
+        <v>30</v>
+      </c>
+      <c r="Q33" s="217">
+        <f t="shared" si="11"/>
+        <v>986301.36986301362</v>
+      </c>
+      <c r="R33" s="212">
+        <f t="shared" si="12"/>
+        <v>534000</v>
+      </c>
+      <c r="S33" s="212">
+        <f t="shared" si="13"/>
+        <v>452301.36986301362</v>
+      </c>
+      <c r="T33">
+        <f t="shared" si="14"/>
+        <v>6.2189106264679446E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="182"/>
       <c r="B34" s="59" t="s">
         <v>45</v>
@@ -3064,8 +3195,27 @@
         <f t="shared" si="10"/>
         <v>6.4311402580918137E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P34">
+        <v>31</v>
+      </c>
+      <c r="Q34" s="217">
+        <f t="shared" si="11"/>
+        <v>1019178.0821917807</v>
+      </c>
+      <c r="R34" s="212">
+        <f t="shared" si="12"/>
+        <v>304000</v>
+      </c>
+      <c r="S34" s="212">
+        <f t="shared" si="13"/>
+        <v>715178.08219178068</v>
+      </c>
+      <c r="T34">
+        <f t="shared" si="14"/>
+        <v>9.833329880266474E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="182"/>
       <c r="B35" s="59" t="s">
         <v>46</v>
@@ -3116,8 +3266,27 @@
         <f t="shared" si="10"/>
         <v>7.700444256399408E-2</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P35">
+        <v>31</v>
+      </c>
+      <c r="Q35" s="217">
+        <f t="shared" si="11"/>
+        <v>1019178.0821917807</v>
+      </c>
+      <c r="R35" s="212">
+        <f t="shared" si="12"/>
+        <v>364000</v>
+      </c>
+      <c r="S35" s="212">
+        <f t="shared" si="13"/>
+        <v>655178.08219178068</v>
+      </c>
+      <c r="T35">
+        <f t="shared" si="14"/>
+        <v>9.0083608166063617E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="182"/>
       <c r="B36" s="59" t="s">
         <v>47</v>
@@ -3168,8 +3337,27 @@
         <f t="shared" si="10"/>
         <v>0.11042944785276074</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P36">
+        <v>30</v>
+      </c>
+      <c r="Q36" s="217">
+        <f t="shared" si="11"/>
+        <v>986301.36986301362</v>
+      </c>
+      <c r="R36" s="212">
+        <f t="shared" si="12"/>
+        <v>522000</v>
+      </c>
+      <c r="S36" s="212">
+        <f t="shared" si="13"/>
+        <v>464301.36986301362</v>
+      </c>
+      <c r="T36">
+        <f t="shared" si="14"/>
+        <v>6.3839044391999666E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="182"/>
       <c r="B37" s="59" t="s">
         <v>48</v>
@@ -3220,8 +3408,27 @@
         <f t="shared" si="10"/>
         <v>5.965728792045695E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P37">
+        <v>31</v>
+      </c>
+      <c r="Q37" s="217">
+        <f t="shared" si="11"/>
+        <v>1019178.0821917807</v>
+      </c>
+      <c r="R37" s="212">
+        <f t="shared" si="12"/>
+        <v>282000</v>
+      </c>
+      <c r="S37" s="212">
+        <f t="shared" si="13"/>
+        <v>737178.08219178068</v>
+      </c>
+      <c r="T37">
+        <f t="shared" si="14"/>
+        <v>0.10135818536941849</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="182"/>
       <c r="B38" s="59" t="s">
         <v>49</v>
@@ -3272,8 +3479,27 @@
         <f t="shared" si="10"/>
         <v>0.10683308652422255</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P38">
+        <v>30</v>
+      </c>
+      <c r="Q38" s="217">
+        <f t="shared" si="11"/>
+        <v>986301.36986301362</v>
+      </c>
+      <c r="R38" s="212">
+        <f t="shared" si="12"/>
+        <v>505000</v>
+      </c>
+      <c r="S38" s="212">
+        <f t="shared" si="13"/>
+        <v>481301.36986301362</v>
+      </c>
+      <c r="T38">
+        <f t="shared" si="14"/>
+        <v>6.617645673903666E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="182"/>
       <c r="B39" s="58" t="s">
         <v>50</v>
@@ -3324,8 +3550,27 @@
         <f t="shared" si="10"/>
         <v>5.7964882589380158E-2</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P39">
+        <v>31</v>
+      </c>
+      <c r="Q39" s="217">
+        <f t="shared" si="11"/>
+        <v>1019178.0821917807</v>
+      </c>
+      <c r="R39" s="212">
+        <f t="shared" si="12"/>
+        <v>274000</v>
+      </c>
+      <c r="S39" s="212">
+        <f t="shared" si="13"/>
+        <v>745178.08219178068</v>
+      </c>
+      <c r="T39">
+        <f t="shared" si="14"/>
+        <v>0.10245814412096531</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="182"/>
       <c r="B40" s="99" t="s">
         <v>190</v>
@@ -3349,11 +3594,15 @@
       <c r="M40" s="46"/>
       <c r="N40" s="46"/>
       <c r="O40" s="46"/>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="S40" s="212">
+        <f>SUM(S28:S39)</f>
+        <v>7273000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="182"/>
     </row>
-    <row r="42" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="182"/>
       <c r="B42" s="21" t="s">
         <v>201</v>
@@ -3362,7 +3611,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="182"/>
       <c r="B43" s="65" t="s">
         <v>52</v>
@@ -3388,8 +3637,22 @@
       <c r="I43" s="71">
         <v>0.48</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K43" s="144">
+        <v>1900</v>
+      </c>
+      <c r="L43">
+        <v>180</v>
+      </c>
+      <c r="M43">
+        <f>L43/K43</f>
+        <v>9.4736842105263161E-2</v>
+      </c>
+      <c r="N43">
+        <f>M43*60</f>
+        <v>5.6842105263157894</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="182"/>
       <c r="B44" s="41" t="s">
         <v>54</v>
@@ -3415,8 +3678,22 @@
       <c r="I44" s="72">
         <v>0.52</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K44" s="144">
+        <v>1750</v>
+      </c>
+      <c r="L44">
+        <v>180</v>
+      </c>
+      <c r="M44">
+        <f>L44/K44</f>
+        <v>0.10285714285714286</v>
+      </c>
+      <c r="N44">
+        <f>M44*60</f>
+        <v>6.1714285714285717</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="182"/>
       <c r="B45" s="42" t="s">
         <v>55</v>
@@ -3442,8 +3719,22 @@
       <c r="I45" s="73">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K45" s="144">
+        <v>1750</v>
+      </c>
+      <c r="L45">
+        <v>210</v>
+      </c>
+      <c r="M45">
+        <f>L45/K45</f>
+        <v>0.12</v>
+      </c>
+      <c r="N45">
+        <f>M45*60</f>
+        <v>7.1999999999999993</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="182"/>
       <c r="B46" s="57"/>
       <c r="C46" s="44"/>
@@ -3454,7 +3745,7 @@
       <c r="H46" s="80"/>
       <c r="I46" s="79"/>
     </row>
-    <row r="47" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="182"/>
       <c r="B47" s="82" t="s">
         <v>121</v>
@@ -3467,7 +3758,7 @@
       <c r="H47" s="80"/>
       <c r="I47" s="79"/>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="182"/>
       <c r="B48" s="83" t="s">
         <v>204</v>
@@ -3910,7 +4201,7 @@
         <v>30</v>
       </c>
       <c r="F72" s="11">
-        <f t="shared" ref="F72:F76" si="11">D72/E72 * 60</f>
+        <f t="shared" ref="F72:F76" si="15">D72/E72 * 60</f>
         <v>5.2</v>
       </c>
     </row>
@@ -3929,7 +4220,7 @@
         <v>30</v>
       </c>
       <c r="F73" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>5.2</v>
       </c>
     </row>
@@ -3948,7 +4239,7 @@
         <v>30</v>
       </c>
       <c r="F74" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>5.2</v>
       </c>
     </row>
@@ -3967,7 +4258,7 @@
         <v>30</v>
       </c>
       <c r="F75" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>5.2</v>
       </c>
     </row>
@@ -3986,7 +4277,7 @@
         <v>50</v>
       </c>
       <c r="F76" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>3</v>
       </c>
     </row>
@@ -4042,14 +4333,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A81" s="184"/>
       <c r="B81" s="41"/>
       <c r="C81" s="29" t="s">
         <v>28</v>
       </c>
       <c r="D81" s="29">
-        <f t="shared" ref="D81:D85" si="12">E81*F81/60</f>
+        <f t="shared" ref="D81:D85" si="16">E81*F81/60</f>
         <v>10</v>
       </c>
       <c r="E81" s="9">
@@ -4059,14 +4350,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A82" s="184"/>
       <c r="B82" s="41"/>
       <c r="C82" s="29" t="s">
         <v>29</v>
       </c>
       <c r="D82" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>10</v>
       </c>
       <c r="E82" s="9">
@@ -4076,7 +4367,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A83" s="184"/>
       <c r="B83" s="8" t="s">
         <v>31</v>
@@ -4085,7 +4376,7 @@
         <v>32</v>
       </c>
       <c r="D83" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="E83" s="9">
@@ -4095,14 +4386,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A84" s="184"/>
       <c r="B84" s="41"/>
       <c r="C84" s="29" t="s">
         <v>28</v>
       </c>
       <c r="D84" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="E84" s="9">
@@ -4112,14 +4403,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="184"/>
       <c r="B85" s="42"/>
       <c r="C85" s="193" t="s">
         <v>29</v>
       </c>
       <c r="D85" s="193">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="E85" s="14">
@@ -4129,7 +4420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A86" s="184"/>
       <c r="B86" s="37"/>
       <c r="C86" s="37"/>
@@ -4137,13 +4428,13 @@
       <c r="E86" s="194"/>
       <c r="F86" s="195"/>
     </row>
-    <row r="87" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="184"/>
       <c r="B87" s="21" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A88" s="184"/>
       <c r="B88" s="43"/>
       <c r="C88" s="54"/>
@@ -4164,7 +4455,7 @@
       <c r="N88" s="34"/>
       <c r="O88" s="35"/>
     </row>
-    <row r="89" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="184"/>
       <c r="B89" s="39"/>
       <c r="C89" s="56" t="s">
@@ -4207,7 +4498,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A90" s="184"/>
       <c r="B90" s="61" t="s">
         <v>38</v>
@@ -4220,19 +4511,19 @@
         <v>0</v>
       </c>
       <c r="E90" s="144">
-        <f t="shared" ref="E90:H90" si="13">SUM(E92:E103)</f>
+        <f t="shared" ref="E90:H90" si="17">SUM(E92:E103)</f>
         <v>8</v>
       </c>
       <c r="F90" s="144">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>409</v>
       </c>
       <c r="G90" s="144">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>2631</v>
       </c>
       <c r="H90" s="144">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="I90" s="145">
@@ -4244,27 +4535,35 @@
         <v>0</v>
       </c>
       <c r="K90" s="46">
-        <f t="shared" ref="K90:N90" si="14">E90/$I$90</f>
+        <f t="shared" ref="K90:N90" si="18">E90/$I$90</f>
         <v>2.6246719160104987E-3</v>
       </c>
       <c r="L90" s="46">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.13418635170603674</v>
       </c>
       <c r="M90" s="46">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.86318897637795278</v>
       </c>
       <c r="N90" s="46">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="O90" s="47">
         <f>SUM(J90:N90)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q90" s="212"/>
+      <c r="R90" s="212">
+        <v>14000000</v>
+      </c>
+      <c r="S90" s="212"/>
+      <c r="T90" s="212"/>
+      <c r="U90" s="212"/>
+      <c r="V90" s="212"/>
+    </row>
+    <row r="91" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A91" s="184"/>
       <c r="B91" s="36" t="s">
         <v>39</v>
@@ -4282,8 +4581,14 @@
       <c r="M91" s="37"/>
       <c r="N91" s="37"/>
       <c r="O91" s="38"/>
-    </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q91" s="212"/>
+      <c r="R91" s="212"/>
+      <c r="S91" s="212"/>
+      <c r="T91" s="212"/>
+      <c r="U91" s="212"/>
+      <c r="V91" s="212"/>
+    </row>
+    <row r="92" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A92" s="184"/>
       <c r="B92" s="59" t="s">
         <v>40</v>
@@ -4315,27 +4620,50 @@
         <v>0</v>
       </c>
       <c r="K92" s="46">
-        <f t="shared" ref="K92:O103" si="15">IF(E$90&gt;0,E92/E$90,0)</f>
+        <f t="shared" ref="K92:O103" si="19">IF(E$90&gt;0,E92/E$90,0)</f>
         <v>0</v>
       </c>
       <c r="L92" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0.1100244498777506</v>
       </c>
       <c r="M92" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="N92" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="O92" s="48">
         <f>IF(I$90&gt;0,I92/I$90,0)</f>
         <v>1.4763779527559055E-2</v>
       </c>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P92">
+        <v>31</v>
+      </c>
+      <c r="Q92" s="212">
+        <f>($R$90/365)*P92</f>
+        <v>1189041.0958904109</v>
+      </c>
+      <c r="R92" s="217">
+        <f>(I92+I156)*1000</f>
+        <v>638000</v>
+      </c>
+      <c r="S92" s="212">
+        <f>Q92-R92</f>
+        <v>551041.09589041094</v>
+      </c>
+      <c r="T92" s="212">
+        <f>S92/2</f>
+        <v>275520.54794520547</v>
+      </c>
+      <c r="U92" s="212">
+        <f>T92/$T$104</f>
+        <v>8.6532835409926331E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A93" s="184"/>
       <c r="B93" s="59" t="s">
         <v>41</v>
@@ -4359,35 +4687,58 @@
         <v>0</v>
       </c>
       <c r="I93" s="145">
-        <f t="shared" ref="I93:I103" si="16">SUM(D93:H93)</f>
+        <f t="shared" ref="I93:I103" si="20">SUM(D93:H93)</f>
         <v>405</v>
       </c>
       <c r="J93" s="45">
-        <f t="shared" ref="J93:J103" si="17">IF(D$90&gt;0,D93/D$90,0)</f>
+        <f t="shared" ref="J93:J103" si="21">IF(D$90&gt;0,D93/D$90,0)</f>
         <v>0</v>
       </c>
       <c r="K93" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="L93" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0.28117359413202936</v>
       </c>
       <c r="M93" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0.10718358038768529</v>
       </c>
       <c r="N93" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="O93" s="48">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0.13287401574803151</v>
       </c>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P93">
+        <v>28</v>
+      </c>
+      <c r="Q93" s="212">
+        <f>($R$90/365)*P93</f>
+        <v>1073972.602739726</v>
+      </c>
+      <c r="R93" s="217">
+        <f t="shared" ref="R93:R103" si="22">(I93+I157)*1000</f>
+        <v>573000</v>
+      </c>
+      <c r="S93" s="212">
+        <f t="shared" ref="S93:S103" si="23">Q93-R93</f>
+        <v>500972.60273972596</v>
+      </c>
+      <c r="T93" s="212">
+        <f t="shared" ref="T93:T103" si="24">S93/2</f>
+        <v>250486.30136986298</v>
+      </c>
+      <c r="U93" s="212">
+        <f t="shared" ref="U93:U103" si="25">T93/$T$104</f>
+        <v>7.8670320781992126E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A94" s="184"/>
       <c r="B94" s="59" t="s">
         <v>42</v>
@@ -4411,19 +4762,19 @@
         <v>0</v>
       </c>
       <c r="I94" s="145">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>352</v>
       </c>
       <c r="J94" s="45">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="K94" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="L94" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="M94" s="46">
@@ -4431,15 +4782,38 @@
         <v>0.1337894336754086</v>
       </c>
       <c r="N94" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="O94" s="48">
         <f>IF(I$90&gt;0,I94/I$90,0)</f>
         <v>0.11548556430446194</v>
       </c>
-    </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P94">
+        <v>31</v>
+      </c>
+      <c r="Q94" s="212">
+        <f>($R$90/365)*P94</f>
+        <v>1189041.0958904109</v>
+      </c>
+      <c r="R94" s="217">
+        <f t="shared" si="22"/>
+        <v>526000</v>
+      </c>
+      <c r="S94" s="212">
+        <f t="shared" si="23"/>
+        <v>663041.09589041094</v>
+      </c>
+      <c r="T94" s="212">
+        <f t="shared" si="24"/>
+        <v>331520.54794520547</v>
+      </c>
+      <c r="U94" s="212">
+        <f t="shared" si="25"/>
+        <v>0.10412077510841879</v>
+      </c>
+    </row>
+    <row r="95" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A95" s="184"/>
       <c r="B95" s="59" t="s">
         <v>43</v>
@@ -4463,35 +4837,58 @@
         <v>0</v>
       </c>
       <c r="I95" s="145">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>272</v>
       </c>
       <c r="J95" s="45">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="K95" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="L95" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="M95" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0.10338274420372481</v>
       </c>
       <c r="N95" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="O95" s="48">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>8.9238845144356954E-2</v>
       </c>
-    </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P95">
+        <v>30</v>
+      </c>
+      <c r="Q95" s="212">
+        <f>($R$90/365)*P95</f>
+        <v>1150684.9315068494</v>
+      </c>
+      <c r="R95" s="217">
+        <f t="shared" si="22"/>
+        <v>272000</v>
+      </c>
+      <c r="S95" s="212">
+        <f t="shared" si="23"/>
+        <v>878684.93150684936</v>
+      </c>
+      <c r="T95" s="212">
+        <f t="shared" si="24"/>
+        <v>439342.46575342468</v>
+      </c>
+      <c r="U95" s="212">
+        <f t="shared" si="25"/>
+        <v>0.13798444276175395</v>
+      </c>
+    </row>
+    <row r="96" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A96" s="184"/>
       <c r="B96" s="59" t="s">
         <v>17</v>
@@ -4515,35 +4912,58 @@
         <v>0</v>
       </c>
       <c r="I96" s="145">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>263</v>
       </c>
       <c r="J96" s="45">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="K96" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="L96" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="M96" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>9.99619916381604E-2</v>
       </c>
       <c r="N96" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="O96" s="48">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>8.6286089238845148E-2</v>
       </c>
-    </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P96">
+        <v>31</v>
+      </c>
+      <c r="Q96" s="212">
+        <f>($R$90/365)*P96</f>
+        <v>1189041.0958904109</v>
+      </c>
+      <c r="R96" s="217">
+        <f t="shared" si="22"/>
+        <v>764000</v>
+      </c>
+      <c r="S96" s="212">
+        <f t="shared" si="23"/>
+        <v>425041.09589041094</v>
+      </c>
+      <c r="T96" s="212">
+        <f t="shared" si="24"/>
+        <v>212520.54794520547</v>
+      </c>
+      <c r="U96" s="212">
+        <f t="shared" si="25"/>
+        <v>6.6746403249122316E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A97" s="184"/>
       <c r="B97" s="59" t="s">
         <v>44</v>
@@ -4567,35 +4987,58 @@
         <v>0</v>
       </c>
       <c r="I97" s="145">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="J97" s="45">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="K97" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="L97" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="M97" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="N97" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="O97" s="48">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="P97">
+        <v>30</v>
+      </c>
+      <c r="Q97" s="212">
+        <f>($R$90/365)*P97</f>
+        <v>1150684.9315068494</v>
+      </c>
+      <c r="R97" s="217">
+        <f t="shared" si="22"/>
+        <v>408000</v>
+      </c>
+      <c r="S97" s="212">
+        <f t="shared" si="23"/>
+        <v>742684.93150684936</v>
+      </c>
+      <c r="T97" s="212">
+        <f t="shared" si="24"/>
+        <v>371342.46575342468</v>
+      </c>
+      <c r="U97" s="212">
+        <f t="shared" si="25"/>
+        <v>0.11662765884215598</v>
+      </c>
+    </row>
+    <row r="98" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A98" s="184"/>
       <c r="B98" s="59" t="s">
         <v>45</v>
@@ -4619,35 +5062,58 @@
         <v>0</v>
       </c>
       <c r="I98" s="145">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>66</v>
       </c>
       <c r="J98" s="45">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="K98" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="L98" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="M98" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>2.5085518814139111E-2</v>
       </c>
       <c r="N98" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="O98" s="48">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>2.1653543307086614E-2</v>
       </c>
-    </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P98">
+        <v>31</v>
+      </c>
+      <c r="Q98" s="212">
+        <f>($R$90/365)*P98</f>
+        <v>1189041.0958904109</v>
+      </c>
+      <c r="R98" s="217">
+        <f t="shared" si="22"/>
+        <v>556000</v>
+      </c>
+      <c r="S98" s="212">
+        <f t="shared" si="23"/>
+        <v>633041.09589041094</v>
+      </c>
+      <c r="T98" s="212">
+        <f t="shared" si="24"/>
+        <v>316520.54794520547</v>
+      </c>
+      <c r="U98" s="212">
+        <f t="shared" si="25"/>
+        <v>9.9409719832036877E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A99" s="184"/>
       <c r="B99" s="59" t="s">
         <v>46</v>
@@ -4671,35 +5137,58 @@
         <v>0</v>
       </c>
       <c r="I99" s="145">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>253</v>
       </c>
       <c r="J99" s="45">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="K99" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="L99" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="M99" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>9.6161155454199926E-2</v>
       </c>
       <c r="N99" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="O99" s="48">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>8.3005249343832022E-2</v>
       </c>
-    </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P99">
+        <v>31</v>
+      </c>
+      <c r="Q99" s="212">
+        <f>($R$90/365)*P99</f>
+        <v>1189041.0958904109</v>
+      </c>
+      <c r="R99" s="217">
+        <f t="shared" si="22"/>
+        <v>549000</v>
+      </c>
+      <c r="S99" s="212">
+        <f t="shared" si="23"/>
+        <v>640041.09589041094</v>
+      </c>
+      <c r="T99" s="212">
+        <f t="shared" si="24"/>
+        <v>320020.54794520547</v>
+      </c>
+      <c r="U99" s="212">
+        <f t="shared" si="25"/>
+        <v>0.10050896606319266</v>
+      </c>
+    </row>
+    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A100" s="184"/>
       <c r="B100" s="59" t="s">
         <v>47</v>
@@ -4723,35 +5212,58 @@
         <v>0</v>
       </c>
       <c r="I100" s="145">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>473</v>
       </c>
       <c r="J100" s="45">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="K100" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="L100" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0.44254278728606355</v>
       </c>
       <c r="M100" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0.11098441657164576</v>
       </c>
       <c r="N100" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="O100" s="48">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0.15518372703412073</v>
       </c>
-    </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P100">
+        <v>30</v>
+      </c>
+      <c r="Q100" s="212">
+        <f>($R$90/365)*P100</f>
+        <v>1150684.9315068494</v>
+      </c>
+      <c r="R100" s="217">
+        <f t="shared" si="22"/>
+        <v>719000</v>
+      </c>
+      <c r="S100" s="212">
+        <f t="shared" si="23"/>
+        <v>431684.93150684936</v>
+      </c>
+      <c r="T100" s="212">
+        <f t="shared" si="24"/>
+        <v>215842.46575342468</v>
+      </c>
+      <c r="U100" s="212">
+        <f t="shared" si="25"/>
+        <v>6.7789719143663524E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A101" s="184"/>
       <c r="B101" s="59" t="s">
         <v>48</v>
@@ -4775,35 +5287,58 @@
         <v>0</v>
       </c>
       <c r="I101" s="145">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>204</v>
       </c>
       <c r="J101" s="45">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="K101" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="L101" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="M101" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>7.7537058152793617E-2</v>
       </c>
       <c r="N101" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="O101" s="48">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>6.6929133858267723E-2</v>
       </c>
-    </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P101">
+        <v>31</v>
+      </c>
+      <c r="Q101" s="212">
+        <f>($R$90/365)*P101</f>
+        <v>1189041.0958904109</v>
+      </c>
+      <c r="R101" s="217">
+        <f t="shared" si="22"/>
+        <v>858000</v>
+      </c>
+      <c r="S101" s="212">
+        <f t="shared" si="23"/>
+        <v>331041.09589041094</v>
+      </c>
+      <c r="T101" s="212">
+        <f t="shared" si="24"/>
+        <v>165520.54794520547</v>
+      </c>
+      <c r="U101" s="212">
+        <f t="shared" si="25"/>
+        <v>5.1985096716458998E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A102" s="184"/>
       <c r="B102" s="59" t="s">
         <v>49</v>
@@ -4827,35 +5362,58 @@
         <v>0</v>
       </c>
       <c r="I102" s="145">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>345</v>
       </c>
       <c r="J102" s="45">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="K102" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="L102" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0.1100244498777506</v>
       </c>
       <c r="M102" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0.11402508551881414</v>
       </c>
       <c r="N102" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="O102" s="48">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0.11318897637795275</v>
       </c>
-    </row>
-    <row r="103" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P102">
+        <v>30</v>
+      </c>
+      <c r="Q102" s="212">
+        <f>($R$90/365)*P102</f>
+        <v>1150684.9315068494</v>
+      </c>
+      <c r="R102" s="217">
+        <f t="shared" si="22"/>
+        <v>784000</v>
+      </c>
+      <c r="S102" s="212">
+        <f t="shared" si="23"/>
+        <v>366684.93150684936</v>
+      </c>
+      <c r="T102" s="212">
+        <f t="shared" si="24"/>
+        <v>183342.46575342468</v>
+      </c>
+      <c r="U102" s="212">
+        <f t="shared" si="25"/>
+        <v>5.7582432711502721E-2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="184"/>
       <c r="B103" s="58" t="s">
         <v>50</v>
@@ -4879,35 +5437,58 @@
         <v>0</v>
       </c>
       <c r="I103" s="145">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>370</v>
       </c>
       <c r="J103" s="49">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="K103" s="50">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="L103" s="50">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>5.623471882640587E-2</v>
       </c>
       <c r="M103" s="50">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0.13188901558342836</v>
       </c>
       <c r="N103" s="50">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="O103" s="51">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0.12139107611548557</v>
       </c>
-    </row>
-    <row r="104" spans="1:15" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P103">
+        <v>31</v>
+      </c>
+      <c r="Q103" s="212">
+        <f>($R$90/365)*P103</f>
+        <v>1189041.0958904109</v>
+      </c>
+      <c r="R103" s="217">
+        <f t="shared" si="22"/>
+        <v>985000</v>
+      </c>
+      <c r="S103" s="212">
+        <f t="shared" si="23"/>
+        <v>204041.09589041094</v>
+      </c>
+      <c r="T103" s="212">
+        <f t="shared" si="24"/>
+        <v>102020.54794520547</v>
+      </c>
+      <c r="U103" s="212">
+        <f t="shared" si="25"/>
+        <v>3.2041629379775581E-2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="184"/>
       <c r="B104" s="99" t="s">
         <v>190</v>
@@ -4931,11 +5512,16 @@
       <c r="M104" s="46"/>
       <c r="N104" s="46"/>
       <c r="O104" s="46"/>
-    </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R104" s="218"/>
+      <c r="T104" s="212">
+        <f>SUM(T92:T103)</f>
+        <v>3184000.0000000005</v>
+      </c>
+    </row>
+    <row r="105" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A105" s="184"/>
     </row>
-    <row r="106" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="184"/>
       <c r="B106" s="21" t="s">
         <v>33</v>
@@ -4959,7 +5545,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A107" s="184"/>
       <c r="B107" s="65" t="s">
         <v>52</v>
@@ -4986,7 +5572,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A108" s="184"/>
       <c r="B108" s="41" t="s">
         <v>54</v>
@@ -5013,7 +5599,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="109" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="184"/>
       <c r="B109" s="42" t="s">
         <v>55</v>
@@ -5040,7 +5626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A110" s="184"/>
       <c r="B110" s="57"/>
       <c r="C110" s="44"/>
@@ -5051,7 +5637,7 @@
       <c r="H110" s="80"/>
       <c r="I110" s="79"/>
     </row>
-    <row r="111" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="184"/>
       <c r="B111" s="82" t="s">
         <v>121</v>
@@ -5064,7 +5650,7 @@
       <c r="H111" s="80"/>
       <c r="I111" s="79"/>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A112" s="184"/>
       <c r="B112" s="83" t="s">
         <v>122</v>
@@ -5504,7 +6090,7 @@
         <v>30</v>
       </c>
       <c r="F136" s="11">
-        <f t="shared" ref="F136:F140" si="18">D136/E136 * 60</f>
+        <f t="shared" ref="F136:F140" si="26">D136/E136 * 60</f>
         <v>6.8</v>
       </c>
     </row>
@@ -5523,7 +6109,7 @@
         <v>30</v>
       </c>
       <c r="F137" s="11">
-        <f t="shared" si="18"/>
+        <f t="shared" si="26"/>
         <v>6.8</v>
       </c>
     </row>
@@ -5542,7 +6128,7 @@
         <v>30</v>
       </c>
       <c r="F138" s="11">
-        <f t="shared" si="18"/>
+        <f t="shared" si="26"/>
         <v>6.8</v>
       </c>
     </row>
@@ -5561,7 +6147,7 @@
         <v>30</v>
       </c>
       <c r="F139" s="11">
-        <f t="shared" si="18"/>
+        <f t="shared" si="26"/>
         <v>6.8</v>
       </c>
     </row>
@@ -5580,7 +6166,7 @@
         <v>50</v>
       </c>
       <c r="F140" s="16">
-        <f t="shared" si="18"/>
+        <f t="shared" si="26"/>
         <v>10.799999999999999</v>
       </c>
     </row>
@@ -5636,14 +6222,14 @@
         <v>28.5</v>
       </c>
     </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A145" s="185"/>
       <c r="B145" s="41"/>
       <c r="C145" s="29" t="s">
         <v>28</v>
       </c>
       <c r="D145" s="29">
-        <f t="shared" ref="D145:D149" si="19">E145*F145/60</f>
+        <f t="shared" ref="D145:D149" si="27">E145*F145/60</f>
         <v>15.25</v>
       </c>
       <c r="E145" s="9">
@@ -5653,14 +6239,14 @@
         <v>30.5</v>
       </c>
     </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A146" s="185"/>
       <c r="B146" s="41"/>
       <c r="C146" s="29" t="s">
         <v>29</v>
       </c>
       <c r="D146" s="29">
-        <f t="shared" si="19"/>
+        <f t="shared" si="27"/>
         <v>13.25</v>
       </c>
       <c r="E146" s="9">
@@ -5670,7 +6256,7 @@
         <v>26.5</v>
       </c>
     </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A147" s="185"/>
       <c r="B147" s="8" t="s">
         <v>31</v>
@@ -5679,7 +6265,7 @@
         <v>32</v>
       </c>
       <c r="D147" s="29">
-        <f t="shared" si="19"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="E147" s="9">
@@ -5689,14 +6275,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A148" s="185"/>
       <c r="B148" s="41"/>
       <c r="C148" s="29" t="s">
         <v>28</v>
       </c>
       <c r="D148" s="29">
-        <f t="shared" si="19"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="E148" s="9">
@@ -5706,14 +6292,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="185"/>
       <c r="B149" s="42"/>
       <c r="C149" s="193" t="s">
         <v>29</v>
       </c>
       <c r="D149" s="193">
-        <f t="shared" si="19"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="E149" s="14">
@@ -5723,7 +6309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A150" s="185"/>
       <c r="B150" s="37"/>
       <c r="C150" s="37"/>
@@ -5731,13 +6317,16 @@
       <c r="E150" s="194"/>
       <c r="F150" s="195"/>
     </row>
-    <row r="151" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="185"/>
       <c r="B151" s="21" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R151">
+        <v>16000000</v>
+      </c>
+    </row>
+    <row r="152" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A152" s="185"/>
       <c r="B152" s="43"/>
       <c r="C152" s="54"/>
@@ -5758,7 +6347,7 @@
       <c r="N152" s="34"/>
       <c r="O152" s="35"/>
     </row>
-    <row r="153" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="185"/>
       <c r="B153" s="39"/>
       <c r="C153" s="56" t="s">
@@ -5801,7 +6390,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="154" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A154" s="185"/>
       <c r="B154" s="61" t="s">
         <v>38</v>
@@ -5814,19 +6403,19 @@
         <v>0</v>
       </c>
       <c r="E154" s="144">
-        <f t="shared" ref="E154:H154" si="20">SUM(E156:E167)</f>
+        <f t="shared" ref="E154:H154" si="28">SUM(E156:E167)</f>
         <v>469</v>
       </c>
       <c r="F154" s="144">
-        <f t="shared" si="20"/>
+        <f t="shared" si="28"/>
         <v>1526</v>
       </c>
       <c r="G154" s="144">
-        <f t="shared" si="20"/>
+        <f t="shared" si="28"/>
         <v>2589</v>
       </c>
       <c r="H154" s="144">
-        <f t="shared" si="20"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="I154" s="145">
@@ -5838,19 +6427,19 @@
         <v>0</v>
       </c>
       <c r="K154" s="46">
-        <f t="shared" ref="K154:N154" si="21">E154/$I$154</f>
+        <f t="shared" ref="K154:N154" si="29">E154/$I$154</f>
         <v>0.10231239092495636</v>
       </c>
       <c r="L154" s="46">
-        <f t="shared" si="21"/>
+        <f t="shared" si="29"/>
         <v>0.33289703315881325</v>
       </c>
       <c r="M154" s="46">
-        <f t="shared" si="21"/>
+        <f t="shared" si="29"/>
         <v>0.56479057591623039</v>
       </c>
       <c r="N154" s="46">
-        <f t="shared" si="21"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="O154" s="47">
@@ -5858,7 +6447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A155" s="185"/>
       <c r="B155" s="36" t="s">
         <v>39</v>
@@ -5877,7 +6466,7 @@
       <c r="N155" s="37"/>
       <c r="O155" s="38"/>
     </row>
-    <row r="156" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A156" s="185"/>
       <c r="B156" s="59" t="s">
         <v>40</v>
@@ -5909,27 +6498,27 @@
         <v>0</v>
       </c>
       <c r="K156" s="46">
-        <f t="shared" ref="K156:O167" si="22">IF(E$154&gt;0,E156/E$154,0)</f>
+        <f t="shared" ref="K156:O167" si="30">IF(E$154&gt;0,E156/E$154,0)</f>
         <v>0</v>
       </c>
       <c r="L156" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>0.11336828309305373</v>
       </c>
       <c r="M156" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>0.16222479721900349</v>
       </c>
       <c r="N156" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="O156" s="48">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>0.12936300174520071</v>
       </c>
     </row>
-    <row r="157" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A157" s="185"/>
       <c r="B157" s="59" t="s">
         <v>41</v>
@@ -5953,35 +6542,35 @@
         <v>0</v>
       </c>
       <c r="I157" s="145">
-        <f t="shared" ref="I157:I167" si="23">SUM(D157:H157)</f>
+        <f t="shared" ref="I157:I167" si="31">SUM(D157:H157)</f>
         <v>168</v>
       </c>
       <c r="J157" s="45">
-        <f t="shared" ref="J157:J167" si="24">IF(D$154&gt;0,D157/D$154,0)</f>
+        <f t="shared" ref="J157:J167" si="32">IF(D$154&gt;0,D157/D$154,0)</f>
         <v>0</v>
       </c>
       <c r="K157" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="L157" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>3.1454783748361727E-2</v>
       </c>
       <c r="M157" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>4.6349942062572425E-2</v>
       </c>
       <c r="N157" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="O157" s="48">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>3.6649214659685861E-2</v>
       </c>
     </row>
-    <row r="158" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A158" s="185"/>
       <c r="B158" s="59" t="s">
         <v>42</v>
@@ -6005,35 +6594,35 @@
         <v>0</v>
       </c>
       <c r="I158" s="145">
-        <f t="shared" si="23"/>
+        <f t="shared" si="31"/>
         <v>174</v>
       </c>
       <c r="J158" s="45">
-        <f t="shared" si="24"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="K158" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>2.1321961620469083E-3</v>
       </c>
       <c r="L158" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="M158" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>6.6821166473541901E-2</v>
       </c>
       <c r="N158" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="O158" s="48">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>3.7958115183246072E-2</v>
       </c>
     </row>
-    <row r="159" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A159" s="185"/>
       <c r="B159" s="59" t="s">
         <v>43</v>
@@ -6057,35 +6646,35 @@
         <v>0</v>
       </c>
       <c r="I159" s="145">
-        <f t="shared" si="23"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="J159" s="45">
-        <f t="shared" si="24"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="K159" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="L159" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="M159" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="N159" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="O159" s="48">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="160" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A160" s="185"/>
       <c r="B160" s="59" t="s">
         <v>17</v>
@@ -6109,31 +6698,31 @@
         <v>0</v>
       </c>
       <c r="I160" s="145">
-        <f t="shared" si="23"/>
+        <f t="shared" si="31"/>
         <v>501</v>
       </c>
       <c r="J160" s="45">
-        <f t="shared" si="24"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="K160" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>6.8230277185501065E-2</v>
       </c>
       <c r="L160" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>9.8296199213630409E-3</v>
       </c>
       <c r="M160" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>0.17535728080339899</v>
       </c>
       <c r="N160" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="O160" s="48">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>0.10929319371727748</v>
       </c>
     </row>
@@ -6161,31 +6750,31 @@
         <v>0</v>
       </c>
       <c r="I161" s="145">
-        <f t="shared" si="23"/>
+        <f t="shared" si="31"/>
         <v>408</v>
       </c>
       <c r="J161" s="45">
-        <f t="shared" si="24"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="K161" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>2.1321961620469083E-3</v>
       </c>
       <c r="L161" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>5.8977719528178242E-2</v>
       </c>
       <c r="M161" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>0.12244109694862881</v>
       </c>
       <c r="N161" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="O161" s="48">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>8.9005235602094238E-2</v>
       </c>
     </row>
@@ -6213,31 +6802,31 @@
         <v>0</v>
       </c>
       <c r="I162" s="145">
-        <f t="shared" si="23"/>
+        <f t="shared" si="31"/>
         <v>490</v>
       </c>
       <c r="J162" s="45">
-        <f t="shared" si="24"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="K162" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>5.3304904051172705E-2</v>
       </c>
       <c r="L162" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>0.10091743119266056</v>
       </c>
       <c r="M162" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>0.1201235998455002</v>
       </c>
       <c r="N162" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="O162" s="48">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>0.10689354275741711</v>
       </c>
     </row>
@@ -6265,31 +6854,31 @@
         <v>0</v>
       </c>
       <c r="I163" s="145">
-        <f t="shared" si="23"/>
+        <f t="shared" si="31"/>
         <v>296</v>
       </c>
       <c r="J163" s="45">
-        <f t="shared" si="24"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="K163" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>0.22601279317697229</v>
       </c>
       <c r="L163" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>9.1743119266055051E-3</v>
       </c>
       <c r="M163" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>6.7979915025106225E-2</v>
       </c>
       <c r="N163" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="O163" s="48">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>6.4572425828970326E-2</v>
       </c>
     </row>
@@ -6317,31 +6906,31 @@
         <v>0</v>
       </c>
       <c r="I164" s="145">
-        <f t="shared" si="23"/>
+        <f t="shared" si="31"/>
         <v>246</v>
       </c>
       <c r="J164" s="45">
-        <f t="shared" si="24"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="K164" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>3.4115138592750532E-2</v>
       </c>
       <c r="L164" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>0.15072083879423329</v>
       </c>
       <c r="M164" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="N164" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="O164" s="48">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>5.3664921465968587E-2</v>
       </c>
     </row>
@@ -6369,31 +6958,31 @@
         <v>0</v>
       </c>
       <c r="I165" s="145">
-        <f t="shared" si="23"/>
+        <f t="shared" si="31"/>
         <v>654</v>
       </c>
       <c r="J165" s="45">
-        <f t="shared" si="24"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="K165" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>0.15991471215351813</v>
       </c>
       <c r="L165" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>0.30013106159895153</v>
       </c>
       <c r="M165" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>4.6736191579760528E-2</v>
       </c>
       <c r="N165" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="O165" s="48">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>0.14267015706806283</v>
       </c>
     </row>
@@ -6421,31 +7010,31 @@
         <v>0</v>
       </c>
       <c r="I166" s="145">
-        <f t="shared" si="23"/>
+        <f t="shared" si="31"/>
         <v>439</v>
       </c>
       <c r="J166" s="45">
-        <f t="shared" si="24"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="K166" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>2.5586353944562899E-2</v>
       </c>
       <c r="L166" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>5.3079947575360421E-2</v>
       </c>
       <c r="M166" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>0.1336423329470838</v>
       </c>
       <c r="N166" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="O166" s="48">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>9.5767888307155324E-2</v>
       </c>
     </row>
@@ -6473,31 +7062,31 @@
         <v>0</v>
       </c>
       <c r="I167" s="145">
-        <f t="shared" si="23"/>
+        <f t="shared" si="31"/>
         <v>615</v>
       </c>
       <c r="J167" s="49">
-        <f t="shared" si="24"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="K167" s="50">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>0.42857142857142855</v>
       </c>
       <c r="L167" s="50">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>0.17234600262123198</v>
       </c>
       <c r="M167" s="50">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>5.8323677095403634E-2</v>
       </c>
       <c r="N167" s="50">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="O167" s="51">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>0.13416230366492146</v>
       </c>
     </row>
@@ -7079,7 +7668,7 @@
         <v>30</v>
       </c>
       <c r="F200" s="11">
-        <f t="shared" ref="F200:F204" si="25">D200/E200 * 60</f>
+        <f t="shared" ref="F200:F204" si="33">D200/E200 * 60</f>
         <v>0.4</v>
       </c>
       <c r="K200">
@@ -7133,7 +7722,7 @@
         <v>30</v>
       </c>
       <c r="F201" s="11">
-        <f t="shared" si="25"/>
+        <f t="shared" si="33"/>
         <v>0.4</v>
       </c>
       <c r="K201">
@@ -7187,7 +7776,7 @@
         <v>30</v>
       </c>
       <c r="F202" s="11">
-        <f t="shared" si="25"/>
+        <f t="shared" si="33"/>
         <v>0.4</v>
       </c>
       <c r="K202">
@@ -7241,7 +7830,7 @@
         <v>30</v>
       </c>
       <c r="F203" s="11">
-        <f t="shared" si="25"/>
+        <f t="shared" si="33"/>
         <v>0.4</v>
       </c>
     </row>
@@ -7259,7 +7848,7 @@
         <v>50</v>
       </c>
       <c r="F204" s="16">
-        <f t="shared" si="25"/>
+        <f t="shared" si="33"/>
         <v>1.2</v>
       </c>
     </row>
@@ -7342,19 +7931,19 @@
         <v>0</v>
       </c>
       <c r="E209" s="175">
-        <f t="shared" ref="E209:H209" si="26">SUM(E211:E222)</f>
+        <f t="shared" ref="E209:H209" si="34">SUM(E211:E222)</f>
         <v>142.26999999999998</v>
       </c>
       <c r="F209" s="175">
-        <f t="shared" si="26"/>
+        <f t="shared" si="34"/>
         <v>1232.05</v>
       </c>
       <c r="G209" s="175">
-        <f t="shared" si="26"/>
+        <f t="shared" si="34"/>
         <v>3316.4900000000002</v>
       </c>
       <c r="H209" s="175">
-        <f t="shared" si="26"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="I209" s="179">
@@ -7366,19 +7955,19 @@
         <v>0</v>
       </c>
       <c r="K209" s="46">
-        <f t="shared" ref="K209:N209" si="27">E209/$I$209</f>
+        <f t="shared" ref="K209:N209" si="35">E209/$I$209</f>
         <v>3.0329516650642419E-2</v>
       </c>
       <c r="L209" s="46">
-        <f t="shared" si="27"/>
+        <f t="shared" si="35"/>
         <v>0.26265186609562097</v>
       </c>
       <c r="M209" s="46">
-        <f t="shared" si="27"/>
+        <f t="shared" si="35"/>
         <v>0.7070186172537366</v>
       </c>
       <c r="N209" s="46">
-        <f t="shared" si="27"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="O209" s="47">
@@ -7435,19 +8024,19 @@
         <v>0</v>
       </c>
       <c r="K211" s="46">
-        <f t="shared" ref="K211:O222" si="28">IF(E$209&gt;0,E211/E$209,0)</f>
+        <f t="shared" ref="K211:O222" si="36">IF(E$209&gt;0,E211/E$209,0)</f>
         <v>0</v>
       </c>
       <c r="L211" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>2.329450915141431E-2</v>
       </c>
       <c r="M211" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>0.10891333910248484</v>
       </c>
       <c r="N211" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="O211" s="48">
@@ -7478,31 +8067,31 @@
         <v>0</v>
       </c>
       <c r="I212" s="180">
-        <f t="shared" ref="I212:I222" si="29">SUM(D212:H212)</f>
+        <f t="shared" ref="I212:I222" si="37">SUM(D212:H212)</f>
         <v>389.49999999999994</v>
       </c>
       <c r="J212" s="45">
-        <f t="shared" ref="J212:J222" si="30">IF(D$209&gt;0,D212/D$209,0)</f>
+        <f t="shared" ref="J212:J222" si="38">IF(D$209&gt;0,D212/D$209,0)</f>
         <v>0</v>
       </c>
       <c r="K212" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>0.21613832853025935</v>
       </c>
       <c r="L212" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>5.6572379367720471E-2</v>
       </c>
       <c r="M212" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>8.7155396217084916E-2</v>
       </c>
       <c r="N212" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="O212" s="48">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>8.3034699764006625E-2</v>
       </c>
     </row>
@@ -7529,31 +8118,31 @@
         <v>0</v>
       </c>
       <c r="I213" s="180">
-        <f t="shared" si="29"/>
+        <f t="shared" si="37"/>
         <v>410.40999999999997</v>
       </c>
       <c r="J213" s="45">
-        <f t="shared" si="30"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="K213" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>0.26224783861671469</v>
       </c>
       <c r="L213" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>9.9833610648918464E-2</v>
       </c>
       <c r="M213" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>7.5411052045988372E-2</v>
       </c>
       <c r="N213" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="O213" s="48">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>8.749235206712698E-2</v>
       </c>
     </row>
@@ -7580,31 +8169,31 @@
         <v>0</v>
       </c>
       <c r="I214" s="180">
-        <f t="shared" si="29"/>
+        <f t="shared" si="37"/>
         <v>391.55</v>
       </c>
       <c r="J214" s="45">
-        <f t="shared" si="30"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="K214" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="L214" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>5.9900166389351084E-2</v>
       </c>
       <c r="M214" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>9.5809123501050808E-2</v>
       </c>
       <c r="N214" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="O214" s="48">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>8.3471724499606673E-2</v>
       </c>
     </row>
@@ -7631,31 +8220,31 @@
         <v>0</v>
       </c>
       <c r="I215" s="180">
-        <f t="shared" si="29"/>
+        <f t="shared" si="37"/>
         <v>403.85</v>
       </c>
       <c r="J215" s="45">
-        <f t="shared" si="30"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="K215" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="L215" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>7.8202995008319467E-2</v>
       </c>
       <c r="M215" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>9.2718506613920129E-2</v>
       </c>
       <c r="N215" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="O215" s="48">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>8.6093872913206887E-2</v>
       </c>
     </row>
@@ -7682,31 +8271,31 @@
         <v>0</v>
       </c>
       <c r="I216" s="180">
-        <f t="shared" si="29"/>
+        <f t="shared" si="37"/>
         <v>395.65</v>
       </c>
       <c r="J216" s="45">
-        <f t="shared" si="30"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="K216" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>2.0172910662824207E-2</v>
       </c>
       <c r="L216" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>0.11813643926788685</v>
       </c>
       <c r="M216" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>7.454567931759179E-2</v>
       </c>
       <c r="N216" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="O216" s="48">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>8.4345773970806739E-2</v>
       </c>
       <c r="Q216" t="s">
@@ -7736,31 +8325,31 @@
         <v>0</v>
       </c>
       <c r="I217" s="180">
-        <f t="shared" si="29"/>
+        <f t="shared" si="37"/>
         <v>215.25</v>
       </c>
       <c r="J217" s="45">
-        <f t="shared" si="30"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="K217" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="L217" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>7.4875207986688855E-2</v>
       </c>
       <c r="M217" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>3.7087402645568049E-2</v>
       </c>
       <c r="N217" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="O217" s="48">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>4.5887597238003668E-2</v>
       </c>
     </row>
@@ -7787,31 +8376,31 @@
         <v>0</v>
       </c>
       <c r="I218" s="180">
-        <f t="shared" si="29"/>
+        <f t="shared" si="37"/>
         <v>436.65</v>
       </c>
       <c r="J218" s="45">
-        <f t="shared" si="30"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="K218" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>8.645533141210375E-2</v>
       </c>
       <c r="L218" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>0.11148086522462562</v>
       </c>
       <c r="M218" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>8.6537272839658785E-2</v>
       </c>
       <c r="N218" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="O218" s="48">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>9.3086268682807435E-2</v>
       </c>
     </row>
@@ -7838,31 +8427,31 @@
         <v>0</v>
       </c>
       <c r="I219" s="180">
-        <f t="shared" si="29"/>
+        <f t="shared" si="37"/>
         <v>430.09000000000003</v>
       </c>
       <c r="J219" s="45">
-        <f t="shared" si="30"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="K219" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>6.9164265129683003E-2</v>
       </c>
       <c r="L219" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>9.1514143094841932E-2</v>
       </c>
       <c r="M219" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>9.2718506613920129E-2</v>
       </c>
       <c r="N219" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="O219" s="48">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>9.1687789528887328E-2</v>
       </c>
     </row>
@@ -7889,31 +8478,31 @@
         <v>0</v>
       </c>
       <c r="I220" s="180">
-        <f t="shared" si="29"/>
+        <f t="shared" si="37"/>
         <v>426.4</v>
       </c>
       <c r="J220" s="45">
-        <f t="shared" si="30"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="K220" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="L220" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>0.1098169717138103</v>
       </c>
       <c r="M220" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>8.7773519594511046E-2</v>
       </c>
       <c r="N220" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="O220" s="48">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>9.0901145004807254E-2</v>
       </c>
     </row>
@@ -7940,31 +8529,31 @@
         <v>0</v>
       </c>
       <c r="I221" s="180">
-        <f t="shared" si="29"/>
+        <f t="shared" si="37"/>
         <v>410</v>
       </c>
       <c r="J221" s="45">
-        <f t="shared" si="30"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="K221" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>0.1729106628242075</v>
       </c>
       <c r="L221" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>7.9866888519134774E-2</v>
       </c>
       <c r="M221" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>8.6537272839658785E-2</v>
       </c>
       <c r="N221" s="46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="O221" s="48">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>8.7404947120006987E-2</v>
       </c>
     </row>
@@ -7991,31 +8580,31 @@
         <v>0</v>
       </c>
       <c r="I222" s="181">
-        <f t="shared" si="29"/>
+        <f t="shared" si="37"/>
         <v>391.54999999999995</v>
       </c>
       <c r="J222" s="49">
-        <f t="shared" si="30"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="K222" s="50">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>0.1729106628242075</v>
       </c>
       <c r="L222" s="50">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>9.6505823627287851E-2</v>
       </c>
       <c r="M222" s="50">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>7.4792928668562228E-2</v>
       </c>
       <c r="N222" s="50">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="O222" s="51">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>8.3471724499606659E-2</v>
       </c>
     </row>
@@ -11786,8 +12375,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B2:E59"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12405,7 +12994,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -13051,8 +13640,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="B2:I37"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13476,8 +14065,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="B2:E29"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:XFD29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed train cancelling issue Pre-Meeting runs
</commit_message>
<xml_diff>
--- a/Rolleston Workzones_ps_140327.xlsx
+++ b/Rolleston Workzones_ps_140327.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="15360" windowHeight="8370" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="15360" windowHeight="8370"/>
   </bookViews>
   <sheets>
     <sheet name="Working Locations" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="271">
   <si>
     <t>Work Zone</t>
   </si>
@@ -830,6 +830,15 @@
   </si>
   <si>
     <t>Gamma</t>
+  </si>
+  <si>
+    <t>Inputs</t>
+  </si>
+  <si>
+    <t>Base</t>
+  </si>
+  <si>
+    <t>Cuml. Diff</t>
   </si>
 </sst>
 </file>
@@ -1485,7 +1494,7 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="219">
+  <cellXfs count="220">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="6" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1861,6 +1870,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="17" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="Comma" xfId="17" builtinId="3"/>
@@ -1896,6 +1906,281 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Working Locations'!$V$97:$V$108</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>-209183.6986301369</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-484528.52054794505</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-545473.3424657532</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-409217.04109588987</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-171411.86301369802</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9754.4383561650757</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>339709.61643835693</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>321024.79452054866</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>338213.34246575425</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>228028.5205479461</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-121255.1780821908</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0477378964424133E-9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="346534320"/>
+        <c:axId val="346535104"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="346534320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="346535104"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="346535104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="346534320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2124,8 +2409,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="369704768"/>
-        <c:axId val="369705160"/>
+        <c:axId val="282492576"/>
+        <c:axId val="282492968"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2342,11 +2627,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="372355016"/>
-        <c:axId val="373300072"/>
+        <c:axId val="344914272"/>
+        <c:axId val="344913488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="369704768"/>
+        <c:axId val="282492576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2389,7 +2674,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="369705160"/>
+        <c:crossAx val="282492968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2397,7 +2682,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="369705160"/>
+        <c:axId val="282492968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2448,12 +2733,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="369704768"/>
+        <c:crossAx val="282492576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="373300072"/>
+        <c:axId val="344913488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2490,12 +2775,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="372355016"/>
+        <c:crossAx val="344914272"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="372355016"/>
+        <c:axId val="344914272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2505,7 +2790,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="373300072"/>
+        <c:crossAx val="344913488"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2596,7 +2882,550 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3116,6 +3945,41 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
       <xdr:row>3</xdr:row>
@@ -3435,10 +4299,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A2:V249"/>
+  <dimension ref="A2:AB249"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16:J16"/>
+    <sheetView tabSelected="1" topLeftCell="F84" workbookViewId="0">
+      <selection activeCell="J120" sqref="J120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3446,8 +4310,9 @@
     <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.85546875" customWidth="1"/>
-    <col min="17" max="17" width="20.140625" customWidth="1"/>
-    <col min="18" max="18" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.7109375" customWidth="1"/>
+    <col min="20" max="23" width="20.140625" customWidth="1"/>
+    <col min="24" max="24" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:15" ht="22.5" x14ac:dyDescent="0.3">
@@ -3696,7 +4561,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="182"/>
       <c r="B17" s="112"/>
       <c r="C17" s="113" t="s">
@@ -3721,7 +4586,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="182"/>
       <c r="B18" s="112"/>
       <c r="C18" s="113" t="s">
@@ -3746,7 +4611,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="182"/>
       <c r="B19" s="116" t="s">
         <v>31</v>
@@ -3773,7 +4638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="182"/>
       <c r="B20" s="112"/>
       <c r="C20" s="113" t="s">
@@ -3798,7 +4663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="182"/>
       <c r="B21" s="117"/>
       <c r="C21" s="118" t="s">
@@ -3823,10 +4688,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="182"/>
     </row>
-    <row r="23" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="182"/>
       <c r="B23" s="21" t="s">
         <v>84</v>
@@ -3835,7 +4700,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="182"/>
       <c r="B24" s="43"/>
       <c r="C24" s="54"/>
@@ -3855,11 +4720,11 @@
       <c r="M24" s="34"/>
       <c r="N24" s="34"/>
       <c r="O24" s="35"/>
-      <c r="S24">
+      <c r="Y24">
         <v>12000000</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="182"/>
       <c r="B25" s="39"/>
       <c r="C25" s="56" t="s">
@@ -3901,13 +4766,16 @@
       <c r="O25" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="Q25" s="44"/>
-      <c r="R25" s="44"/>
-      <c r="S25">
+      <c r="T25" s="44"/>
+      <c r="U25" s="44"/>
+      <c r="V25" s="44"/>
+      <c r="W25" s="44"/>
+      <c r="X25" s="44"/>
+      <c r="Y25">
         <v>12000000</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="182"/>
       <c r="B26" s="61" t="s">
         <v>38</v>
@@ -3964,7 +4832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" s="182"/>
       <c r="B27" s="36" t="s">
         <v>39</v>
@@ -3982,11 +4850,14 @@
       <c r="M27" s="37"/>
       <c r="N27" s="37"/>
       <c r="O27" s="38"/>
-      <c r="Q27" s="212"/>
-      <c r="R27" s="212"/>
-      <c r="S27" s="212"/>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T27" s="212"/>
+      <c r="U27" s="212"/>
+      <c r="V27" s="212"/>
+      <c r="W27" s="212"/>
+      <c r="X27" s="212"/>
+      <c r="Y27" s="212"/>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" s="182"/>
       <c r="B28" s="59" t="s">
         <v>40</v>
@@ -4040,24 +4911,27 @@
       <c r="P28">
         <v>31</v>
       </c>
-      <c r="Q28" s="217">
-        <f>($S$25/365)*P28</f>
+      <c r="T28" s="217">
+        <f>($Y$25/365)*P28</f>
         <v>1019178.0821917807</v>
       </c>
-      <c r="R28" s="212">
+      <c r="U28" s="217"/>
+      <c r="V28" s="217"/>
+      <c r="W28" s="217"/>
+      <c r="X28" s="212">
         <f>I28*1000</f>
         <v>481000</v>
       </c>
-      <c r="S28" s="212">
-        <f>Q28-R28</f>
+      <c r="Y28" s="212">
+        <f>T28-X28</f>
         <v>538178.08219178068</v>
       </c>
-      <c r="T28">
-        <f>S28/$S$40</f>
+      <c r="Z28">
+        <f>Y28/$Y$40</f>
         <v>7.3996711424691414E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" s="182"/>
       <c r="B29" s="59" t="s">
         <v>41</v>
@@ -4111,24 +4985,27 @@
       <c r="P29">
         <v>28</v>
       </c>
-      <c r="Q29" s="217">
-        <f t="shared" ref="Q29:Q39" si="11">($S$25/365)*P29</f>
+      <c r="T29" s="217">
+        <f t="shared" ref="T29:T39" si="11">($Y$25/365)*P29</f>
         <v>920547.94520547939</v>
       </c>
-      <c r="R29" s="212">
-        <f t="shared" ref="R29:R39" si="12">I29*1000</f>
+      <c r="U29" s="217"/>
+      <c r="V29" s="217"/>
+      <c r="W29" s="217"/>
+      <c r="X29" s="212">
+        <f t="shared" ref="X29:X39" si="12">I29*1000</f>
         <v>181000</v>
       </c>
-      <c r="S29" s="212">
-        <f t="shared" ref="S29:S39" si="13">Q29-R29</f>
+      <c r="Y29" s="212">
+        <f t="shared" ref="Y29:Y39" si="13">T29-X29</f>
         <v>739547.94520547939</v>
       </c>
-      <c r="T29">
-        <f t="shared" ref="T29:T39" si="14">S29/$S$40</f>
+      <c r="Z29">
+        <f t="shared" ref="Z29:Z39" si="14">Y29/$Y$40</f>
         <v>0.10168402931465412</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" s="182"/>
       <c r="B30" s="59" t="s">
         <v>42</v>
@@ -4182,24 +5059,27 @@
       <c r="P30">
         <v>31</v>
       </c>
-      <c r="Q30" s="217">
+      <c r="T30" s="217">
         <f t="shared" si="11"/>
         <v>1019178.0821917807</v>
       </c>
-      <c r="R30" s="212">
+      <c r="U30" s="217"/>
+      <c r="V30" s="217"/>
+      <c r="W30" s="217"/>
+      <c r="X30" s="212">
         <f t="shared" si="12"/>
         <v>563000</v>
       </c>
-      <c r="S30" s="212">
+      <c r="Y30" s="212">
         <f t="shared" si="13"/>
         <v>456178.08219178068</v>
       </c>
-      <c r="T30">
+      <c r="Z30">
         <f t="shared" si="14"/>
         <v>6.2722134221336545E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" s="182"/>
       <c r="B31" s="59" t="s">
         <v>43</v>
@@ -4253,24 +5133,27 @@
       <c r="P31">
         <v>30</v>
       </c>
-      <c r="Q31" s="217">
+      <c r="T31" s="217">
         <f t="shared" si="11"/>
         <v>986301.36986301362</v>
       </c>
-      <c r="R31" s="212">
+      <c r="U31" s="217"/>
+      <c r="V31" s="217"/>
+      <c r="W31" s="217"/>
+      <c r="X31" s="212">
         <f t="shared" si="12"/>
         <v>431000</v>
       </c>
-      <c r="S31" s="212">
+      <c r="Y31" s="212">
         <f t="shared" si="13"/>
         <v>555301.36986301362</v>
       </c>
-      <c r="T31">
+      <c r="Z31">
         <f t="shared" si="14"/>
         <v>7.6351075190844719E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" s="182"/>
       <c r="B32" s="59" t="s">
         <v>17</v>
@@ -4324,24 +5207,27 @@
       <c r="P32">
         <v>31</v>
       </c>
-      <c r="Q32" s="217">
+      <c r="T32" s="217">
         <f t="shared" si="11"/>
         <v>1019178.0821917807</v>
       </c>
-      <c r="R32" s="212">
+      <c r="U32" s="217"/>
+      <c r="V32" s="217"/>
+      <c r="W32" s="217"/>
+      <c r="X32" s="212">
         <f t="shared" si="12"/>
         <v>286000</v>
       </c>
-      <c r="S32" s="212">
+      <c r="Y32" s="212">
         <f t="shared" si="13"/>
         <v>733178.08219178068</v>
       </c>
-      <c r="T32">
+      <c r="Z32">
         <f t="shared" si="14"/>
         <v>0.10080820599364508</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="182"/>
       <c r="B33" s="59" t="s">
         <v>44</v>
@@ -4395,24 +5281,27 @@
       <c r="P33">
         <v>30</v>
       </c>
-      <c r="Q33" s="217">
+      <c r="T33" s="217">
         <f t="shared" si="11"/>
         <v>986301.36986301362</v>
       </c>
-      <c r="R33" s="212">
+      <c r="U33" s="217"/>
+      <c r="V33" s="217"/>
+      <c r="W33" s="217"/>
+      <c r="X33" s="212">
         <f t="shared" si="12"/>
         <v>534000</v>
       </c>
-      <c r="S33" s="212">
+      <c r="Y33" s="212">
         <f t="shared" si="13"/>
         <v>452301.36986301362</v>
       </c>
-      <c r="T33">
+      <c r="Z33">
         <f t="shared" si="14"/>
         <v>6.2189106264679446E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="182"/>
       <c r="B34" s="59" t="s">
         <v>45</v>
@@ -4466,24 +5355,27 @@
       <c r="P34">
         <v>31</v>
       </c>
-      <c r="Q34" s="217">
+      <c r="T34" s="217">
         <f t="shared" si="11"/>
         <v>1019178.0821917807</v>
       </c>
-      <c r="R34" s="212">
+      <c r="U34" s="217"/>
+      <c r="V34" s="217"/>
+      <c r="W34" s="217"/>
+      <c r="X34" s="212">
         <f t="shared" si="12"/>
         <v>304000</v>
       </c>
-      <c r="S34" s="212">
+      <c r="Y34" s="212">
         <f t="shared" si="13"/>
         <v>715178.08219178068</v>
       </c>
-      <c r="T34">
+      <c r="Z34">
         <f t="shared" si="14"/>
         <v>9.833329880266474E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="182"/>
       <c r="B35" s="59" t="s">
         <v>46</v>
@@ -4537,24 +5429,27 @@
       <c r="P35">
         <v>31</v>
       </c>
-      <c r="Q35" s="217">
+      <c r="T35" s="217">
         <f t="shared" si="11"/>
         <v>1019178.0821917807</v>
       </c>
-      <c r="R35" s="212">
+      <c r="U35" s="217"/>
+      <c r="V35" s="217"/>
+      <c r="W35" s="217"/>
+      <c r="X35" s="212">
         <f t="shared" si="12"/>
         <v>364000</v>
       </c>
-      <c r="S35" s="212">
+      <c r="Y35" s="212">
         <f t="shared" si="13"/>
         <v>655178.08219178068</v>
       </c>
-      <c r="T35">
+      <c r="Z35">
         <f t="shared" si="14"/>
         <v>9.0083608166063617E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="182"/>
       <c r="B36" s="59" t="s">
         <v>47</v>
@@ -4608,24 +5503,27 @@
       <c r="P36">
         <v>30</v>
       </c>
-      <c r="Q36" s="217">
+      <c r="T36" s="217">
         <f t="shared" si="11"/>
         <v>986301.36986301362</v>
       </c>
-      <c r="R36" s="212">
+      <c r="U36" s="217"/>
+      <c r="V36" s="217"/>
+      <c r="W36" s="217"/>
+      <c r="X36" s="212">
         <f t="shared" si="12"/>
         <v>522000</v>
       </c>
-      <c r="S36" s="212">
+      <c r="Y36" s="212">
         <f t="shared" si="13"/>
         <v>464301.36986301362</v>
       </c>
-      <c r="T36">
+      <c r="Z36">
         <f t="shared" si="14"/>
         <v>6.3839044391999666E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" s="182"/>
       <c r="B37" s="59" t="s">
         <v>48</v>
@@ -4679,24 +5577,27 @@
       <c r="P37">
         <v>31</v>
       </c>
-      <c r="Q37" s="217">
+      <c r="T37" s="217">
         <f t="shared" si="11"/>
         <v>1019178.0821917807</v>
       </c>
-      <c r="R37" s="212">
+      <c r="U37" s="217"/>
+      <c r="V37" s="217"/>
+      <c r="W37" s="217"/>
+      <c r="X37" s="212">
         <f t="shared" si="12"/>
         <v>282000</v>
       </c>
-      <c r="S37" s="212">
+      <c r="Y37" s="212">
         <f t="shared" si="13"/>
         <v>737178.08219178068</v>
       </c>
-      <c r="T37">
+      <c r="Z37">
         <f t="shared" si="14"/>
         <v>0.10135818536941849</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" s="182"/>
       <c r="B38" s="59" t="s">
         <v>49</v>
@@ -4750,24 +5651,27 @@
       <c r="P38">
         <v>30</v>
       </c>
-      <c r="Q38" s="217">
+      <c r="T38" s="217">
         <f t="shared" si="11"/>
         <v>986301.36986301362</v>
       </c>
-      <c r="R38" s="212">
+      <c r="U38" s="217"/>
+      <c r="V38" s="217"/>
+      <c r="W38" s="217"/>
+      <c r="X38" s="212">
         <f t="shared" si="12"/>
         <v>505000</v>
       </c>
-      <c r="S38" s="212">
+      <c r="Y38" s="212">
         <f t="shared" si="13"/>
         <v>481301.36986301362</v>
       </c>
-      <c r="T38">
+      <c r="Z38">
         <f t="shared" si="14"/>
         <v>6.617645673903666E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="182"/>
       <c r="B39" s="58" t="s">
         <v>50</v>
@@ -4821,24 +5725,27 @@
       <c r="P39">
         <v>31</v>
       </c>
-      <c r="Q39" s="217">
+      <c r="T39" s="217">
         <f t="shared" si="11"/>
         <v>1019178.0821917807</v>
       </c>
-      <c r="R39" s="212">
+      <c r="U39" s="217"/>
+      <c r="V39" s="217"/>
+      <c r="W39" s="217"/>
+      <c r="X39" s="212">
         <f t="shared" si="12"/>
         <v>274000</v>
       </c>
-      <c r="S39" s="212">
+      <c r="Y39" s="212">
         <f t="shared" si="13"/>
         <v>745178.08219178068</v>
       </c>
-      <c r="T39">
+      <c r="Z39">
         <f t="shared" si="14"/>
         <v>0.10245814412096531</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:26" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="182"/>
       <c r="B40" s="99" t="s">
         <v>190</v>
@@ -4862,15 +5769,15 @@
       <c r="M40" s="46"/>
       <c r="N40" s="46"/>
       <c r="O40" s="46"/>
-      <c r="S40" s="212">
-        <f>SUM(S28:S39)</f>
+      <c r="Y40" s="212">
+        <f>SUM(Y28:Y39)</f>
         <v>7273000</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" s="182"/>
     </row>
-    <row r="42" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="182"/>
       <c r="B42" s="21" t="s">
         <v>201</v>
@@ -4879,7 +5786,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43" s="182"/>
       <c r="B43" s="65" t="s">
         <v>52</v>
@@ -4920,7 +5827,7 @@
         <v>5.6842105263157894</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44" s="182"/>
       <c r="B44" s="41" t="s">
         <v>54</v>
@@ -4961,7 +5868,7 @@
         <v>6.1714285714285717</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="182"/>
       <c r="B45" s="42" t="s">
         <v>55</v>
@@ -5002,7 +5909,7 @@
         <v>7.1999999999999993</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" s="182"/>
       <c r="B46" s="57"/>
       <c r="C46" s="44"/>
@@ -5013,7 +5920,7 @@
       <c r="H46" s="80"/>
       <c r="I46" s="79"/>
     </row>
-    <row r="47" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="182"/>
       <c r="B47" s="82" t="s">
         <v>121</v>
@@ -5026,7 +5933,7 @@
       <c r="H47" s="80"/>
       <c r="I47" s="79"/>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48" s="182"/>
       <c r="B48" s="83" t="s">
         <v>204</v>
@@ -5601,7 +6508,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="81" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A81" s="184"/>
       <c r="B81" s="41"/>
       <c r="C81" s="29" t="s">
@@ -5618,7 +6525,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="82" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A82" s="184"/>
       <c r="B82" s="41"/>
       <c r="C82" s="29" t="s">
@@ -5635,7 +6542,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="83" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A83" s="184"/>
       <c r="B83" s="8" t="s">
         <v>31</v>
@@ -5654,7 +6561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A84" s="184"/>
       <c r="B84" s="41"/>
       <c r="C84" s="29" t="s">
@@ -5671,7 +6578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="184"/>
       <c r="B85" s="42"/>
       <c r="C85" s="193" t="s">
@@ -5688,7 +6595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A86" s="184"/>
       <c r="B86" s="37"/>
       <c r="C86" s="37"/>
@@ -5696,13 +6603,13 @@
       <c r="E86" s="194"/>
       <c r="F86" s="195"/>
     </row>
-    <row r="87" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="184"/>
       <c r="B87" s="21" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="88" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A88" s="184"/>
       <c r="B88" s="43"/>
       <c r="C88" s="54"/>
@@ -5723,7 +6630,7 @@
       <c r="N88" s="34"/>
       <c r="O88" s="35"/>
     </row>
-    <row r="89" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="184"/>
       <c r="B89" s="39"/>
       <c r="C89" s="56" t="s">
@@ -5765,8 +6672,11 @@
       <c r="O89" s="64" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="90" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="R89">
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="90" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A90" s="184"/>
       <c r="B90" s="61" t="s">
         <v>38</v>
@@ -5822,16 +6732,19 @@
         <f>SUM(J90:N90)</f>
         <v>1</v>
       </c>
-      <c r="Q90" s="212"/>
-      <c r="R90" s="212">
-        <v>14000000</v>
-      </c>
-      <c r="S90" s="212"/>
       <c r="T90" s="212"/>
       <c r="U90" s="212"/>
       <c r="V90" s="212"/>
-    </row>
-    <row r="91" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W90" s="212"/>
+      <c r="X90" s="212">
+        <v>14000000</v>
+      </c>
+      <c r="Y90" s="212"/>
+      <c r="Z90" s="212"/>
+      <c r="AA90" s="212"/>
+      <c r="AB90" s="212"/>
+    </row>
+    <row r="91" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A91" s="184"/>
       <c r="B91" s="36" t="s">
         <v>39</v>
@@ -5849,14 +6762,23 @@
       <c r="M91" s="37"/>
       <c r="N91" s="37"/>
       <c r="O91" s="38"/>
-      <c r="Q91" s="212"/>
-      <c r="R91" s="212"/>
-      <c r="S91" s="212"/>
-      <c r="T91" s="212"/>
-      <c r="U91" s="212"/>
-      <c r="V91" s="212"/>
-    </row>
-    <row r="92" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="T91" s="212" t="s">
+        <v>269</v>
+      </c>
+      <c r="U91" s="212" t="s">
+        <v>268</v>
+      </c>
+      <c r="V91" s="212" t="s">
+        <v>270</v>
+      </c>
+      <c r="W91" s="212"/>
+      <c r="X91" s="212"/>
+      <c r="Y91" s="212"/>
+      <c r="Z91" s="212"/>
+      <c r="AA91" s="212"/>
+      <c r="AB91" s="212"/>
+    </row>
+    <row r="92" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A92" s="184"/>
       <c r="B92" s="59" t="s">
         <v>40</v>
@@ -5910,28 +6832,49 @@
       <c r="P92">
         <v>31</v>
       </c>
-      <c r="Q92" s="212">
-        <f t="shared" ref="Q92:Q103" si="20">($R$90/365)*P92</f>
-        <v>1189041.0958904109</v>
-      </c>
-      <c r="R92" s="217">
+      <c r="Q92" s="217">
+        <f>P92*24</f>
+        <v>744</v>
+      </c>
+      <c r="R92" s="212">
+        <f>Q92/$R$89</f>
+        <v>141.71428571428572</v>
+      </c>
+      <c r="S92" s="212">
+        <f>R92*8100</f>
+        <v>1147885.7142857143</v>
+      </c>
+      <c r="T92" s="212">
+        <f>($U$104/365)*P92</f>
+        <v>1046594.8219178081</v>
+      </c>
+      <c r="U92" s="219">
+        <f>(I92+I156+I211)*1000</f>
+        <v>1027909.9999999999</v>
+      </c>
+      <c r="V92" s="219"/>
+      <c r="W92" s="219">
+        <f>U92-T92</f>
+        <v>-18684.821917808265</v>
+      </c>
+      <c r="X92" s="217">
         <f>(I92+I156)*1000</f>
         <v>638000</v>
       </c>
-      <c r="S92" s="212">
-        <f>Q92-R92</f>
-        <v>551041.09589041094</v>
-      </c>
-      <c r="T92" s="212">
-        <f>S92/2</f>
-        <v>275520.54794520547</v>
-      </c>
-      <c r="U92" s="212">
-        <f>T92/$T$104</f>
-        <v>8.6532835409926331E-2</v>
-      </c>
-    </row>
-    <row r="93" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Y92" s="212">
+        <f>T92-X92</f>
+        <v>408594.82191780815</v>
+      </c>
+      <c r="Z92" s="212">
+        <f>Y92/2</f>
+        <v>204297.41095890407</v>
+      </c>
+      <c r="AA92" s="212">
+        <f>Z92/$Z$104</f>
+        <v>8.7105387324962702E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A93" s="184"/>
       <c r="B93" s="59" t="s">
         <v>41</v>
@@ -5955,11 +6898,11 @@
         <v>0</v>
       </c>
       <c r="I93" s="145">
-        <f t="shared" ref="I93:I103" si="21">SUM(D93:H93)</f>
+        <f t="shared" ref="I93:I103" si="20">SUM(D93:H93)</f>
         <v>405</v>
       </c>
       <c r="J93" s="45">
-        <f t="shared" ref="J93:J103" si="22">IF(D$90&gt;0,D93/D$90,0)</f>
+        <f t="shared" ref="J93:J103" si="21">IF(D$90&gt;0,D93/D$90,0)</f>
         <v>0</v>
       </c>
       <c r="K93" s="46">
@@ -5985,28 +6928,49 @@
       <c r="P93">
         <v>28</v>
       </c>
-      <c r="Q93" s="212">
-        <f t="shared" si="20"/>
-        <v>1073972.602739726</v>
-      </c>
-      <c r="R93" s="217">
-        <f t="shared" ref="R93:R103" si="23">(I93+I157)*1000</f>
+      <c r="Q93" s="217">
+        <f t="shared" ref="Q93:Q103" si="22">P93*24</f>
+        <v>672</v>
+      </c>
+      <c r="R93" s="212">
+        <f t="shared" ref="R93:R103" si="23">Q93/$R$89</f>
+        <v>128</v>
+      </c>
+      <c r="S93" s="212">
+        <f t="shared" ref="S93:S103" si="24">R93*8100</f>
+        <v>1036800</v>
+      </c>
+      <c r="T93" s="212">
+        <f t="shared" ref="T93:T103" si="25">($U$104/365)*P93</f>
+        <v>945311.45205479441</v>
+      </c>
+      <c r="U93" s="219">
+        <f t="shared" ref="U93:U103" si="26">(I93+I157+I212)*1000</f>
+        <v>962500</v>
+      </c>
+      <c r="V93" s="219"/>
+      <c r="W93" s="219">
+        <f t="shared" ref="W93:W103" si="27">U93-T93</f>
+        <v>17188.547945205588</v>
+      </c>
+      <c r="X93" s="217">
+        <f t="shared" ref="X93:X103" si="28">(I93+I157)*1000</f>
         <v>573000</v>
       </c>
-      <c r="S93" s="212">
-        <f t="shared" ref="S93:S103" si="24">Q93-R93</f>
-        <v>500972.60273972596</v>
-      </c>
-      <c r="T93" s="212">
-        <f t="shared" ref="T93:T103" si="25">S93/2</f>
-        <v>250486.30136986298</v>
-      </c>
-      <c r="U93" s="212">
-        <f t="shared" ref="U93:U103" si="26">T93/$T$104</f>
-        <v>7.8670320781992126E-2</v>
-      </c>
-    </row>
-    <row r="94" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Y93" s="212">
+        <f t="shared" ref="Y93:Y103" si="29">T93-X93</f>
+        <v>372311.45205479441</v>
+      </c>
+      <c r="Z93" s="212">
+        <f t="shared" ref="Z93:Z103" si="30">Y93/2</f>
+        <v>186155.72602739721</v>
+      </c>
+      <c r="AA93" s="212">
+        <f t="shared" ref="AA93:AA103" si="31">Z93/$Z$104</f>
+        <v>7.9370397022005698E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A94" s="184"/>
       <c r="B94" s="59" t="s">
         <v>42</v>
@@ -6030,11 +6994,11 @@
         <v>0</v>
       </c>
       <c r="I94" s="145">
+        <f t="shared" si="20"/>
+        <v>352</v>
+      </c>
+      <c r="J94" s="45">
         <f t="shared" si="21"/>
-        <v>352</v>
-      </c>
-      <c r="J94" s="45">
-        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="K94" s="46">
@@ -6060,28 +7024,49 @@
       <c r="P94">
         <v>31</v>
       </c>
-      <c r="Q94" s="212">
-        <f t="shared" si="20"/>
-        <v>1189041.0958904109</v>
-      </c>
-      <c r="R94" s="217">
+      <c r="Q94" s="217">
+        <f t="shared" si="22"/>
+        <v>744</v>
+      </c>
+      <c r="R94" s="212">
         <f t="shared" si="23"/>
-        <v>526000</v>
+        <v>141.71428571428572</v>
       </c>
       <c r="S94" s="212">
         <f t="shared" si="24"/>
-        <v>663041.09589041094</v>
+        <v>1147885.7142857143</v>
       </c>
       <c r="T94" s="212">
         <f t="shared" si="25"/>
-        <v>331520.54794520547</v>
-      </c>
-      <c r="U94" s="212">
+        <v>1046594.8219178081</v>
+      </c>
+      <c r="U94" s="219">
         <f t="shared" si="26"/>
-        <v>0.10412077510841879</v>
-      </c>
-    </row>
-    <row r="95" spans="1:22" x14ac:dyDescent="0.25">
+        <v>936410</v>
+      </c>
+      <c r="V94" s="219"/>
+      <c r="W94" s="219">
+        <f t="shared" si="27"/>
+        <v>-110184.82191780815</v>
+      </c>
+      <c r="X94" s="217">
+        <f t="shared" si="28"/>
+        <v>526000</v>
+      </c>
+      <c r="Y94" s="212">
+        <f t="shared" si="29"/>
+        <v>520594.82191780815</v>
+      </c>
+      <c r="Z94" s="212">
+        <f t="shared" si="30"/>
+        <v>260297.41095890407</v>
+      </c>
+      <c r="AA94" s="212">
+        <f t="shared" si="31"/>
+        <v>0.11098186068457438</v>
+      </c>
+    </row>
+    <row r="95" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A95" s="184"/>
       <c r="B95" s="59" t="s">
         <v>43</v>
@@ -6105,11 +7090,11 @@
         <v>0</v>
       </c>
       <c r="I95" s="145">
+        <f t="shared" si="20"/>
+        <v>272</v>
+      </c>
+      <c r="J95" s="45">
         <f t="shared" si="21"/>
-        <v>272</v>
-      </c>
-      <c r="J95" s="45">
-        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="K95" s="46">
@@ -6135,28 +7120,49 @@
       <c r="P95">
         <v>30</v>
       </c>
-      <c r="Q95" s="212">
-        <f t="shared" si="20"/>
-        <v>1150684.9315068494</v>
-      </c>
-      <c r="R95" s="217">
+      <c r="Q95" s="217">
+        <f t="shared" si="22"/>
+        <v>720</v>
+      </c>
+      <c r="R95" s="212">
         <f t="shared" si="23"/>
-        <v>272000</v>
+        <v>137.14285714285714</v>
       </c>
       <c r="S95" s="212">
         <f t="shared" si="24"/>
-        <v>878684.93150684936</v>
+        <v>1110857.1428571427</v>
       </c>
       <c r="T95" s="212">
         <f t="shared" si="25"/>
-        <v>439342.46575342468</v>
-      </c>
-      <c r="U95" s="212">
+        <v>1012833.6986301369</v>
+      </c>
+      <c r="U95" s="219">
         <f t="shared" si="26"/>
-        <v>0.13798444276175395</v>
-      </c>
-    </row>
-    <row r="96" spans="1:22" x14ac:dyDescent="0.25">
+        <v>663550</v>
+      </c>
+      <c r="V95" s="219"/>
+      <c r="W95" s="219">
+        <f t="shared" si="27"/>
+        <v>-349283.6986301369</v>
+      </c>
+      <c r="X95" s="217">
+        <f t="shared" si="28"/>
+        <v>272000</v>
+      </c>
+      <c r="Y95" s="212">
+        <f t="shared" si="29"/>
+        <v>740833.6986301369</v>
+      </c>
+      <c r="Z95" s="212">
+        <f t="shared" si="30"/>
+        <v>370416.84931506845</v>
+      </c>
+      <c r="AA95" s="212">
+        <f t="shared" si="31"/>
+        <v>0.15793300061825935</v>
+      </c>
+    </row>
+    <row r="96" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A96" s="184"/>
       <c r="B96" s="59" t="s">
         <v>17</v>
@@ -6180,11 +7186,11 @@
         <v>0</v>
       </c>
       <c r="I96" s="145">
+        <f t="shared" si="20"/>
+        <v>263</v>
+      </c>
+      <c r="J96" s="45">
         <f t="shared" si="21"/>
-        <v>263</v>
-      </c>
-      <c r="J96" s="45">
-        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="K96" s="46">
@@ -6210,28 +7216,49 @@
       <c r="P96">
         <v>31</v>
       </c>
-      <c r="Q96" s="212">
-        <f t="shared" si="20"/>
-        <v>1189041.0958904109</v>
-      </c>
-      <c r="R96" s="217">
+      <c r="Q96" s="217">
+        <f t="shared" si="22"/>
+        <v>744</v>
+      </c>
+      <c r="R96" s="212">
         <f t="shared" si="23"/>
-        <v>764000</v>
+        <v>141.71428571428572</v>
       </c>
       <c r="S96" s="212">
         <f t="shared" si="24"/>
-        <v>425041.09589041094</v>
+        <v>1147885.7142857143</v>
       </c>
       <c r="T96" s="212">
         <f t="shared" si="25"/>
-        <v>212520.54794520547</v>
-      </c>
-      <c r="U96" s="212">
+        <v>1046594.8219178081</v>
+      </c>
+      <c r="U96" s="219">
         <f t="shared" si="26"/>
-        <v>6.6746403249122316E-2</v>
-      </c>
-    </row>
-    <row r="97" spans="1:21" x14ac:dyDescent="0.25">
+        <v>1167850</v>
+      </c>
+      <c r="V96" s="219"/>
+      <c r="W96" s="219">
+        <f t="shared" si="27"/>
+        <v>121255.17808219185</v>
+      </c>
+      <c r="X96" s="217">
+        <f t="shared" si="28"/>
+        <v>764000</v>
+      </c>
+      <c r="Y96" s="212">
+        <f t="shared" si="29"/>
+        <v>282594.82191780815</v>
+      </c>
+      <c r="Z96" s="212">
+        <f t="shared" si="30"/>
+        <v>141297.41095890407</v>
+      </c>
+      <c r="AA96" s="212">
+        <f t="shared" si="31"/>
+        <v>6.0244354795399573E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A97" s="184"/>
       <c r="B97" s="59" t="s">
         <v>44</v>
@@ -6255,11 +7282,11 @@
         <v>0</v>
       </c>
       <c r="I97" s="145">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="J97" s="45">
         <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="J97" s="45">
-        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="K97" s="46">
@@ -6285,28 +7312,52 @@
       <c r="P97">
         <v>30</v>
       </c>
-      <c r="Q97" s="212">
-        <f t="shared" si="20"/>
-        <v>1150684.9315068494</v>
-      </c>
-      <c r="R97" s="217">
+      <c r="Q97" s="217">
+        <f t="shared" si="22"/>
+        <v>720</v>
+      </c>
+      <c r="R97" s="212">
         <f t="shared" si="23"/>
-        <v>408000</v>
+        <v>137.14285714285714</v>
       </c>
       <c r="S97" s="212">
         <f t="shared" si="24"/>
-        <v>742684.93150684936</v>
+        <v>1110857.1428571427</v>
       </c>
       <c r="T97" s="212">
         <f t="shared" si="25"/>
-        <v>371342.46575342468</v>
-      </c>
-      <c r="U97" s="212">
+        <v>1012833.6986301369</v>
+      </c>
+      <c r="U97" s="219">
         <f t="shared" si="26"/>
-        <v>0.11662765884215598</v>
-      </c>
-    </row>
-    <row r="98" spans="1:21" x14ac:dyDescent="0.25">
+        <v>803650</v>
+      </c>
+      <c r="V97" s="219">
+        <f>0+W97</f>
+        <v>-209183.6986301369</v>
+      </c>
+      <c r="W97" s="219">
+        <f t="shared" si="27"/>
+        <v>-209183.6986301369</v>
+      </c>
+      <c r="X97" s="217">
+        <f t="shared" si="28"/>
+        <v>408000</v>
+      </c>
+      <c r="Y97" s="212">
+        <f t="shared" si="29"/>
+        <v>604833.6986301369</v>
+      </c>
+      <c r="Z97" s="212">
+        <f t="shared" si="30"/>
+        <v>302416.84931506845</v>
+      </c>
+      <c r="AA97" s="212">
+        <f t="shared" si="31"/>
+        <v>0.12894014011015947</v>
+      </c>
+    </row>
+    <row r="98" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A98" s="184"/>
       <c r="B98" s="59" t="s">
         <v>45</v>
@@ -6330,11 +7381,11 @@
         <v>0</v>
       </c>
       <c r="I98" s="145">
+        <f t="shared" si="20"/>
+        <v>66</v>
+      </c>
+      <c r="J98" s="45">
         <f t="shared" si="21"/>
-        <v>66</v>
-      </c>
-      <c r="J98" s="45">
-        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="K98" s="46">
@@ -6360,28 +7411,52 @@
       <c r="P98">
         <v>31</v>
       </c>
-      <c r="Q98" s="212">
-        <f t="shared" si="20"/>
-        <v>1189041.0958904109</v>
-      </c>
-      <c r="R98" s="217">
+      <c r="Q98" s="217">
+        <f t="shared" si="22"/>
+        <v>744</v>
+      </c>
+      <c r="R98" s="212">
         <f t="shared" si="23"/>
-        <v>556000</v>
+        <v>141.71428571428572</v>
       </c>
       <c r="S98" s="212">
         <f t="shared" si="24"/>
-        <v>633041.09589041094</v>
+        <v>1147885.7142857143</v>
       </c>
       <c r="T98" s="212">
         <f t="shared" si="25"/>
-        <v>316520.54794520547</v>
-      </c>
-      <c r="U98" s="212">
+        <v>1046594.8219178081</v>
+      </c>
+      <c r="U98" s="219">
         <f t="shared" si="26"/>
-        <v>9.9409719832036877E-2</v>
-      </c>
-    </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.25">
+        <v>771250</v>
+      </c>
+      <c r="V98" s="219">
+        <f>V97+W98</f>
+        <v>-484528.52054794505</v>
+      </c>
+      <c r="W98" s="219">
+        <f t="shared" si="27"/>
+        <v>-275344.82191780815</v>
+      </c>
+      <c r="X98" s="217">
+        <f t="shared" si="28"/>
+        <v>556000</v>
+      </c>
+      <c r="Y98" s="212">
+        <f t="shared" si="29"/>
+        <v>490594.82191780815</v>
+      </c>
+      <c r="Z98" s="212">
+        <f t="shared" si="30"/>
+        <v>245297.41095890407</v>
+      </c>
+      <c r="AA98" s="212">
+        <f t="shared" si="31"/>
+        <v>0.10458637674896411</v>
+      </c>
+    </row>
+    <row r="99" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A99" s="184"/>
       <c r="B99" s="59" t="s">
         <v>46</v>
@@ -6405,11 +7480,11 @@
         <v>0</v>
       </c>
       <c r="I99" s="145">
+        <f t="shared" si="20"/>
+        <v>253</v>
+      </c>
+      <c r="J99" s="45">
         <f t="shared" si="21"/>
-        <v>253</v>
-      </c>
-      <c r="J99" s="45">
-        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="K99" s="46">
@@ -6435,28 +7510,52 @@
       <c r="P99">
         <v>31</v>
       </c>
-      <c r="Q99" s="212">
-        <f t="shared" si="20"/>
-        <v>1189041.0958904109</v>
-      </c>
-      <c r="R99" s="217">
+      <c r="Q99" s="217">
+        <f t="shared" si="22"/>
+        <v>744</v>
+      </c>
+      <c r="R99" s="212">
         <f t="shared" si="23"/>
-        <v>549000</v>
+        <v>141.71428571428572</v>
       </c>
       <c r="S99" s="212">
         <f t="shared" si="24"/>
-        <v>640041.09589041094</v>
+        <v>1147885.7142857143</v>
       </c>
       <c r="T99" s="212">
         <f t="shared" si="25"/>
-        <v>320020.54794520547</v>
-      </c>
-      <c r="U99" s="212">
+        <v>1046594.8219178081</v>
+      </c>
+      <c r="U99" s="219">
         <f t="shared" si="26"/>
-        <v>0.10050896606319266</v>
-      </c>
-    </row>
-    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
+        <v>985650</v>
+      </c>
+      <c r="V99" s="219">
+        <f t="shared" ref="V99:V107" si="32">V98+W99</f>
+        <v>-545473.3424657532</v>
+      </c>
+      <c r="W99" s="219">
+        <f t="shared" si="27"/>
+        <v>-60944.821917808149</v>
+      </c>
+      <c r="X99" s="217">
+        <f t="shared" si="28"/>
+        <v>549000</v>
+      </c>
+      <c r="Y99" s="212">
+        <f t="shared" si="29"/>
+        <v>497594.82191780815</v>
+      </c>
+      <c r="Z99" s="212">
+        <f t="shared" si="30"/>
+        <v>248797.41095890407</v>
+      </c>
+      <c r="AA99" s="212">
+        <f t="shared" si="31"/>
+        <v>0.10607865633393984</v>
+      </c>
+    </row>
+    <row r="100" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A100" s="184"/>
       <c r="B100" s="59" t="s">
         <v>47</v>
@@ -6480,11 +7579,11 @@
         <v>0</v>
       </c>
       <c r="I100" s="145">
+        <f t="shared" si="20"/>
+        <v>473</v>
+      </c>
+      <c r="J100" s="45">
         <f t="shared" si="21"/>
-        <v>473</v>
-      </c>
-      <c r="J100" s="45">
-        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="K100" s="46">
@@ -6510,28 +7609,52 @@
       <c r="P100">
         <v>30</v>
       </c>
-      <c r="Q100" s="212">
-        <f t="shared" si="20"/>
-        <v>1150684.9315068494</v>
-      </c>
-      <c r="R100" s="217">
+      <c r="Q100" s="217">
+        <f t="shared" si="22"/>
+        <v>720</v>
+      </c>
+      <c r="R100" s="212">
         <f t="shared" si="23"/>
-        <v>719000</v>
+        <v>137.14285714285714</v>
       </c>
       <c r="S100" s="212">
         <f t="shared" si="24"/>
-        <v>431684.93150684936</v>
+        <v>1110857.1428571427</v>
       </c>
       <c r="T100" s="212">
         <f t="shared" si="25"/>
-        <v>215842.46575342468</v>
-      </c>
-      <c r="U100" s="212">
+        <v>1012833.6986301369</v>
+      </c>
+      <c r="U100" s="219">
         <f t="shared" si="26"/>
-        <v>6.7789719143663524E-2</v>
-      </c>
-    </row>
-    <row r="101" spans="1:21" x14ac:dyDescent="0.25">
+        <v>1149090.0000000002</v>
+      </c>
+      <c r="V100" s="219">
+        <f t="shared" si="32"/>
+        <v>-409217.04109588987</v>
+      </c>
+      <c r="W100" s="219">
+        <f t="shared" si="27"/>
+        <v>136256.30136986333</v>
+      </c>
+      <c r="X100" s="217">
+        <f t="shared" si="28"/>
+        <v>719000</v>
+      </c>
+      <c r="Y100" s="212">
+        <f t="shared" si="29"/>
+        <v>293833.6986301369</v>
+      </c>
+      <c r="Z100" s="212">
+        <f t="shared" si="30"/>
+        <v>146916.84931506845</v>
+      </c>
+      <c r="AA100" s="212">
+        <f t="shared" si="31"/>
+        <v>6.2640289977666339E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A101" s="184"/>
       <c r="B101" s="59" t="s">
         <v>48</v>
@@ -6555,11 +7678,11 @@
         <v>0</v>
       </c>
       <c r="I101" s="145">
+        <f t="shared" si="20"/>
+        <v>204</v>
+      </c>
+      <c r="J101" s="45">
         <f t="shared" si="21"/>
-        <v>204</v>
-      </c>
-      <c r="J101" s="45">
-        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="K101" s="46">
@@ -6585,28 +7708,52 @@
       <c r="P101">
         <v>31</v>
       </c>
-      <c r="Q101" s="212">
-        <f t="shared" si="20"/>
-        <v>1189041.0958904109</v>
-      </c>
-      <c r="R101" s="217">
+      <c r="Q101" s="217">
+        <f t="shared" si="22"/>
+        <v>744</v>
+      </c>
+      <c r="R101" s="212">
         <f t="shared" si="23"/>
-        <v>858000</v>
+        <v>141.71428571428572</v>
       </c>
       <c r="S101" s="212">
         <f t="shared" si="24"/>
-        <v>331041.09589041094</v>
+        <v>1147885.7142857143</v>
       </c>
       <c r="T101" s="212">
         <f t="shared" si="25"/>
-        <v>165520.54794520547</v>
-      </c>
-      <c r="U101" s="212">
+        <v>1046594.8219178081</v>
+      </c>
+      <c r="U101" s="219">
         <f t="shared" si="26"/>
-        <v>5.1985096716458998E-2</v>
-      </c>
-    </row>
-    <row r="102" spans="1:21" x14ac:dyDescent="0.25">
+        <v>1284400</v>
+      </c>
+      <c r="V101" s="219">
+        <f t="shared" si="32"/>
+        <v>-171411.86301369802</v>
+      </c>
+      <c r="W101" s="219">
+        <f t="shared" si="27"/>
+        <v>237805.17808219185</v>
+      </c>
+      <c r="X101" s="217">
+        <f t="shared" si="28"/>
+        <v>858000</v>
+      </c>
+      <c r="Y101" s="212">
+        <f t="shared" si="29"/>
+        <v>188594.82191780815</v>
+      </c>
+      <c r="Z101" s="212">
+        <f t="shared" si="30"/>
+        <v>94297.410958904075</v>
+      </c>
+      <c r="AA101" s="212">
+        <f t="shared" si="31"/>
+        <v>4.0205171797154056E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A102" s="184"/>
       <c r="B102" s="59" t="s">
         <v>49</v>
@@ -6630,11 +7777,11 @@
         <v>0</v>
       </c>
       <c r="I102" s="145">
+        <f t="shared" si="20"/>
+        <v>345</v>
+      </c>
+      <c r="J102" s="45">
         <f t="shared" si="21"/>
-        <v>345</v>
-      </c>
-      <c r="J102" s="45">
-        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="K102" s="46">
@@ -6660,28 +7807,52 @@
       <c r="P102">
         <v>30</v>
       </c>
-      <c r="Q102" s="212">
-        <f t="shared" si="20"/>
-        <v>1150684.9315068494</v>
-      </c>
-      <c r="R102" s="217">
+      <c r="Q102" s="217">
+        <f t="shared" si="22"/>
+        <v>720</v>
+      </c>
+      <c r="R102" s="212">
         <f t="shared" si="23"/>
-        <v>784000</v>
+        <v>137.14285714285714</v>
       </c>
       <c r="S102" s="212">
         <f t="shared" si="24"/>
-        <v>366684.93150684936</v>
+        <v>1110857.1428571427</v>
       </c>
       <c r="T102" s="212">
         <f t="shared" si="25"/>
-        <v>183342.46575342468</v>
-      </c>
-      <c r="U102" s="212">
+        <v>1012833.6986301369</v>
+      </c>
+      <c r="U102" s="219">
         <f t="shared" si="26"/>
-        <v>5.7582432711502721E-2</v>
-      </c>
-    </row>
-    <row r="103" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>1194000</v>
+      </c>
+      <c r="V102" s="219">
+        <f t="shared" si="32"/>
+        <v>9754.4383561650757</v>
+      </c>
+      <c r="W102" s="219">
+        <f t="shared" si="27"/>
+        <v>181166.3013698631</v>
+      </c>
+      <c r="X102" s="217">
+        <f t="shared" si="28"/>
+        <v>784000</v>
+      </c>
+      <c r="Y102" s="212">
+        <f t="shared" si="29"/>
+        <v>228833.6986301369</v>
+      </c>
+      <c r="Z102" s="212">
+        <f t="shared" si="30"/>
+        <v>114416.84931506845</v>
+      </c>
+      <c r="AA102" s="212">
+        <f t="shared" si="31"/>
+        <v>4.8783408117177414E-2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="184"/>
       <c r="B103" s="58" t="s">
         <v>50</v>
@@ -6705,11 +7876,11 @@
         <v>0</v>
       </c>
       <c r="I103" s="145">
+        <f t="shared" si="20"/>
+        <v>370</v>
+      </c>
+      <c r="J103" s="49">
         <f t="shared" si="21"/>
-        <v>370</v>
-      </c>
-      <c r="J103" s="49">
-        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="K103" s="50">
@@ -6735,28 +7906,52 @@
       <c r="P103">
         <v>31</v>
       </c>
-      <c r="Q103" s="212">
-        <f t="shared" si="20"/>
-        <v>1189041.0958904109</v>
-      </c>
-      <c r="R103" s="217">
+      <c r="Q103" s="217">
+        <f t="shared" si="22"/>
+        <v>744</v>
+      </c>
+      <c r="R103" s="212">
         <f t="shared" si="23"/>
-        <v>985000</v>
+        <v>141.71428571428572</v>
       </c>
       <c r="S103" s="212">
         <f t="shared" si="24"/>
-        <v>204041.09589041094</v>
+        <v>1147885.7142857143</v>
       </c>
       <c r="T103" s="212">
         <f t="shared" si="25"/>
-        <v>102020.54794520547</v>
-      </c>
-      <c r="U103" s="212">
+        <v>1046594.8219178081</v>
+      </c>
+      <c r="U103" s="219">
         <f t="shared" si="26"/>
-        <v>3.2041629379775581E-2</v>
-      </c>
-    </row>
-    <row r="104" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>1376550</v>
+      </c>
+      <c r="V103" s="219">
+        <f>V102+W103</f>
+        <v>339709.61643835693</v>
+      </c>
+      <c r="W103" s="219">
+        <f t="shared" si="27"/>
+        <v>329955.17808219185</v>
+      </c>
+      <c r="X103" s="217">
+        <f t="shared" si="28"/>
+        <v>985000</v>
+      </c>
+      <c r="Y103" s="212">
+        <f t="shared" si="29"/>
+        <v>61594.821917808149</v>
+      </c>
+      <c r="Z103" s="212">
+        <f t="shared" si="30"/>
+        <v>30797.410958904075</v>
+      </c>
+      <c r="AA103" s="212">
+        <f t="shared" si="31"/>
+        <v>1.3130956469737247E-2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:27" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="184"/>
       <c r="B104" s="99" t="s">
         <v>190</v>
@@ -6780,16 +7975,28 @@
       <c r="M104" s="46"/>
       <c r="N104" s="46"/>
       <c r="O104" s="46"/>
-      <c r="R104" s="218"/>
-      <c r="T104" s="212">
-        <f>SUM(T92:T103)</f>
-        <v>3184000.0000000005</v>
-      </c>
-    </row>
-    <row r="105" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U104" s="219">
+        <f>SUM(U92:U103)</f>
+        <v>12322810</v>
+      </c>
+      <c r="V104" s="219">
+        <f>V103+W92</f>
+        <v>321024.79452054866</v>
+      </c>
+      <c r="X104" s="218"/>
+      <c r="Z104" s="212">
+        <f>SUM(Z92:Z103)</f>
+        <v>2345404.9999999991</v>
+      </c>
+    </row>
+    <row r="105" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A105" s="184"/>
-    </row>
-    <row r="106" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V105" s="219">
+        <f t="shared" ref="V105:V108" si="33">V104+W93</f>
+        <v>338213.34246575425</v>
+      </c>
+    </row>
+    <row r="106" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="184"/>
       <c r="B106" s="21" t="s">
         <v>33</v>
@@ -6812,8 +8019,12 @@
       <c r="I106" s="70" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="107" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V106" s="219">
+        <f t="shared" si="33"/>
+        <v>228028.5205479461</v>
+      </c>
+    </row>
+    <row r="107" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A107" s="184"/>
       <c r="B107" s="65" t="s">
         <v>52</v>
@@ -6839,8 +8050,12 @@
       <c r="I107" s="71">
         <v>0.48</v>
       </c>
-    </row>
-    <row r="108" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V107" s="219">
+        <f t="shared" si="33"/>
+        <v>-121255.1780821908</v>
+      </c>
+    </row>
+    <row r="108" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A108" s="184"/>
       <c r="B108" s="41" t="s">
         <v>54</v>
@@ -6866,8 +8081,12 @@
       <c r="I108" s="72">
         <v>0.52</v>
       </c>
-    </row>
-    <row r="109" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V108" s="219">
+        <f>V107+W96</f>
+        <v>1.0477378964424133E-9</v>
+      </c>
+    </row>
+    <row r="109" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="184"/>
       <c r="B109" s="42" t="s">
         <v>55</v>
@@ -6894,7 +8113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A110" s="184"/>
       <c r="B110" s="57"/>
       <c r="C110" s="44"/>
@@ -6905,7 +8124,7 @@
       <c r="H110" s="80"/>
       <c r="I110" s="79"/>
     </row>
-    <row r="111" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="184"/>
       <c r="B111" s="82" t="s">
         <v>121</v>
@@ -6918,7 +8137,7 @@
       <c r="H111" s="80"/>
       <c r="I111" s="79"/>
     </row>
-    <row r="112" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A112" s="184"/>
       <c r="B112" s="83" t="s">
         <v>122</v>
@@ -7358,7 +8577,7 @@
         <v>30</v>
       </c>
       <c r="F136" s="11">
-        <f t="shared" ref="F136:F140" si="27">D136/E136 * 60</f>
+        <f t="shared" ref="F136:F140" si="34">D136/E136 * 60</f>
         <v>6.8</v>
       </c>
     </row>
@@ -7377,7 +8596,7 @@
         <v>30</v>
       </c>
       <c r="F137" s="11">
-        <f t="shared" si="27"/>
+        <f t="shared" si="34"/>
         <v>6.8</v>
       </c>
     </row>
@@ -7396,7 +8615,7 @@
         <v>30</v>
       </c>
       <c r="F138" s="11">
-        <f t="shared" si="27"/>
+        <f t="shared" si="34"/>
         <v>6.8</v>
       </c>
     </row>
@@ -7415,7 +8634,7 @@
         <v>30</v>
       </c>
       <c r="F139" s="11">
-        <f t="shared" si="27"/>
+        <f t="shared" si="34"/>
         <v>6.8</v>
       </c>
     </row>
@@ -7434,7 +8653,7 @@
         <v>50</v>
       </c>
       <c r="F140" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" si="34"/>
         <v>10.799999999999999</v>
       </c>
     </row>
@@ -7490,14 +8709,14 @@
         <v>28.5</v>
       </c>
     </row>
-    <row r="145" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A145" s="185"/>
       <c r="B145" s="41"/>
       <c r="C145" s="29" t="s">
         <v>28</v>
       </c>
       <c r="D145" s="29">
-        <f t="shared" ref="D145:D149" si="28">E145*F145/60</f>
+        <f t="shared" ref="D145:D149" si="35">E145*F145/60</f>
         <v>15.25</v>
       </c>
       <c r="E145" s="9">
@@ -7507,14 +8726,14 @@
         <v>30.5</v>
       </c>
     </row>
-    <row r="146" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A146" s="185"/>
       <c r="B146" s="41"/>
       <c r="C146" s="29" t="s">
         <v>29</v>
       </c>
       <c r="D146" s="29">
-        <f t="shared" si="28"/>
+        <f t="shared" si="35"/>
         <v>13.25</v>
       </c>
       <c r="E146" s="9">
@@ -7524,7 +8743,7 @@
         <v>26.5</v>
       </c>
     </row>
-    <row r="147" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A147" s="185"/>
       <c r="B147" s="8" t="s">
         <v>31</v>
@@ -7533,7 +8752,7 @@
         <v>32</v>
       </c>
       <c r="D147" s="29">
-        <f t="shared" si="28"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="E147" s="9">
@@ -7543,14 +8762,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A148" s="185"/>
       <c r="B148" s="41"/>
       <c r="C148" s="29" t="s">
         <v>28</v>
       </c>
       <c r="D148" s="29">
-        <f t="shared" si="28"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="E148" s="9">
@@ -7560,14 +8779,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="185"/>
       <c r="B149" s="42"/>
       <c r="C149" s="193" t="s">
         <v>29</v>
       </c>
       <c r="D149" s="193">
-        <f t="shared" si="28"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="E149" s="14">
@@ -7577,7 +8796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A150" s="185"/>
       <c r="B150" s="37"/>
       <c r="C150" s="37"/>
@@ -7585,16 +8804,16 @@
       <c r="E150" s="194"/>
       <c r="F150" s="195"/>
     </row>
-    <row r="151" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="185"/>
       <c r="B151" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="R151">
+      <c r="X151">
         <v>16000000</v>
       </c>
     </row>
-    <row r="152" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A152" s="185"/>
       <c r="B152" s="43"/>
       <c r="C152" s="54"/>
@@ -7615,7 +8834,7 @@
       <c r="N152" s="34"/>
       <c r="O152" s="35"/>
     </row>
-    <row r="153" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="185"/>
       <c r="B153" s="39"/>
       <c r="C153" s="56" t="s">
@@ -7658,7 +8877,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="154" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A154" s="185"/>
       <c r="B154" s="61" t="s">
         <v>38</v>
@@ -7671,19 +8890,19 @@
         <v>0</v>
       </c>
       <c r="E154" s="144">
-        <f t="shared" ref="E154:H154" si="29">SUM(E156:E167)</f>
+        <f t="shared" ref="E154:H154" si="36">SUM(E156:E167)</f>
         <v>469</v>
       </c>
       <c r="F154" s="144">
-        <f t="shared" si="29"/>
+        <f t="shared" si="36"/>
         <v>1526</v>
       </c>
       <c r="G154" s="144">
-        <f t="shared" si="29"/>
+        <f t="shared" si="36"/>
         <v>2589</v>
       </c>
       <c r="H154" s="144">
-        <f t="shared" si="29"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="I154" s="145">
@@ -7695,19 +8914,19 @@
         <v>0</v>
       </c>
       <c r="K154" s="46">
-        <f t="shared" ref="K154:N154" si="30">E154/$I$154</f>
+        <f t="shared" ref="K154:N154" si="37">E154/$I$154</f>
         <v>0.10231239092495636</v>
       </c>
       <c r="L154" s="46">
-        <f t="shared" si="30"/>
+        <f t="shared" si="37"/>
         <v>0.33289703315881325</v>
       </c>
       <c r="M154" s="46">
-        <f t="shared" si="30"/>
+        <f t="shared" si="37"/>
         <v>0.56479057591623039</v>
       </c>
       <c r="N154" s="46">
-        <f t="shared" si="30"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="O154" s="47">
@@ -7715,7 +8934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A155" s="185"/>
       <c r="B155" s="36" t="s">
         <v>39</v>
@@ -7734,7 +8953,7 @@
       <c r="N155" s="37"/>
       <c r="O155" s="38"/>
     </row>
-    <row r="156" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A156" s="185"/>
       <c r="B156" s="59" t="s">
         <v>40</v>
@@ -7766,27 +8985,27 @@
         <v>0</v>
       </c>
       <c r="K156" s="46">
-        <f t="shared" ref="K156:O167" si="31">IF(E$154&gt;0,E156/E$154,0)</f>
+        <f t="shared" ref="K156:O167" si="38">IF(E$154&gt;0,E156/E$154,0)</f>
         <v>0</v>
       </c>
       <c r="L156" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0.11336828309305373</v>
       </c>
       <c r="M156" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0.16222479721900349</v>
       </c>
       <c r="N156" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="O156" s="48">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0.12936300174520071</v>
       </c>
     </row>
-    <row r="157" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A157" s="185"/>
       <c r="B157" s="59" t="s">
         <v>41</v>
@@ -7810,35 +9029,35 @@
         <v>0</v>
       </c>
       <c r="I157" s="145">
-        <f t="shared" ref="I157:I167" si="32">SUM(D157:H157)</f>
+        <f t="shared" ref="I157:I167" si="39">SUM(D157:H157)</f>
         <v>168</v>
       </c>
       <c r="J157" s="45">
-        <f t="shared" ref="J157:J167" si="33">IF(D$154&gt;0,D157/D$154,0)</f>
+        <f t="shared" ref="J157:J167" si="40">IF(D$154&gt;0,D157/D$154,0)</f>
         <v>0</v>
       </c>
       <c r="K157" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="L157" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>3.1454783748361727E-2</v>
       </c>
       <c r="M157" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>4.6349942062572425E-2</v>
       </c>
       <c r="N157" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="O157" s="48">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>3.6649214659685861E-2</v>
       </c>
     </row>
-    <row r="158" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A158" s="185"/>
       <c r="B158" s="59" t="s">
         <v>42</v>
@@ -7862,35 +9081,35 @@
         <v>0</v>
       </c>
       <c r="I158" s="145">
-        <f t="shared" si="32"/>
+        <f t="shared" si="39"/>
         <v>174</v>
       </c>
       <c r="J158" s="45">
-        <f t="shared" si="33"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="K158" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>2.1321961620469083E-3</v>
       </c>
       <c r="L158" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="M158" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>6.6821166473541901E-2</v>
       </c>
       <c r="N158" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="O158" s="48">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>3.7958115183246072E-2</v>
       </c>
     </row>
-    <row r="159" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A159" s="185"/>
       <c r="B159" s="59" t="s">
         <v>43</v>
@@ -7914,35 +9133,35 @@
         <v>0</v>
       </c>
       <c r="I159" s="145">
-        <f t="shared" si="32"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="J159" s="45">
-        <f t="shared" si="33"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="K159" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="L159" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="M159" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="N159" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="O159" s="48">
-        <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="160" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A160" s="185"/>
       <c r="B160" s="59" t="s">
         <v>17</v>
@@ -7966,35 +9185,35 @@
         <v>0</v>
       </c>
       <c r="I160" s="145">
-        <f t="shared" si="32"/>
+        <f t="shared" si="39"/>
         <v>501</v>
       </c>
       <c r="J160" s="45">
-        <f t="shared" si="33"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="K160" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>6.8230277185501065E-2</v>
       </c>
       <c r="L160" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>9.8296199213630409E-3</v>
       </c>
       <c r="M160" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0.17535728080339899</v>
       </c>
       <c r="N160" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="O160" s="48">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0.10929319371727748</v>
       </c>
     </row>
-    <row r="161" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A161" s="185"/>
       <c r="B161" s="59" t="s">
         <v>44</v>
@@ -8018,35 +9237,35 @@
         <v>0</v>
       </c>
       <c r="I161" s="145">
-        <f t="shared" si="32"/>
+        <f t="shared" si="39"/>
         <v>408</v>
       </c>
       <c r="J161" s="45">
-        <f t="shared" si="33"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="K161" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>2.1321961620469083E-3</v>
       </c>
       <c r="L161" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>5.8977719528178242E-2</v>
       </c>
       <c r="M161" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0.12244109694862881</v>
       </c>
       <c r="N161" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="O161" s="48">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>8.9005235602094238E-2</v>
       </c>
     </row>
-    <row r="162" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A162" s="185"/>
       <c r="B162" s="59" t="s">
         <v>45</v>
@@ -8070,35 +9289,35 @@
         <v>0</v>
       </c>
       <c r="I162" s="145">
-        <f t="shared" si="32"/>
+        <f t="shared" si="39"/>
         <v>490</v>
       </c>
       <c r="J162" s="45">
-        <f t="shared" si="33"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="K162" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>5.3304904051172705E-2</v>
       </c>
       <c r="L162" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0.10091743119266056</v>
       </c>
       <c r="M162" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0.1201235998455002</v>
       </c>
       <c r="N162" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="O162" s="48">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0.10689354275741711</v>
       </c>
     </row>
-    <row r="163" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A163" s="185"/>
       <c r="B163" s="59" t="s">
         <v>46</v>
@@ -8122,35 +9341,35 @@
         <v>0</v>
       </c>
       <c r="I163" s="145">
-        <f t="shared" si="32"/>
+        <f t="shared" si="39"/>
         <v>296</v>
       </c>
       <c r="J163" s="45">
-        <f t="shared" si="33"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="K163" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0.22601279317697229</v>
       </c>
       <c r="L163" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>9.1743119266055051E-3</v>
       </c>
       <c r="M163" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>6.7979915025106225E-2</v>
       </c>
       <c r="N163" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="O163" s="48">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>6.4572425828970326E-2</v>
       </c>
     </row>
-    <row r="164" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A164" s="185"/>
       <c r="B164" s="59" t="s">
         <v>47</v>
@@ -8174,35 +9393,35 @@
         <v>0</v>
       </c>
       <c r="I164" s="145">
-        <f t="shared" si="32"/>
+        <f t="shared" si="39"/>
         <v>246</v>
       </c>
       <c r="J164" s="45">
-        <f t="shared" si="33"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="K164" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>3.4115138592750532E-2</v>
       </c>
       <c r="L164" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0.15072083879423329</v>
       </c>
       <c r="M164" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="N164" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="O164" s="48">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>5.3664921465968587E-2</v>
       </c>
     </row>
-    <row r="165" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A165" s="185"/>
       <c r="B165" s="59" t="s">
         <v>48</v>
@@ -8226,35 +9445,35 @@
         <v>0</v>
       </c>
       <c r="I165" s="145">
-        <f t="shared" si="32"/>
+        <f t="shared" si="39"/>
         <v>654</v>
       </c>
       <c r="J165" s="45">
-        <f t="shared" si="33"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="K165" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0.15991471215351813</v>
       </c>
       <c r="L165" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0.30013106159895153</v>
       </c>
       <c r="M165" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>4.6736191579760528E-2</v>
       </c>
       <c r="N165" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="O165" s="48">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0.14267015706806283</v>
       </c>
     </row>
-    <row r="166" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A166" s="185"/>
       <c r="B166" s="59" t="s">
         <v>49</v>
@@ -8278,35 +9497,35 @@
         <v>0</v>
       </c>
       <c r="I166" s="145">
-        <f t="shared" si="32"/>
+        <f t="shared" si="39"/>
         <v>439</v>
       </c>
       <c r="J166" s="45">
-        <f t="shared" si="33"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="K166" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>2.5586353944562899E-2</v>
       </c>
       <c r="L166" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>5.3079947575360421E-2</v>
       </c>
       <c r="M166" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0.1336423329470838</v>
       </c>
       <c r="N166" s="46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="O166" s="48">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>9.5767888307155324E-2</v>
       </c>
     </row>
-    <row r="167" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="185"/>
       <c r="B167" s="58" t="s">
         <v>50</v>
@@ -8330,35 +9549,35 @@
         <v>0</v>
       </c>
       <c r="I167" s="145">
-        <f t="shared" si="32"/>
+        <f t="shared" si="39"/>
         <v>615</v>
       </c>
       <c r="J167" s="49">
-        <f t="shared" si="33"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="K167" s="50">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0.42857142857142855</v>
       </c>
       <c r="L167" s="50">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0.17234600262123198</v>
       </c>
       <c r="M167" s="50">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>5.8323677095403634E-2</v>
       </c>
       <c r="N167" s="50">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="O167" s="51">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0.13416230366492146</v>
       </c>
     </row>
-    <row r="168" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:23" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="185"/>
       <c r="B168" s="99" t="s">
         <v>190</v>
@@ -8383,10 +9602,10 @@
       <c r="N168" s="46"/>
       <c r="O168" s="46"/>
     </row>
-    <row r="169" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A169" s="185"/>
     </row>
-    <row r="170" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="185"/>
       <c r="B170" s="21" t="s">
         <v>33</v>
@@ -8395,7 +9614,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="171" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A171" s="185"/>
       <c r="B171" s="65" t="s">
         <v>52</v>
@@ -8422,7 +9641,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="172" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A172" s="185"/>
       <c r="B172" s="41" t="s">
         <v>54</v>
@@ -8448,9 +9667,12 @@
       <c r="I172" s="72">
         <v>0.52</v>
       </c>
-      <c r="Q172" s="171"/>
-    </row>
-    <row r="173" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T172" s="171"/>
+      <c r="U172" s="171"/>
+      <c r="V172" s="171"/>
+      <c r="W172" s="171"/>
+    </row>
+    <row r="173" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="185"/>
       <c r="B173" s="42" t="s">
         <v>55</v>
@@ -8477,7 +9699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A174" s="185"/>
       <c r="B174" s="57"/>
       <c r="C174" s="44"/>
@@ -8488,7 +9710,7 @@
       <c r="H174" s="80"/>
       <c r="I174" s="79"/>
     </row>
-    <row r="175" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="185"/>
       <c r="B175" s="82" t="s">
         <v>121</v>
@@ -8501,7 +9723,7 @@
       <c r="H175" s="80"/>
       <c r="I175" s="79"/>
     </row>
-    <row r="176" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A176" s="185"/>
       <c r="B176" s="83" t="s">
         <v>122</v>
@@ -8775,7 +9997,7 @@
         <v>210</v>
       </c>
       <c r="P187">
-        <f t="shared" ref="P187" si="34">O187/N187</f>
+        <f t="shared" ref="P187" si="41">O187/N187</f>
         <v>2157.0066030814378</v>
       </c>
     </row>
@@ -8860,7 +10082,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="193" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A193" s="185"/>
       <c r="B193" s="65" t="s">
         <v>117</v>
@@ -8870,7 +10092,7 @@
       </c>
       <c r="D193" s="149"/>
     </row>
-    <row r="194" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A194" s="185"/>
       <c r="B194" s="42" t="s">
         <v>116</v>
@@ -8880,7 +10102,7 @@
       </c>
       <c r="D194" s="162"/>
     </row>
-    <row r="196" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B196" s="26" t="s">
         <v>7</v>
       </c>
@@ -8900,7 +10122,7 @@
       <c r="N196" s="26"/>
       <c r="O196" s="26"/>
     </row>
-    <row r="197" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B197" s="17"/>
       <c r="C197" s="1"/>
       <c r="D197" s="2" t="s">
@@ -8913,7 +10135,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="198" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B198" s="12"/>
       <c r="C198" s="18"/>
       <c r="D198" s="19" t="s">
@@ -8926,7 +10148,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="199" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B199" s="4" t="s">
         <v>14</v>
       </c>
@@ -8944,7 +10166,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="200" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B200" s="8" t="s">
         <v>14</v>
       </c>
@@ -8958,7 +10180,7 @@
         <v>30</v>
       </c>
       <c r="F200" s="11">
-        <f t="shared" ref="F200:F204" si="35">D200/E200 * 60</f>
+        <f t="shared" ref="F200:F204" si="42">D200/E200 * 60</f>
         <v>0.4</v>
       </c>
       <c r="K200">
@@ -8979,26 +10201,26 @@
       <c r="P200">
         <v>0.41</v>
       </c>
-      <c r="Q200">
-        <v>0.41</v>
-      </c>
-      <c r="R200">
-        <v>0.41</v>
-      </c>
-      <c r="S200">
-        <v>0.41</v>
-      </c>
       <c r="T200">
         <v>0.41</v>
       </c>
-      <c r="U200">
+      <c r="X200">
         <v>0.41</v>
       </c>
-      <c r="V200">
+      <c r="Y200">
         <v>0.41</v>
       </c>
-    </row>
-    <row r="201" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Z200">
+        <v>0.41</v>
+      </c>
+      <c r="AA200">
+        <v>0.41</v>
+      </c>
+      <c r="AB200">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="201" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B201" s="8" t="s">
         <v>15</v>
       </c>
@@ -9012,7 +10234,7 @@
         <v>30</v>
       </c>
       <c r="F201" s="11">
-        <f t="shared" si="35"/>
+        <f t="shared" si="42"/>
         <v>0.4</v>
       </c>
       <c r="K201">
@@ -9033,26 +10255,26 @@
       <c r="P201">
         <v>0.41</v>
       </c>
-      <c r="Q201">
-        <v>0.41</v>
-      </c>
-      <c r="R201">
-        <v>0.41</v>
-      </c>
-      <c r="S201">
-        <v>0.41</v>
-      </c>
       <c r="T201">
         <v>0.41</v>
       </c>
-      <c r="U201">
+      <c r="X201">
         <v>0.41</v>
       </c>
-      <c r="V201">
+      <c r="Y201">
         <v>0.41</v>
       </c>
-    </row>
-    <row r="202" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Z201">
+        <v>0.41</v>
+      </c>
+      <c r="AA201">
+        <v>0.41</v>
+      </c>
+      <c r="AB201">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="202" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B202" s="8" t="s">
         <v>15</v>
       </c>
@@ -9066,7 +10288,7 @@
         <v>30</v>
       </c>
       <c r="F202" s="11">
-        <f t="shared" si="35"/>
+        <f t="shared" si="42"/>
         <v>0.4</v>
       </c>
       <c r="K202">
@@ -9087,26 +10309,26 @@
       <c r="P202">
         <v>0.41</v>
       </c>
-      <c r="Q202">
-        <v>0.41</v>
-      </c>
-      <c r="R202">
-        <v>0.41</v>
-      </c>
-      <c r="S202">
-        <v>0.41</v>
-      </c>
       <c r="T202">
         <v>0.41</v>
       </c>
-      <c r="U202">
+      <c r="X202">
         <v>0.41</v>
       </c>
-      <c r="V202">
+      <c r="Y202">
         <v>0.41</v>
       </c>
-    </row>
-    <row r="203" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Z202">
+        <v>0.41</v>
+      </c>
+      <c r="AA202">
+        <v>0.41</v>
+      </c>
+      <c r="AB202">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="203" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B203" s="8" t="s">
         <v>16</v>
       </c>
@@ -9120,11 +10342,11 @@
         <v>30</v>
       </c>
       <c r="F203" s="11">
-        <f t="shared" si="35"/>
+        <f t="shared" si="42"/>
         <v>0.4</v>
       </c>
     </row>
-    <row r="204" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B204" s="13" t="s">
         <v>16</v>
       </c>
@@ -9138,16 +10360,16 @@
         <v>50</v>
       </c>
       <c r="F204" s="16">
-        <f t="shared" si="35"/>
+        <f t="shared" si="42"/>
         <v>1.2</v>
       </c>
     </row>
-    <row r="206" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B206" s="21" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="207" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B207" s="43"/>
       <c r="C207" s="54"/>
       <c r="D207" s="43" t="s">
@@ -9167,7 +10389,7 @@
       <c r="N207" s="34"/>
       <c r="O207" s="35"/>
     </row>
-    <row r="208" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B208" s="39"/>
       <c r="C208" s="56" t="s">
         <v>53</v>
@@ -9209,7 +10431,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="209" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B209" s="61" t="s">
         <v>38</v>
       </c>
@@ -9221,19 +10443,19 @@
         <v>0</v>
       </c>
       <c r="E209" s="175">
-        <f t="shared" ref="E209:H209" si="36">SUM(E211:E222)</f>
+        <f t="shared" ref="E209:H209" si="43">SUM(E211:E222)</f>
         <v>142.26999999999998</v>
       </c>
       <c r="F209" s="175">
-        <f t="shared" si="36"/>
+        <f t="shared" si="43"/>
         <v>1232.05</v>
       </c>
       <c r="G209" s="175">
-        <f t="shared" si="36"/>
+        <f t="shared" si="43"/>
         <v>3316.4900000000002</v>
       </c>
       <c r="H209" s="175">
-        <f t="shared" si="36"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="I209" s="179">
@@ -9245,19 +10467,19 @@
         <v>0</v>
       </c>
       <c r="K209" s="46">
-        <f t="shared" ref="K209:N209" si="37">E209/$I$209</f>
+        <f t="shared" ref="K209:N209" si="44">E209/$I$209</f>
         <v>3.0329516650642419E-2</v>
       </c>
       <c r="L209" s="46">
-        <f t="shared" si="37"/>
+        <f t="shared" si="44"/>
         <v>0.26265186609562097</v>
       </c>
       <c r="M209" s="46">
-        <f t="shared" si="37"/>
+        <f t="shared" si="44"/>
         <v>0.7070186172537366</v>
       </c>
       <c r="N209" s="46">
-        <f t="shared" si="37"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="O209" s="47">
@@ -9265,7 +10487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B210" s="36" t="s">
         <v>39</v>
       </c>
@@ -9283,7 +10505,7 @@
       <c r="N210" s="37"/>
       <c r="O210" s="38"/>
     </row>
-    <row r="211" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B211" s="59" t="s">
         <v>40</v>
       </c>
@@ -9314,19 +10536,19 @@
         <v>0</v>
       </c>
       <c r="K211" s="46">
-        <f t="shared" ref="K211:O222" si="38">IF(E$209&gt;0,E211/E$209,0)</f>
+        <f t="shared" ref="K211:O222" si="45">IF(E$209&gt;0,E211/E$209,0)</f>
         <v>0</v>
       </c>
       <c r="L211" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>2.329450915141431E-2</v>
       </c>
       <c r="M211" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>0.10891333910248484</v>
       </c>
       <c r="N211" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="O211" s="48">
@@ -9334,7 +10556,7 @@
         <v>8.3122104711126632E-2</v>
       </c>
     </row>
-    <row r="212" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B212" s="59" t="s">
         <v>41</v>
       </c>
@@ -9357,35 +10579,35 @@
         <v>0</v>
       </c>
       <c r="I212" s="180">
-        <f t="shared" ref="I212:I222" si="39">SUM(D212:H212)</f>
+        <f t="shared" ref="I212:I222" si="46">SUM(D212:H212)</f>
         <v>389.49999999999994</v>
       </c>
       <c r="J212" s="45">
-        <f t="shared" ref="J212:J222" si="40">IF(D$209&gt;0,D212/D$209,0)</f>
+        <f t="shared" ref="J212:J222" si="47">IF(D$209&gt;0,D212/D$209,0)</f>
         <v>0</v>
       </c>
       <c r="K212" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>0.21613832853025935</v>
       </c>
       <c r="L212" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>5.6572379367720471E-2</v>
       </c>
       <c r="M212" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>8.7155396217084916E-2</v>
       </c>
       <c r="N212" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="O212" s="48">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>8.3034699764006625E-2</v>
       </c>
     </row>
-    <row r="213" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="213" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B213" s="59" t="s">
         <v>42</v>
       </c>
@@ -9408,35 +10630,35 @@
         <v>0</v>
       </c>
       <c r="I213" s="180">
-        <f t="shared" si="39"/>
+        <f t="shared" si="46"/>
         <v>410.40999999999997</v>
       </c>
       <c r="J213" s="45">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="K213" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>0.26224783861671469</v>
       </c>
       <c r="L213" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>9.9833610648918464E-2</v>
       </c>
       <c r="M213" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>7.5411052045988372E-2</v>
       </c>
       <c r="N213" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="O213" s="48">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>8.749235206712698E-2</v>
       </c>
     </row>
-    <row r="214" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B214" s="59" t="s">
         <v>43</v>
       </c>
@@ -9459,35 +10681,35 @@
         <v>0</v>
       </c>
       <c r="I214" s="180">
-        <f t="shared" si="39"/>
+        <f t="shared" si="46"/>
         <v>391.55</v>
       </c>
       <c r="J214" s="45">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="K214" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="L214" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>5.9900166389351084E-2</v>
       </c>
       <c r="M214" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>9.5809123501050808E-2</v>
       </c>
       <c r="N214" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="O214" s="48">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>8.3471724499606673E-2</v>
       </c>
     </row>
-    <row r="215" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B215" s="59" t="s">
         <v>17</v>
       </c>
@@ -9510,35 +10732,35 @@
         <v>0</v>
       </c>
       <c r="I215" s="180">
-        <f t="shared" si="39"/>
+        <f t="shared" si="46"/>
         <v>403.85</v>
       </c>
       <c r="J215" s="45">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="K215" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="L215" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>7.8202995008319467E-2</v>
       </c>
       <c r="M215" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>9.2718506613920129E-2</v>
       </c>
       <c r="N215" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="O215" s="48">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>8.6093872913206887E-2</v>
       </c>
     </row>
-    <row r="216" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B216" s="59" t="s">
         <v>44</v>
       </c>
@@ -9561,38 +10783,38 @@
         <v>0</v>
       </c>
       <c r="I216" s="180">
-        <f t="shared" si="39"/>
+        <f t="shared" si="46"/>
         <v>395.65</v>
       </c>
       <c r="J216" s="45">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="K216" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>2.0172910662824207E-2</v>
       </c>
       <c r="L216" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>0.11813643926788685</v>
       </c>
       <c r="M216" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>7.454567931759179E-2</v>
       </c>
       <c r="N216" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="O216" s="48">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>8.4345773970806739E-2</v>
       </c>
-      <c r="Q216" t="s">
+      <c r="T216" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="217" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="217" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B217" s="59" t="s">
         <v>45</v>
       </c>
@@ -9615,35 +10837,35 @@
         <v>0</v>
       </c>
       <c r="I217" s="180">
-        <f t="shared" si="39"/>
+        <f t="shared" si="46"/>
         <v>215.25</v>
       </c>
       <c r="J217" s="45">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="K217" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="L217" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>7.4875207986688855E-2</v>
       </c>
       <c r="M217" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>3.7087402645568049E-2</v>
       </c>
       <c r="N217" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="O217" s="48">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>4.5887597238003668E-2</v>
       </c>
     </row>
-    <row r="218" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="218" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B218" s="59" t="s">
         <v>46</v>
       </c>
@@ -9666,35 +10888,35 @@
         <v>0</v>
       </c>
       <c r="I218" s="180">
-        <f t="shared" si="39"/>
+        <f t="shared" si="46"/>
         <v>436.65</v>
       </c>
       <c r="J218" s="45">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="K218" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>8.645533141210375E-2</v>
       </c>
       <c r="L218" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>0.11148086522462562</v>
       </c>
       <c r="M218" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>8.6537272839658785E-2</v>
       </c>
       <c r="N218" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="O218" s="48">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>9.3086268682807435E-2</v>
       </c>
     </row>
-    <row r="219" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="219" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B219" s="59" t="s">
         <v>47</v>
       </c>
@@ -9717,35 +10939,35 @@
         <v>0</v>
       </c>
       <c r="I219" s="180">
-        <f t="shared" si="39"/>
+        <f t="shared" si="46"/>
         <v>430.09000000000003</v>
       </c>
       <c r="J219" s="45">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="K219" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>6.9164265129683003E-2</v>
       </c>
       <c r="L219" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>9.1514143094841932E-2</v>
       </c>
       <c r="M219" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>9.2718506613920129E-2</v>
       </c>
       <c r="N219" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="O219" s="48">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>9.1687789528887328E-2</v>
       </c>
     </row>
-    <row r="220" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="220" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B220" s="59" t="s">
         <v>48</v>
       </c>
@@ -9768,35 +10990,35 @@
         <v>0</v>
       </c>
       <c r="I220" s="180">
-        <f t="shared" si="39"/>
+        <f t="shared" si="46"/>
         <v>426.4</v>
       </c>
       <c r="J220" s="45">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="K220" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="L220" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>0.1098169717138103</v>
       </c>
       <c r="M220" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>8.7773519594511046E-2</v>
       </c>
       <c r="N220" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="O220" s="48">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>9.0901145004807254E-2</v>
       </c>
     </row>
-    <row r="221" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="221" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B221" s="59" t="s">
         <v>49</v>
       </c>
@@ -9819,35 +11041,35 @@
         <v>0</v>
       </c>
       <c r="I221" s="180">
-        <f t="shared" si="39"/>
+        <f t="shared" si="46"/>
         <v>410</v>
       </c>
       <c r="J221" s="45">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="K221" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>0.1729106628242075</v>
       </c>
       <c r="L221" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>7.9866888519134774E-2</v>
       </c>
       <c r="M221" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>8.6537272839658785E-2</v>
       </c>
       <c r="N221" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="O221" s="48">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>8.7404947120006987E-2</v>
       </c>
     </row>
-    <row r="222" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B222" s="58" t="s">
         <v>50</v>
       </c>
@@ -9870,35 +11092,35 @@
         <v>0</v>
       </c>
       <c r="I222" s="181">
-        <f t="shared" si="39"/>
+        <f t="shared" si="46"/>
         <v>391.54999999999995</v>
       </c>
       <c r="J222" s="49">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="K222" s="50">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>0.1729106628242075</v>
       </c>
       <c r="L222" s="50">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>9.6505823627287851E-2</v>
       </c>
       <c r="M222" s="50">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>7.4792928668562228E-2</v>
       </c>
       <c r="N222" s="50">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="O222" s="51">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>8.3471724499606659E-2</v>
       </c>
     </row>
-    <row r="223" spans="2:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="2:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B223" s="99" t="s">
         <v>190</v>
       </c>
@@ -10349,6 +11571,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -10357,7 +11580,7 @@
   <dimension ref="A1:N55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9:N23"/>
+      <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14287,7 +15510,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -14691,27 +15914,28 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G29"/>
+  <dimension ref="A2:I29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.7109375" customWidth="1"/>
     <col min="2" max="2" width="31.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
     <col min="5" max="5" width="8.140625" customWidth="1"/>
     <col min="6" max="6" width="26.140625" customWidth="1"/>
     <col min="7" max="7" width="58.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>250</v>
       </c>
@@ -14725,7 +15949,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="209">
         <v>0.24305555555555555</v>
       </c>
@@ -14748,7 +15972,7 @@
         <v>Day Shift Staff Arrive</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="209">
         <v>0.25</v>
       </c>
@@ -14756,7 +15980,7 @@
       <c r="F5" s="214"/>
       <c r="G5" s="215"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="211">
         <v>0.2638888888888889</v>
       </c>
@@ -14780,7 +16004,7 @@
         <v>Preshift Finishes, Excavator Product Begin, Trucks Cycles Begin</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="213">
         <v>0.41145833333333331</v>
       </c>
@@ -14803,8 +16027,12 @@
         <f t="shared" si="2"/>
         <v>Excavator Stops Loading Trucks, Truck Cycles Stop</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <f>C7+C11+C15</f>
+        <v>10.083333333333332</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="213">
         <v>0.41666666666666669</v>
       </c>
@@ -14832,7 +16060,7 @@
         <v>First Break Start</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="213">
         <v>0.4375</v>
       </c>
@@ -14856,7 +16084,7 @@
         <v>First break End</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="213">
         <v>0.44270833333333331</v>
       </c>
@@ -14880,7 +16108,7 @@
         <v>Excavator product begins, Trucks Cycles Begin</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="213">
         <v>0.578125</v>
       </c>
@@ -14904,7 +16132,7 @@
         <v>Excavator Stops Loading Trucks, Trucks Cycles Stop</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="213">
         <v>0.58333333333333337</v>
       </c>
@@ -14932,7 +16160,7 @@
         <v>Second Break Start</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="213">
         <v>0.60416666666666663</v>
       </c>
@@ -14956,7 +16184,7 @@
         <v>Second break End</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="213">
         <v>0.609375</v>
       </c>
@@ -14980,7 +16208,7 @@
         <v>Excavator product begins, Trucks Cycles Begin</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="213">
         <v>0.74652777777777779</v>
       </c>
@@ -15004,7 +16232,7 @@
         <v>Excavator Stops Loading Trucks, Trucks Cycles Stop</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="213">
         <v>0.75</v>
       </c>

</xml_diff>

<commit_message>
End of day Pre Experiment
</commit_message>
<xml_diff>
--- a/Rolleston Workzones_ps_140327.xlsx
+++ b/Rolleston Workzones_ps_140327.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="272">
   <si>
     <t>Work Zone</t>
   </si>
@@ -839,6 +839,9 @@
   </si>
   <si>
     <t>Cuml. Diff</t>
+  </si>
+  <si>
+    <t>Total Monthly Contents</t>
   </si>
 </sst>
 </file>
@@ -2026,11 +2029,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="293638616"/>
-        <c:axId val="293639792"/>
+        <c:axId val="703884224"/>
+        <c:axId val="703884616"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="293638616"/>
+        <c:axId val="703884224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2072,7 +2075,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="293639792"/>
+        <c:crossAx val="703884616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2080,7 +2083,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="293639792"/>
+        <c:axId val="703884616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2131,7 +2134,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="293638616"/>
+        <c:crossAx val="703884224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2409,8 +2412,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="293637048"/>
-        <c:axId val="293637832"/>
+        <c:axId val="703877560"/>
+        <c:axId val="703878736"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2627,11 +2630,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="293639008"/>
-        <c:axId val="293638224"/>
+        <c:axId val="632720672"/>
+        <c:axId val="703879520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="293637048"/>
+        <c:axId val="703877560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2674,7 +2677,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="293637832"/>
+        <c:crossAx val="703878736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2682,7 +2685,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="293637832"/>
+        <c:axId val="703878736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2733,12 +2736,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="293637048"/>
+        <c:crossAx val="703877560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="293638224"/>
+        <c:axId val="703879520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2775,12 +2778,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="293639008"/>
+        <c:crossAx val="632720672"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="293639008"/>
+        <c:axId val="632720672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2790,7 +2793,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="293638224"/>
+        <c:crossAx val="703879520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4301,8 +4304,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:AB249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L13" workbookViewId="0">
-      <selection activeCell="T28" sqref="T28:T39"/>
+    <sheetView tabSelected="1" topLeftCell="I13" workbookViewId="0">
+      <selection activeCell="V28" sqref="V28:V39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4747,6 +4750,9 @@
       <c r="M24" s="34"/>
       <c r="N24" s="34"/>
       <c r="O24" s="35"/>
+      <c r="V24" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="25" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="182"/>
@@ -4952,7 +4958,10 @@
         <v>6.9151989562948477E-2</v>
       </c>
       <c r="U28" s="217"/>
-      <c r="V28" s="217"/>
+      <c r="V28" s="217">
+        <f>Q28+Q156</f>
+        <v>1119000</v>
+      </c>
       <c r="W28" s="217"/>
       <c r="X28" s="212"/>
       <c r="Y28" s="212"/>
@@ -5028,7 +5037,10 @@
         <v>0.11274787997390737</v>
       </c>
       <c r="U29" s="217"/>
-      <c r="V29" s="217"/>
+      <c r="V29" s="217">
+        <f t="shared" ref="V29:V39" si="15">Q29+Q157</f>
+        <v>754000</v>
+      </c>
       <c r="W29" s="217"/>
       <c r="X29" s="212"/>
       <c r="Y29" s="212"/>
@@ -5104,7 +5116,10 @@
         <v>5.2882148293107202E-2</v>
       </c>
       <c r="U30" s="217"/>
-      <c r="V30" s="217"/>
+      <c r="V30" s="217">
+        <f t="shared" si="15"/>
+        <v>1089000</v>
+      </c>
       <c r="W30" s="217"/>
       <c r="X30" s="212"/>
       <c r="Y30" s="212"/>
@@ -5180,7 +5195,10 @@
         <v>7.3763318112633189E-2</v>
       </c>
       <c r="U31" s="217"/>
-      <c r="V31" s="217"/>
+      <c r="V31" s="217">
+        <f t="shared" si="15"/>
+        <v>703000</v>
+      </c>
       <c r="W31" s="217"/>
       <c r="X31" s="212"/>
       <c r="Y31" s="212"/>
@@ -5256,7 +5274,10 @@
         <v>0.10784246575342467</v>
       </c>
       <c r="U32" s="217"/>
-      <c r="V32" s="217"/>
+      <c r="V32" s="217">
+        <f t="shared" si="15"/>
+        <v>1050000</v>
+      </c>
       <c r="W32" s="217"/>
       <c r="X32" s="212"/>
       <c r="Y32" s="212"/>
@@ -5332,7 +5353,10 @@
         <v>5.3326810176125249E-2</v>
       </c>
       <c r="U33" s="217"/>
-      <c r="V33" s="217"/>
+      <c r="V33" s="217">
+        <f t="shared" si="15"/>
+        <v>942000</v>
+      </c>
       <c r="W33" s="217"/>
       <c r="X33" s="212"/>
       <c r="Y33" s="212"/>
@@ -5408,7 +5432,10 @@
         <v>0.1042710371819961</v>
       </c>
       <c r="U34" s="217"/>
-      <c r="V34" s="217"/>
+      <c r="V34" s="217">
+        <f t="shared" si="15"/>
+        <v>860000</v>
+      </c>
       <c r="W34" s="217"/>
       <c r="X34" s="212"/>
       <c r="Y34" s="212"/>
@@ -5484,7 +5511,10 @@
         <v>9.2366275277234192E-2</v>
       </c>
       <c r="U35" s="217"/>
-      <c r="V35" s="217"/>
+      <c r="V35" s="217">
+        <f t="shared" si="15"/>
+        <v>913000</v>
+      </c>
       <c r="W35" s="217"/>
       <c r="X35" s="212"/>
       <c r="Y35" s="212"/>
@@ -5560,7 +5590,10 @@
         <v>5.5707762557077628E-2</v>
       </c>
       <c r="U36" s="217"/>
-      <c r="V36" s="217"/>
+      <c r="V36" s="217">
+        <f t="shared" si="15"/>
+        <v>1241000</v>
+      </c>
       <c r="W36" s="217"/>
       <c r="X36" s="212"/>
       <c r="Y36" s="212"/>
@@ -5636,7 +5669,10 @@
         <v>0.10863611654707546</v>
       </c>
       <c r="U37" s="217"/>
-      <c r="V37" s="217"/>
+      <c r="V37" s="217">
+        <f t="shared" si="15"/>
+        <v>1140000</v>
+      </c>
       <c r="W37" s="217"/>
       <c r="X37" s="212"/>
       <c r="Y37" s="212"/>
@@ -5712,7 +5748,10 @@
         <v>5.9080778430093503E-2</v>
       </c>
       <c r="U38" s="217"/>
-      <c r="V38" s="217"/>
+      <c r="V38" s="217">
+        <f t="shared" si="15"/>
+        <v>1289000</v>
+      </c>
       <c r="W38" s="217"/>
       <c r="X38" s="212"/>
       <c r="Y38" s="212"/>
@@ -5788,7 +5827,10 @@
         <v>0.11022341813437704</v>
       </c>
       <c r="U39" s="217"/>
-      <c r="V39" s="217"/>
+      <c r="V39" s="217">
+        <f t="shared" si="15"/>
+        <v>1259000</v>
+      </c>
       <c r="W39" s="217"/>
       <c r="X39" s="212"/>
       <c r="Y39" s="212"/>
@@ -6421,7 +6463,7 @@
         <v>30</v>
       </c>
       <c r="F72" s="11">
-        <f t="shared" ref="F72:F76" si="15">D72/E72 * 60</f>
+        <f t="shared" ref="F72:F76" si="16">D72/E72 * 60</f>
         <v>5.2</v>
       </c>
     </row>
@@ -6440,7 +6482,7 @@
         <v>30</v>
       </c>
       <c r="F73" s="11">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>5.2</v>
       </c>
     </row>
@@ -6459,7 +6501,7 @@
         <v>30</v>
       </c>
       <c r="F74" s="11">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>5.2</v>
       </c>
     </row>
@@ -6478,7 +6520,7 @@
         <v>30</v>
       </c>
       <c r="F75" s="11">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>5.2</v>
       </c>
     </row>
@@ -6497,7 +6539,7 @@
         <v>50</v>
       </c>
       <c r="F76" s="16">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>3</v>
       </c>
     </row>
@@ -6560,7 +6602,7 @@
         <v>28</v>
       </c>
       <c r="D81" s="29">
-        <f t="shared" ref="D81:D85" si="16">E81*F81/60</f>
+        <f t="shared" ref="D81:D85" si="17">E81*F81/60</f>
         <v>10</v>
       </c>
       <c r="E81" s="9">
@@ -6577,7 +6619,7 @@
         <v>29</v>
       </c>
       <c r="D82" s="29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
       <c r="E82" s="9">
@@ -6596,7 +6638,7 @@
         <v>32</v>
       </c>
       <c r="D83" s="29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="E83" s="9">
@@ -6613,7 +6655,7 @@
         <v>28</v>
       </c>
       <c r="D84" s="29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="E84" s="9">
@@ -6630,7 +6672,7 @@
         <v>29</v>
       </c>
       <c r="D85" s="193">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="E85" s="14">
@@ -6734,19 +6776,19 @@
         <v>0</v>
       </c>
       <c r="E90" s="144">
-        <f t="shared" ref="E90:H90" si="17">SUM(E92:E103)</f>
+        <f t="shared" ref="E90:H90" si="18">SUM(E92:E103)</f>
         <v>8</v>
       </c>
       <c r="F90" s="144">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>409</v>
       </c>
       <c r="G90" s="144">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2631</v>
       </c>
       <c r="H90" s="144">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="I90" s="145">
@@ -6758,19 +6800,19 @@
         <v>0</v>
       </c>
       <c r="K90" s="46">
-        <f t="shared" ref="K90:N90" si="18">E90/$I$90</f>
+        <f t="shared" ref="K90:N90" si="19">E90/$I$90</f>
         <v>2.6246719160104987E-3</v>
       </c>
       <c r="L90" s="46">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.13418635170603674</v>
       </c>
       <c r="M90" s="46">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.86318897637795278</v>
       </c>
       <c r="N90" s="46">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="O90" s="47">
@@ -6855,19 +6897,19 @@
         <v>0</v>
       </c>
       <c r="K92" s="46">
-        <f t="shared" ref="K92:O103" si="19">IF(E$90&gt;0,E92/E$90,0)</f>
+        <f t="shared" ref="K92:O103" si="20">IF(E$90&gt;0,E92/E$90,0)</f>
         <v>0</v>
       </c>
       <c r="L92" s="46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.1100244498777506</v>
       </c>
       <c r="M92" s="46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="N92" s="46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="O92" s="48">
@@ -6943,75 +6985,75 @@
         <v>0</v>
       </c>
       <c r="I93" s="145">
-        <f t="shared" ref="I93:I103" si="20">SUM(D93:H93)</f>
+        <f t="shared" ref="I93:I103" si="21">SUM(D93:H93)</f>
         <v>405</v>
       </c>
       <c r="J93" s="45">
-        <f t="shared" ref="J93:J103" si="21">IF(D$90&gt;0,D93/D$90,0)</f>
+        <f t="shared" ref="J93:J103" si="22">IF(D$90&gt;0,D93/D$90,0)</f>
         <v>0</v>
       </c>
       <c r="K93" s="46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="L93" s="46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.28117359413202936</v>
       </c>
       <c r="M93" s="46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.10718358038768529</v>
       </c>
       <c r="N93" s="46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="O93" s="48">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.13287401574803151</v>
       </c>
       <c r="P93">
         <v>28</v>
       </c>
       <c r="Q93" s="217">
-        <f t="shared" ref="Q93:Q103" si="22">P93*24</f>
+        <f t="shared" ref="Q93:Q103" si="23">P93*24</f>
         <v>672</v>
       </c>
       <c r="R93" s="212">
-        <f t="shared" ref="R93:R103" si="23">Q93/$R$89</f>
+        <f t="shared" ref="R93:R103" si="24">Q93/$R$89</f>
         <v>128</v>
       </c>
       <c r="S93" s="212">
-        <f t="shared" ref="S93:S103" si="24">R93*8100</f>
+        <f t="shared" ref="S93:S103" si="25">R93*8100</f>
         <v>1036800</v>
       </c>
       <c r="T93" s="212">
-        <f t="shared" ref="T93:T103" si="25">($U$104/365)*P93</f>
+        <f t="shared" ref="T93:T103" si="26">($U$104/365)*P93</f>
         <v>945311.45205479441</v>
       </c>
       <c r="U93" s="219">
-        <f t="shared" ref="U93:U103" si="26">(I93+I157+I212)*1000</f>
+        <f t="shared" ref="U93:U103" si="27">(I93+I157+I212)*1000</f>
         <v>962500</v>
       </c>
       <c r="V93" s="219"/>
       <c r="W93" s="219">
-        <f t="shared" ref="W93:W103" si="27">U93-T93</f>
+        <f t="shared" ref="W93:W103" si="28">U93-T93</f>
         <v>17188.547945205588</v>
       </c>
       <c r="X93" s="217">
-        <f t="shared" ref="X93:X103" si="28">(I93+I157)*1000</f>
+        <f t="shared" ref="X93:X103" si="29">(I93+I157)*1000</f>
         <v>573000</v>
       </c>
       <c r="Y93" s="212">
-        <f t="shared" ref="Y93:Y103" si="29">T93-X93</f>
+        <f t="shared" ref="Y93:Y103" si="30">T93-X93</f>
         <v>372311.45205479441</v>
       </c>
       <c r="Z93" s="212">
-        <f t="shared" ref="Z93:Z103" si="30">Y93/2</f>
+        <f t="shared" ref="Z93:Z103" si="31">Y93/2</f>
         <v>186155.72602739721</v>
       </c>
       <c r="AA93" s="212">
-        <f t="shared" ref="AA93:AA103" si="31">Z93/$Z$104</f>
+        <f t="shared" ref="AA93:AA103" si="32">Z93/$Z$104</f>
         <v>7.9370397022005698E-2</v>
       </c>
     </row>
@@ -7039,19 +7081,19 @@
         <v>0</v>
       </c>
       <c r="I94" s="145">
+        <f t="shared" si="21"/>
+        <v>352</v>
+      </c>
+      <c r="J94" s="45">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="K94" s="46">
         <f t="shared" si="20"/>
-        <v>352</v>
-      </c>
-      <c r="J94" s="45">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="K94" s="46">
-        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="L94" s="46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="M94" s="46">
@@ -7059,7 +7101,7 @@
         <v>0.1337894336754086</v>
       </c>
       <c r="N94" s="46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="O94" s="48">
@@ -7070,44 +7112,44 @@
         <v>31</v>
       </c>
       <c r="Q94" s="217">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>744</v>
       </c>
       <c r="R94" s="212">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>141.71428571428572</v>
       </c>
       <c r="S94" s="212">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1147885.7142857143</v>
       </c>
       <c r="T94" s="212">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1046594.8219178081</v>
       </c>
       <c r="U94" s="219">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>936410</v>
       </c>
       <c r="V94" s="219"/>
       <c r="W94" s="219">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>-110184.82191780815</v>
       </c>
       <c r="X94" s="217">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>526000</v>
       </c>
       <c r="Y94" s="212">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>520594.82191780815</v>
       </c>
       <c r="Z94" s="212">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>260297.41095890407</v>
       </c>
       <c r="AA94" s="212">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.11098186068457438</v>
       </c>
     </row>
@@ -7135,75 +7177,75 @@
         <v>0</v>
       </c>
       <c r="I95" s="145">
+        <f t="shared" si="21"/>
+        <v>272</v>
+      </c>
+      <c r="J95" s="45">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="K95" s="46">
         <f t="shared" si="20"/>
-        <v>272</v>
-      </c>
-      <c r="J95" s="45">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="K95" s="46">
-        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="L95" s="46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="M95" s="46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.10338274420372481</v>
       </c>
       <c r="N95" s="46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="O95" s="48">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>8.9238845144356954E-2</v>
       </c>
       <c r="P95">
         <v>30</v>
       </c>
       <c r="Q95" s="217">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>720</v>
       </c>
       <c r="R95" s="212">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>137.14285714285714</v>
       </c>
       <c r="S95" s="212">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1110857.1428571427</v>
       </c>
       <c r="T95" s="212">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1012833.6986301369</v>
       </c>
       <c r="U95" s="219">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>663550</v>
       </c>
       <c r="V95" s="219"/>
       <c r="W95" s="219">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>-349283.6986301369</v>
       </c>
       <c r="X95" s="217">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>272000</v>
       </c>
       <c r="Y95" s="212">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>740833.6986301369</v>
       </c>
       <c r="Z95" s="212">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>370416.84931506845</v>
       </c>
       <c r="AA95" s="212">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.15793300061825935</v>
       </c>
     </row>
@@ -7231,75 +7273,75 @@
         <v>0</v>
       </c>
       <c r="I96" s="145">
+        <f t="shared" si="21"/>
+        <v>263</v>
+      </c>
+      <c r="J96" s="45">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="K96" s="46">
         <f t="shared" si="20"/>
-        <v>263</v>
-      </c>
-      <c r="J96" s="45">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="K96" s="46">
-        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="L96" s="46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="M96" s="46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>9.99619916381604E-2</v>
       </c>
       <c r="N96" s="46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="O96" s="48">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>8.6286089238845148E-2</v>
       </c>
       <c r="P96">
         <v>31</v>
       </c>
       <c r="Q96" s="217">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>744</v>
       </c>
       <c r="R96" s="212">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>141.71428571428572</v>
       </c>
       <c r="S96" s="212">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1147885.7142857143</v>
       </c>
       <c r="T96" s="212">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1046594.8219178081</v>
       </c>
       <c r="U96" s="219">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>1167850</v>
       </c>
       <c r="V96" s="219"/>
       <c r="W96" s="219">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>121255.17808219185</v>
       </c>
       <c r="X96" s="217">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>764000</v>
       </c>
       <c r="Y96" s="212">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>282594.82191780815</v>
       </c>
       <c r="Z96" s="212">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>141297.41095890407</v>
       </c>
       <c r="AA96" s="212">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>6.0244354795399573E-2</v>
       </c>
     </row>
@@ -7327,54 +7369,54 @@
         <v>0</v>
       </c>
       <c r="I97" s="145">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="J97" s="45">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="K97" s="46">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="J97" s="45">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="K97" s="46">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
       <c r="L97" s="46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="M97" s="46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="N97" s="46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="O97" s="48">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="P97">
         <v>30</v>
       </c>
       <c r="Q97" s="217">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>720</v>
       </c>
       <c r="R97" s="212">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>137.14285714285714</v>
       </c>
       <c r="S97" s="212">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1110857.1428571427</v>
       </c>
       <c r="T97" s="212">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1012833.6986301369</v>
       </c>
       <c r="U97" s="219">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>803650</v>
       </c>
       <c r="V97" s="219">
@@ -7382,23 +7424,23 @@
         <v>-209183.6986301369</v>
       </c>
       <c r="W97" s="219">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>-209183.6986301369</v>
       </c>
       <c r="X97" s="217">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>408000</v>
       </c>
       <c r="Y97" s="212">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>604833.6986301369</v>
       </c>
       <c r="Z97" s="212">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>302416.84931506845</v>
       </c>
       <c r="AA97" s="212">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.12894014011015947</v>
       </c>
     </row>
@@ -7426,54 +7468,54 @@
         <v>0</v>
       </c>
       <c r="I98" s="145">
+        <f t="shared" si="21"/>
+        <v>66</v>
+      </c>
+      <c r="J98" s="45">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="K98" s="46">
         <f t="shared" si="20"/>
-        <v>66</v>
-      </c>
-      <c r="J98" s="45">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="K98" s="46">
-        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="L98" s="46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="M98" s="46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>2.5085518814139111E-2</v>
       </c>
       <c r="N98" s="46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="O98" s="48">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>2.1653543307086614E-2</v>
       </c>
       <c r="P98">
         <v>31</v>
       </c>
       <c r="Q98" s="217">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>744</v>
       </c>
       <c r="R98" s="212">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>141.71428571428572</v>
       </c>
       <c r="S98" s="212">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1147885.7142857143</v>
       </c>
       <c r="T98" s="212">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1046594.8219178081</v>
       </c>
       <c r="U98" s="219">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>771250</v>
       </c>
       <c r="V98" s="219">
@@ -7481,23 +7523,23 @@
         <v>-484528.52054794505</v>
       </c>
       <c r="W98" s="219">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>-275344.82191780815</v>
       </c>
       <c r="X98" s="217">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>556000</v>
       </c>
       <c r="Y98" s="212">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>490594.82191780815</v>
       </c>
       <c r="Z98" s="212">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>245297.41095890407</v>
       </c>
       <c r="AA98" s="212">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.10458637674896411</v>
       </c>
     </row>
@@ -7525,78 +7567,78 @@
         <v>0</v>
       </c>
       <c r="I99" s="145">
+        <f t="shared" si="21"/>
+        <v>253</v>
+      </c>
+      <c r="J99" s="45">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="K99" s="46">
         <f t="shared" si="20"/>
-        <v>253</v>
-      </c>
-      <c r="J99" s="45">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="K99" s="46">
-        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="L99" s="46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="M99" s="46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>9.6161155454199926E-2</v>
       </c>
       <c r="N99" s="46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="O99" s="48">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>8.3005249343832022E-2</v>
       </c>
       <c r="P99">
         <v>31</v>
       </c>
       <c r="Q99" s="217">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>744</v>
       </c>
       <c r="R99" s="212">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>141.71428571428572</v>
       </c>
       <c r="S99" s="212">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1147885.7142857143</v>
       </c>
       <c r="T99" s="212">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1046594.8219178081</v>
       </c>
       <c r="U99" s="219">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>985650</v>
       </c>
       <c r="V99" s="219">
-        <f t="shared" ref="V99:V102" si="32">V98+W99</f>
+        <f t="shared" ref="V99:V102" si="33">V98+W99</f>
         <v>-545473.3424657532</v>
       </c>
       <c r="W99" s="219">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>-60944.821917808149</v>
       </c>
       <c r="X99" s="217">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>549000</v>
       </c>
       <c r="Y99" s="212">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>497594.82191780815</v>
       </c>
       <c r="Z99" s="212">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>248797.41095890407</v>
       </c>
       <c r="AA99" s="212">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.10607865633393984</v>
       </c>
     </row>
@@ -7624,78 +7666,78 @@
         <v>0</v>
       </c>
       <c r="I100" s="145">
+        <f t="shared" si="21"/>
+        <v>473</v>
+      </c>
+      <c r="J100" s="45">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="K100" s="46">
         <f t="shared" si="20"/>
-        <v>473</v>
-      </c>
-      <c r="J100" s="45">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="K100" s="46">
-        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="L100" s="46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.44254278728606355</v>
       </c>
       <c r="M100" s="46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.11098441657164576</v>
       </c>
       <c r="N100" s="46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="O100" s="48">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.15518372703412073</v>
       </c>
       <c r="P100">
         <v>30</v>
       </c>
       <c r="Q100" s="217">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>720</v>
       </c>
       <c r="R100" s="212">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>137.14285714285714</v>
       </c>
       <c r="S100" s="212">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1110857.1428571427</v>
       </c>
       <c r="T100" s="212">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1012833.6986301369</v>
       </c>
       <c r="U100" s="219">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>1149090.0000000002</v>
       </c>
       <c r="V100" s="219">
+        <f t="shared" si="33"/>
+        <v>-409217.04109588987</v>
+      </c>
+      <c r="W100" s="219">
+        <f t="shared" si="28"/>
+        <v>136256.30136986333</v>
+      </c>
+      <c r="X100" s="217">
+        <f t="shared" si="29"/>
+        <v>719000</v>
+      </c>
+      <c r="Y100" s="212">
+        <f t="shared" si="30"/>
+        <v>293833.6986301369</v>
+      </c>
+      <c r="Z100" s="212">
+        <f t="shared" si="31"/>
+        <v>146916.84931506845</v>
+      </c>
+      <c r="AA100" s="212">
         <f t="shared" si="32"/>
-        <v>-409217.04109588987</v>
-      </c>
-      <c r="W100" s="219">
-        <f t="shared" si="27"/>
-        <v>136256.30136986333</v>
-      </c>
-      <c r="X100" s="217">
-        <f t="shared" si="28"/>
-        <v>719000</v>
-      </c>
-      <c r="Y100" s="212">
-        <f t="shared" si="29"/>
-        <v>293833.6986301369</v>
-      </c>
-      <c r="Z100" s="212">
-        <f t="shared" si="30"/>
-        <v>146916.84931506845</v>
-      </c>
-      <c r="AA100" s="212">
-        <f t="shared" si="31"/>
         <v>6.2640289977666339E-2</v>
       </c>
     </row>
@@ -7723,78 +7765,78 @@
         <v>0</v>
       </c>
       <c r="I101" s="145">
+        <f t="shared" si="21"/>
+        <v>204</v>
+      </c>
+      <c r="J101" s="45">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="K101" s="46">
         <f t="shared" si="20"/>
-        <v>204</v>
-      </c>
-      <c r="J101" s="45">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="K101" s="46">
-        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="L101" s="46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="M101" s="46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>7.7537058152793617E-2</v>
       </c>
       <c r="N101" s="46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="O101" s="48">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>6.6929133858267723E-2</v>
       </c>
       <c r="P101">
         <v>31</v>
       </c>
       <c r="Q101" s="217">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>744</v>
       </c>
       <c r="R101" s="212">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>141.71428571428572</v>
       </c>
       <c r="S101" s="212">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1147885.7142857143</v>
       </c>
       <c r="T101" s="212">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1046594.8219178081</v>
       </c>
       <c r="U101" s="219">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>1284400</v>
       </c>
       <c r="V101" s="219">
+        <f t="shared" si="33"/>
+        <v>-171411.86301369802</v>
+      </c>
+      <c r="W101" s="219">
+        <f t="shared" si="28"/>
+        <v>237805.17808219185</v>
+      </c>
+      <c r="X101" s="217">
+        <f t="shared" si="29"/>
+        <v>858000</v>
+      </c>
+      <c r="Y101" s="212">
+        <f t="shared" si="30"/>
+        <v>188594.82191780815</v>
+      </c>
+      <c r="Z101" s="212">
+        <f t="shared" si="31"/>
+        <v>94297.410958904075</v>
+      </c>
+      <c r="AA101" s="212">
         <f t="shared" si="32"/>
-        <v>-171411.86301369802</v>
-      </c>
-      <c r="W101" s="219">
-        <f t="shared" si="27"/>
-        <v>237805.17808219185</v>
-      </c>
-      <c r="X101" s="217">
-        <f t="shared" si="28"/>
-        <v>858000</v>
-      </c>
-      <c r="Y101" s="212">
-        <f t="shared" si="29"/>
-        <v>188594.82191780815</v>
-      </c>
-      <c r="Z101" s="212">
-        <f t="shared" si="30"/>
-        <v>94297.410958904075</v>
-      </c>
-      <c r="AA101" s="212">
-        <f t="shared" si="31"/>
         <v>4.0205171797154056E-2</v>
       </c>
     </row>
@@ -7822,78 +7864,78 @@
         <v>0</v>
       </c>
       <c r="I102" s="145">
+        <f t="shared" si="21"/>
+        <v>345</v>
+      </c>
+      <c r="J102" s="45">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="K102" s="46">
         <f t="shared" si="20"/>
-        <v>345</v>
-      </c>
-      <c r="J102" s="45">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="K102" s="46">
-        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="L102" s="46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.1100244498777506</v>
       </c>
       <c r="M102" s="46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.11402508551881414</v>
       </c>
       <c r="N102" s="46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="O102" s="48">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.11318897637795275</v>
       </c>
       <c r="P102">
         <v>30</v>
       </c>
       <c r="Q102" s="217">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>720</v>
       </c>
       <c r="R102" s="212">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>137.14285714285714</v>
       </c>
       <c r="S102" s="212">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1110857.1428571427</v>
       </c>
       <c r="T102" s="212">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1012833.6986301369</v>
       </c>
       <c r="U102" s="219">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>1194000</v>
       </c>
       <c r="V102" s="219">
+        <f t="shared" si="33"/>
+        <v>9754.4383561650757</v>
+      </c>
+      <c r="W102" s="219">
+        <f t="shared" si="28"/>
+        <v>181166.3013698631</v>
+      </c>
+      <c r="X102" s="217">
+        <f t="shared" si="29"/>
+        <v>784000</v>
+      </c>
+      <c r="Y102" s="212">
+        <f t="shared" si="30"/>
+        <v>228833.6986301369</v>
+      </c>
+      <c r="Z102" s="212">
+        <f t="shared" si="31"/>
+        <v>114416.84931506845</v>
+      </c>
+      <c r="AA102" s="212">
         <f t="shared" si="32"/>
-        <v>9754.4383561650757</v>
-      </c>
-      <c r="W102" s="219">
-        <f t="shared" si="27"/>
-        <v>181166.3013698631</v>
-      </c>
-      <c r="X102" s="217">
-        <f t="shared" si="28"/>
-        <v>784000</v>
-      </c>
-      <c r="Y102" s="212">
-        <f t="shared" si="29"/>
-        <v>228833.6986301369</v>
-      </c>
-      <c r="Z102" s="212">
-        <f t="shared" si="30"/>
-        <v>114416.84931506845</v>
-      </c>
-      <c r="AA102" s="212">
-        <f t="shared" si="31"/>
         <v>4.8783408117177414E-2</v>
       </c>
     </row>
@@ -7921,54 +7963,54 @@
         <v>0</v>
       </c>
       <c r="I103" s="145">
+        <f t="shared" si="21"/>
+        <v>370</v>
+      </c>
+      <c r="J103" s="49">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="K103" s="50">
         <f t="shared" si="20"/>
-        <v>370</v>
-      </c>
-      <c r="J103" s="49">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="K103" s="50">
-        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="L103" s="50">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>5.623471882640587E-2</v>
       </c>
       <c r="M103" s="50">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.13188901558342836</v>
       </c>
       <c r="N103" s="50">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="O103" s="51">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.12139107611548557</v>
       </c>
       <c r="P103">
         <v>31</v>
       </c>
       <c r="Q103" s="217">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>744</v>
       </c>
       <c r="R103" s="212">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>141.71428571428572</v>
       </c>
       <c r="S103" s="212">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1147885.7142857143</v>
       </c>
       <c r="T103" s="212">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1046594.8219178081</v>
       </c>
       <c r="U103" s="219">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>1376550</v>
       </c>
       <c r="V103" s="219">
@@ -7976,23 +8018,23 @@
         <v>339709.61643835693</v>
       </c>
       <c r="W103" s="219">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>329955.17808219185</v>
       </c>
       <c r="X103" s="217">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>985000</v>
       </c>
       <c r="Y103" s="212">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>61594.821917808149</v>
       </c>
       <c r="Z103" s="212">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>30797.410958904075</v>
       </c>
       <c r="AA103" s="212">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>1.3130956469737247E-2</v>
       </c>
     </row>
@@ -8037,7 +8079,7 @@
     <row r="105" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A105" s="184"/>
       <c r="V105" s="219">
-        <f t="shared" ref="V105:V107" si="33">V104+W93</f>
+        <f t="shared" ref="V105:V107" si="34">V104+W93</f>
         <v>338213.34246575425</v>
       </c>
     </row>
@@ -8065,7 +8107,7 @@
         <v>108</v>
       </c>
       <c r="V106" s="219">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>228028.5205479461</v>
       </c>
     </row>
@@ -8096,7 +8138,7 @@
         <v>0.48</v>
       </c>
       <c r="V107" s="219">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>-121255.1780821908</v>
       </c>
     </row>
@@ -8622,7 +8664,7 @@
         <v>30</v>
       </c>
       <c r="F136" s="11">
-        <f t="shared" ref="F136:F140" si="34">D136/E136 * 60</f>
+        <f t="shared" ref="F136:F140" si="35">D136/E136 * 60</f>
         <v>6.8</v>
       </c>
     </row>
@@ -8641,7 +8683,7 @@
         <v>30</v>
       </c>
       <c r="F137" s="11">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>6.8</v>
       </c>
     </row>
@@ -8660,7 +8702,7 @@
         <v>30</v>
       </c>
       <c r="F138" s="11">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>6.8</v>
       </c>
     </row>
@@ -8679,7 +8721,7 @@
         <v>30</v>
       </c>
       <c r="F139" s="11">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>6.8</v>
       </c>
     </row>
@@ -8698,7 +8740,7 @@
         <v>50</v>
       </c>
       <c r="F140" s="16">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>10.799999999999999</v>
       </c>
     </row>
@@ -8761,7 +8803,7 @@
         <v>28</v>
       </c>
       <c r="D145" s="29">
-        <f t="shared" ref="D145:D149" si="35">E145*F145/60</f>
+        <f t="shared" ref="D145:D149" si="36">E145*F145/60</f>
         <v>15.25</v>
       </c>
       <c r="E145" s="9">
@@ -8778,7 +8820,7 @@
         <v>29</v>
       </c>
       <c r="D146" s="29">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>13.25</v>
       </c>
       <c r="E146" s="9">
@@ -8797,7 +8839,7 @@
         <v>32</v>
       </c>
       <c r="D147" s="29">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="E147" s="9">
@@ -8814,7 +8856,7 @@
         <v>28</v>
       </c>
       <c r="D148" s="29">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="E148" s="9">
@@ -8831,7 +8873,7 @@
         <v>29</v>
       </c>
       <c r="D149" s="193">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="E149" s="14">
@@ -8953,19 +8995,19 @@
         <v>0</v>
       </c>
       <c r="E154" s="144">
-        <f t="shared" ref="E154:H154" si="36">SUM(E156:E167)</f>
+        <f t="shared" ref="E154:H154" si="37">SUM(E156:E167)</f>
         <v>469</v>
       </c>
       <c r="F154" s="144">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>1526</v>
       </c>
       <c r="G154" s="144">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>2589</v>
       </c>
       <c r="H154" s="144">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="I154" s="145">
@@ -8977,19 +9019,19 @@
         <v>0</v>
       </c>
       <c r="K154" s="46">
-        <f t="shared" ref="K154:N154" si="37">E154/$I$154</f>
+        <f t="shared" ref="K154:N154" si="38">E154/$I$154</f>
         <v>0.10231239092495636</v>
       </c>
       <c r="L154" s="46">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0.33289703315881325</v>
       </c>
       <c r="M154" s="46">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0.56479057591623039</v>
       </c>
       <c r="N154" s="46">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="O154" s="47">
@@ -9056,23 +9098,23 @@
         <v>0</v>
       </c>
       <c r="K156" s="46">
-        <f t="shared" ref="K156:O167" si="38">IF(E$154&gt;0,E156/E$154,0)</f>
+        <f t="shared" ref="K156:O167" si="39">IF(E$154&gt;0,E156/E$154,0)</f>
         <v>0</v>
       </c>
       <c r="L156" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0.11336828309305373</v>
       </c>
       <c r="M156" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0.16222479721900349</v>
       </c>
       <c r="N156" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="O156" s="48">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0.12936300174520071</v>
       </c>
       <c r="P156">
@@ -9123,54 +9165,54 @@
         <v>0</v>
       </c>
       <c r="I157" s="145">
-        <f t="shared" ref="I157:I167" si="39">SUM(D157:H157)</f>
+        <f t="shared" ref="I157:I167" si="40">SUM(D157:H157)</f>
         <v>168</v>
       </c>
       <c r="J157" s="45">
-        <f t="shared" ref="J157:J167" si="40">IF(D$154&gt;0,D157/D$154,0)</f>
+        <f t="shared" ref="J157:J167" si="41">IF(D$154&gt;0,D157/D$154,0)</f>
         <v>0</v>
       </c>
       <c r="K157" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="L157" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>3.1454783748361727E-2</v>
       </c>
       <c r="M157" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>4.6349942062572425E-2</v>
       </c>
       <c r="N157" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="O157" s="48">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>3.6649214659685861E-2</v>
       </c>
       <c r="P157">
         <v>28</v>
       </c>
       <c r="Q157" s="217">
-        <f t="shared" ref="Q157:Q167" si="41">(I157+I93)*1000</f>
+        <f t="shared" ref="Q157:Q167" si="42">(I157+I93)*1000</f>
         <v>573000</v>
       </c>
       <c r="S157">
-        <f t="shared" ref="S157:S167" si="42">($T$153/365)*P157</f>
+        <f t="shared" ref="S157:S167" si="43">($T$153/365)*P157</f>
         <v>843221.91780821909</v>
       </c>
       <c r="T157">
-        <f t="shared" ref="T157:T167" si="43">S157-Q157</f>
+        <f t="shared" ref="T157:T167" si="44">S157-Q157</f>
         <v>270221.91780821909</v>
       </c>
       <c r="U157">
-        <f t="shared" ref="U157:U167" si="44">T157/2</f>
+        <f t="shared" ref="U157:U166" si="45">T157/2</f>
         <v>135110.95890410955</v>
       </c>
       <c r="V157">
-        <f t="shared" ref="V157:V167" si="45">U157/$V$154</f>
+        <f t="shared" ref="V157:V167" si="46">U157/$V$154</f>
         <v>7.9210679961740235E-2</v>
       </c>
     </row>
@@ -9198,54 +9240,54 @@
         <v>0</v>
       </c>
       <c r="I158" s="145">
+        <f t="shared" si="40"/>
+        <v>174</v>
+      </c>
+      <c r="J158" s="45">
+        <f t="shared" si="41"/>
+        <v>0</v>
+      </c>
+      <c r="K158" s="46">
         <f t="shared" si="39"/>
-        <v>174</v>
-      </c>
-      <c r="J158" s="45">
-        <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="K158" s="46">
-        <f t="shared" si="38"/>
         <v>2.1321961620469083E-3</v>
       </c>
       <c r="L158" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="M158" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>6.6821166473541901E-2</v>
       </c>
       <c r="N158" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="O158" s="48">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>3.7958115183246072E-2</v>
       </c>
       <c r="P158">
         <v>31</v>
       </c>
       <c r="Q158" s="217">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>526000</v>
       </c>
       <c r="S158">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>933567.12328767125</v>
       </c>
       <c r="T158">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>407567.12328767125</v>
       </c>
       <c r="U158">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>203783.56164383562</v>
       </c>
       <c r="V158">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>0.11947094901672298</v>
       </c>
     </row>
@@ -9273,54 +9315,54 @@
         <v>0</v>
       </c>
       <c r="I159" s="145">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="J159" s="45">
+        <f t="shared" si="41"/>
+        <v>0</v>
+      </c>
+      <c r="K159" s="46">
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="J159" s="45">
-        <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="K159" s="46">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
       <c r="L159" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="M159" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="N159" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="O159" s="48">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="P159">
         <v>30</v>
       </c>
       <c r="Q159" s="217">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>272000</v>
       </c>
       <c r="S159">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>903452.05479452049</v>
       </c>
       <c r="T159">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>631452.05479452049</v>
       </c>
       <c r="U159">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>315726.02739726024</v>
       </c>
       <c r="V159">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>0.18509877743895828</v>
       </c>
     </row>
@@ -9348,54 +9390,54 @@
         <v>0</v>
       </c>
       <c r="I160" s="145">
+        <f t="shared" si="40"/>
+        <v>501</v>
+      </c>
+      <c r="J160" s="45">
+        <f t="shared" si="41"/>
+        <v>0</v>
+      </c>
+      <c r="K160" s="46">
         <f t="shared" si="39"/>
-        <v>501</v>
-      </c>
-      <c r="J160" s="45">
-        <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="K160" s="46">
-        <f t="shared" si="38"/>
         <v>6.8230277185501065E-2</v>
       </c>
       <c r="L160" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>9.8296199213630409E-3</v>
       </c>
       <c r="M160" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0.17535728080339899</v>
       </c>
       <c r="N160" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="O160" s="48">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0.10929319371727748</v>
       </c>
       <c r="P160">
         <v>31</v>
       </c>
       <c r="Q160" s="217">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>764000</v>
       </c>
       <c r="S160">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>933567.12328767125</v>
       </c>
       <c r="T160">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>169567.12328767125</v>
       </c>
       <c r="U160">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>84783.561643835623</v>
       </c>
       <c r="V160">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>4.9705542924557478E-2</v>
       </c>
     </row>
@@ -9423,54 +9465,54 @@
         <v>0</v>
       </c>
       <c r="I161" s="145">
+        <f t="shared" si="40"/>
+        <v>408</v>
+      </c>
+      <c r="J161" s="45">
+        <f t="shared" si="41"/>
+        <v>0</v>
+      </c>
+      <c r="K161" s="46">
         <f t="shared" si="39"/>
-        <v>408</v>
-      </c>
-      <c r="J161" s="45">
-        <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="K161" s="46">
-        <f t="shared" si="38"/>
         <v>2.1321961620469083E-3</v>
       </c>
       <c r="L161" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>5.8977719528178242E-2</v>
       </c>
       <c r="M161" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0.12244109694862881</v>
       </c>
       <c r="N161" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="O161" s="48">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>8.9005235602094238E-2</v>
       </c>
       <c r="P161">
         <v>30</v>
       </c>
       <c r="Q161" s="217">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>408000</v>
       </c>
       <c r="S161">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>903452.05479452049</v>
       </c>
       <c r="T161">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>495452.05479452049</v>
       </c>
       <c r="U161">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>247726.02739726024</v>
       </c>
       <c r="V161">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>0.14523283110057797</v>
       </c>
     </row>
@@ -9498,54 +9540,54 @@
         <v>0</v>
       </c>
       <c r="I162" s="145">
+        <f t="shared" si="40"/>
+        <v>490</v>
+      </c>
+      <c r="J162" s="45">
+        <f t="shared" si="41"/>
+        <v>0</v>
+      </c>
+      <c r="K162" s="46">
         <f t="shared" si="39"/>
-        <v>490</v>
-      </c>
-      <c r="J162" s="45">
-        <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="K162" s="46">
-        <f t="shared" si="38"/>
         <v>5.3304904051172705E-2</v>
       </c>
       <c r="L162" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0.10091743119266056</v>
       </c>
       <c r="M162" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0.1201235998455002</v>
       </c>
       <c r="N162" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="O162" s="48">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0.10689354275741711</v>
       </c>
       <c r="P162">
         <v>31</v>
       </c>
       <c r="Q162" s="217">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>556000</v>
       </c>
       <c r="S162">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>933567.12328767125</v>
       </c>
       <c r="T162">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>377567.12328767125</v>
       </c>
       <c r="U162">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>188783.56164383562</v>
       </c>
       <c r="V162">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>0.11067699026560968</v>
       </c>
     </row>
@@ -9573,54 +9615,54 @@
         <v>0</v>
       </c>
       <c r="I163" s="145">
+        <f t="shared" si="40"/>
+        <v>296</v>
+      </c>
+      <c r="J163" s="45">
+        <f t="shared" si="41"/>
+        <v>0</v>
+      </c>
+      <c r="K163" s="46">
         <f t="shared" si="39"/>
-        <v>296</v>
-      </c>
-      <c r="J163" s="45">
-        <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="K163" s="46">
-        <f t="shared" si="38"/>
         <v>0.22601279317697229</v>
       </c>
       <c r="L163" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>9.1743119266055051E-3</v>
       </c>
       <c r="M163" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>6.7979915025106225E-2</v>
       </c>
       <c r="N163" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="O163" s="48">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>6.4572425828970326E-2</v>
       </c>
       <c r="P163">
         <v>31</v>
       </c>
       <c r="Q163" s="217">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>549000</v>
       </c>
       <c r="S163">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>933567.12328767125</v>
       </c>
       <c r="T163">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>384567.12328767125</v>
       </c>
       <c r="U163">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>192283.56164383562</v>
       </c>
       <c r="V163">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>0.11272891397420279</v>
       </c>
     </row>
@@ -9648,54 +9690,54 @@
         <v>0</v>
       </c>
       <c r="I164" s="145">
+        <f t="shared" si="40"/>
+        <v>246</v>
+      </c>
+      <c r="J164" s="45">
+        <f t="shared" si="41"/>
+        <v>0</v>
+      </c>
+      <c r="K164" s="46">
         <f t="shared" si="39"/>
-        <v>246</v>
-      </c>
-      <c r="J164" s="45">
-        <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="K164" s="46">
-        <f t="shared" si="38"/>
         <v>3.4115138592750532E-2</v>
       </c>
       <c r="L164" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0.15072083879423329</v>
       </c>
       <c r="M164" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="N164" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="O164" s="48">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>5.3664921465968587E-2</v>
       </c>
       <c r="P164">
         <v>30</v>
       </c>
       <c r="Q164" s="217">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>719000</v>
       </c>
       <c r="S164">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>903452.05479452049</v>
       </c>
       <c r="T164">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>184452.05479452049</v>
       </c>
       <c r="U164">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>92226.027397260244</v>
       </c>
       <c r="V164">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>5.4068792047370105E-2</v>
       </c>
     </row>
@@ -9723,54 +9765,54 @@
         <v>0</v>
       </c>
       <c r="I165" s="145">
+        <f t="shared" si="40"/>
+        <v>654</v>
+      </c>
+      <c r="J165" s="45">
+        <f t="shared" si="41"/>
+        <v>0</v>
+      </c>
+      <c r="K165" s="46">
         <f t="shared" si="39"/>
-        <v>654</v>
-      </c>
-      <c r="J165" s="45">
-        <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="K165" s="46">
-        <f t="shared" si="38"/>
         <v>0.15991471215351813</v>
       </c>
       <c r="L165" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0.30013106159895153</v>
       </c>
       <c r="M165" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>4.6736191579760528E-2</v>
       </c>
       <c r="N165" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="O165" s="48">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0.14267015706806283</v>
       </c>
       <c r="P165">
         <v>31</v>
       </c>
       <c r="Q165" s="217">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>858000</v>
       </c>
       <c r="S165">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>933567.12328767125</v>
       </c>
       <c r="T165">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>75567.123287671246</v>
       </c>
       <c r="U165">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>37783.561643835623</v>
       </c>
       <c r="V165">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>2.2151138837735805E-2</v>
       </c>
     </row>
@@ -9798,54 +9840,54 @@
         <v>0</v>
       </c>
       <c r="I166" s="145">
+        <f t="shared" si="40"/>
+        <v>439</v>
+      </c>
+      <c r="J166" s="45">
+        <f t="shared" si="41"/>
+        <v>0</v>
+      </c>
+      <c r="K166" s="46">
         <f t="shared" si="39"/>
-        <v>439</v>
-      </c>
-      <c r="J166" s="45">
-        <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="K166" s="46">
-        <f t="shared" si="38"/>
         <v>2.5586353944562899E-2</v>
       </c>
       <c r="L166" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>5.3079947575360421E-2</v>
       </c>
       <c r="M166" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0.1336423329470838</v>
       </c>
       <c r="N166" s="46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="O166" s="48">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>9.5767888307155324E-2</v>
       </c>
       <c r="P166">
         <v>30</v>
       </c>
       <c r="Q166" s="217">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>784000</v>
       </c>
       <c r="S166">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>903452.05479452049</v>
       </c>
       <c r="T166">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>119452.05479452049</v>
       </c>
       <c r="U166">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>59726.027397260244</v>
       </c>
       <c r="V166">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>3.5015214753291293E-2</v>
       </c>
     </row>
@@ -9873,53 +9915,53 @@
         <v>0</v>
       </c>
       <c r="I167" s="145">
+        <f t="shared" si="40"/>
+        <v>615</v>
+      </c>
+      <c r="J167" s="49">
+        <f t="shared" si="41"/>
+        <v>0</v>
+      </c>
+      <c r="K167" s="50">
         <f t="shared" si="39"/>
-        <v>615</v>
-      </c>
-      <c r="J167" s="49">
-        <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="K167" s="50">
-        <f t="shared" si="38"/>
         <v>0.42857142857142855</v>
       </c>
       <c r="L167" s="50">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0.17234600262123198</v>
       </c>
       <c r="M167" s="50">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>5.8323677095403634E-2</v>
       </c>
       <c r="N167" s="50">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="O167" s="51">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0.13416230366492146</v>
       </c>
       <c r="P167">
         <v>31</v>
       </c>
       <c r="Q167" s="217">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>985000</v>
       </c>
       <c r="S167">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>933567.12328767125</v>
       </c>
       <c r="T167">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>-51432.876712328754</v>
       </c>
       <c r="U167">
         <v>0</v>
       </c>
       <c r="V167">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
     </row>
@@ -10343,7 +10385,7 @@
         <v>210</v>
       </c>
       <c r="P187">
-        <f t="shared" ref="P187" si="46">O187/N187</f>
+        <f t="shared" ref="P187" si="47">O187/N187</f>
         <v>2157.0066030814378</v>
       </c>
     </row>
@@ -10526,7 +10568,7 @@
         <v>30</v>
       </c>
       <c r="F200" s="11">
-        <f t="shared" ref="F200:F204" si="47">D200/E200 * 60</f>
+        <f t="shared" ref="F200:F204" si="48">D200/E200 * 60</f>
         <v>0.4</v>
       </c>
       <c r="K200">
@@ -10580,7 +10622,7 @@
         <v>30</v>
       </c>
       <c r="F201" s="11">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>0.4</v>
       </c>
       <c r="K201">
@@ -10634,7 +10676,7 @@
         <v>30</v>
       </c>
       <c r="F202" s="11">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>0.4</v>
       </c>
       <c r="K202">
@@ -10688,7 +10730,7 @@
         <v>30</v>
       </c>
       <c r="F203" s="11">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>0.4</v>
       </c>
     </row>
@@ -10706,7 +10748,7 @@
         <v>50</v>
       </c>
       <c r="F204" s="16">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>1.2</v>
       </c>
     </row>
@@ -10789,19 +10831,19 @@
         <v>0</v>
       </c>
       <c r="E209" s="175">
-        <f t="shared" ref="E209:H209" si="48">SUM(E211:E222)</f>
+        <f t="shared" ref="E209:H209" si="49">SUM(E211:E222)</f>
         <v>142.26999999999998</v>
       </c>
       <c r="F209" s="175">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>1232.05</v>
       </c>
       <c r="G209" s="175">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>3316.4900000000002</v>
       </c>
       <c r="H209" s="175">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="I209" s="179">
@@ -10813,19 +10855,19 @@
         <v>0</v>
       </c>
       <c r="K209" s="46">
-        <f t="shared" ref="K209:N209" si="49">E209/$I$209</f>
+        <f t="shared" ref="K209:N209" si="50">E209/$I$209</f>
         <v>3.0329516650642419E-2</v>
       </c>
       <c r="L209" s="46">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>0.26265186609562097</v>
       </c>
       <c r="M209" s="46">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>0.7070186172537366</v>
       </c>
       <c r="N209" s="46">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="O209" s="47">
@@ -10882,19 +10924,19 @@
         <v>0</v>
       </c>
       <c r="K211" s="46">
-        <f t="shared" ref="K211:O222" si="50">IF(E$209&gt;0,E211/E$209,0)</f>
+        <f t="shared" ref="K211:O222" si="51">IF(E$209&gt;0,E211/E$209,0)</f>
         <v>0</v>
       </c>
       <c r="L211" s="46">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>2.329450915141431E-2</v>
       </c>
       <c r="M211" s="46">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>0.10891333910248484</v>
       </c>
       <c r="N211" s="46">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="O211" s="48">
@@ -10925,31 +10967,31 @@
         <v>0</v>
       </c>
       <c r="I212" s="180">
-        <f t="shared" ref="I212:I222" si="51">SUM(D212:H212)</f>
+        <f t="shared" ref="I212:I222" si="52">SUM(D212:H212)</f>
         <v>389.49999999999994</v>
       </c>
       <c r="J212" s="45">
-        <f t="shared" ref="J212:J222" si="52">IF(D$209&gt;0,D212/D$209,0)</f>
+        <f t="shared" ref="J212:J222" si="53">IF(D$209&gt;0,D212/D$209,0)</f>
         <v>0</v>
       </c>
       <c r="K212" s="46">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>0.21613832853025935</v>
       </c>
       <c r="L212" s="46">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>5.6572379367720471E-2</v>
       </c>
       <c r="M212" s="46">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>8.7155396217084916E-2</v>
       </c>
       <c r="N212" s="46">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="O212" s="48">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>8.3034699764006625E-2</v>
       </c>
     </row>
@@ -10976,31 +11018,31 @@
         <v>0</v>
       </c>
       <c r="I213" s="180">
+        <f t="shared" si="52"/>
+        <v>410.40999999999997</v>
+      </c>
+      <c r="J213" s="45">
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+      <c r="K213" s="46">
         <f t="shared" si="51"/>
-        <v>410.40999999999997</v>
-      </c>
-      <c r="J213" s="45">
-        <f t="shared" si="52"/>
-        <v>0</v>
-      </c>
-      <c r="K213" s="46">
-        <f t="shared" si="50"/>
         <v>0.26224783861671469</v>
       </c>
       <c r="L213" s="46">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>9.9833610648918464E-2</v>
       </c>
       <c r="M213" s="46">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>7.5411052045988372E-2</v>
       </c>
       <c r="N213" s="46">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="O213" s="48">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>8.749235206712698E-2</v>
       </c>
     </row>
@@ -11027,31 +11069,31 @@
         <v>0</v>
       </c>
       <c r="I214" s="180">
+        <f t="shared" si="52"/>
+        <v>391.55</v>
+      </c>
+      <c r="J214" s="45">
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+      <c r="K214" s="46">
         <f t="shared" si="51"/>
-        <v>391.55</v>
-      </c>
-      <c r="J214" s="45">
-        <f t="shared" si="52"/>
-        <v>0</v>
-      </c>
-      <c r="K214" s="46">
-        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="L214" s="46">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>5.9900166389351084E-2</v>
       </c>
       <c r="M214" s="46">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>9.5809123501050808E-2</v>
       </c>
       <c r="N214" s="46">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="O214" s="48">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>8.3471724499606673E-2</v>
       </c>
     </row>
@@ -11078,31 +11120,31 @@
         <v>0</v>
       </c>
       <c r="I215" s="180">
+        <f t="shared" si="52"/>
+        <v>403.85</v>
+      </c>
+      <c r="J215" s="45">
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+      <c r="K215" s="46">
         <f t="shared" si="51"/>
-        <v>403.85</v>
-      </c>
-      <c r="J215" s="45">
-        <f t="shared" si="52"/>
-        <v>0</v>
-      </c>
-      <c r="K215" s="46">
-        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="L215" s="46">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>7.8202995008319467E-2</v>
       </c>
       <c r="M215" s="46">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>9.2718506613920129E-2</v>
       </c>
       <c r="N215" s="46">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="O215" s="48">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>8.6093872913206887E-2</v>
       </c>
     </row>
@@ -11129,31 +11171,31 @@
         <v>0</v>
       </c>
       <c r="I216" s="180">
+        <f t="shared" si="52"/>
+        <v>395.65</v>
+      </c>
+      <c r="J216" s="45">
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+      <c r="K216" s="46">
         <f t="shared" si="51"/>
-        <v>395.65</v>
-      </c>
-      <c r="J216" s="45">
-        <f t="shared" si="52"/>
-        <v>0</v>
-      </c>
-      <c r="K216" s="46">
-        <f t="shared" si="50"/>
         <v>2.0172910662824207E-2</v>
       </c>
       <c r="L216" s="46">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>0.11813643926788685</v>
       </c>
       <c r="M216" s="46">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>7.454567931759179E-2</v>
       </c>
       <c r="N216" s="46">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="O216" s="48">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>8.4345773970806739E-2</v>
       </c>
       <c r="T216" t="s">
@@ -11183,31 +11225,31 @@
         <v>0</v>
       </c>
       <c r="I217" s="180">
+        <f t="shared" si="52"/>
+        <v>215.25</v>
+      </c>
+      <c r="J217" s="45">
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+      <c r="K217" s="46">
         <f t="shared" si="51"/>
-        <v>215.25</v>
-      </c>
-      <c r="J217" s="45">
-        <f t="shared" si="52"/>
-        <v>0</v>
-      </c>
-      <c r="K217" s="46">
-        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="L217" s="46">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>7.4875207986688855E-2</v>
       </c>
       <c r="M217" s="46">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>3.7087402645568049E-2</v>
       </c>
       <c r="N217" s="46">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="O217" s="48">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>4.5887597238003668E-2</v>
       </c>
     </row>
@@ -11234,31 +11276,31 @@
         <v>0</v>
       </c>
       <c r="I218" s="180">
+        <f t="shared" si="52"/>
+        <v>436.65</v>
+      </c>
+      <c r="J218" s="45">
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+      <c r="K218" s="46">
         <f t="shared" si="51"/>
-        <v>436.65</v>
-      </c>
-      <c r="J218" s="45">
-        <f t="shared" si="52"/>
-        <v>0</v>
-      </c>
-      <c r="K218" s="46">
-        <f t="shared" si="50"/>
         <v>8.645533141210375E-2</v>
       </c>
       <c r="L218" s="46">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>0.11148086522462562</v>
       </c>
       <c r="M218" s="46">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>8.6537272839658785E-2</v>
       </c>
       <c r="N218" s="46">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="O218" s="48">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>9.3086268682807435E-2</v>
       </c>
     </row>
@@ -11285,31 +11327,31 @@
         <v>0</v>
       </c>
       <c r="I219" s="180">
+        <f t="shared" si="52"/>
+        <v>430.09000000000003</v>
+      </c>
+      <c r="J219" s="45">
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+      <c r="K219" s="46">
         <f t="shared" si="51"/>
-        <v>430.09000000000003</v>
-      </c>
-      <c r="J219" s="45">
-        <f t="shared" si="52"/>
-        <v>0</v>
-      </c>
-      <c r="K219" s="46">
-        <f t="shared" si="50"/>
         <v>6.9164265129683003E-2</v>
       </c>
       <c r="L219" s="46">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>9.1514143094841932E-2</v>
       </c>
       <c r="M219" s="46">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>9.2718506613920129E-2</v>
       </c>
       <c r="N219" s="46">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="O219" s="48">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>9.1687789528887328E-2</v>
       </c>
     </row>
@@ -11336,31 +11378,31 @@
         <v>0</v>
       </c>
       <c r="I220" s="180">
+        <f t="shared" si="52"/>
+        <v>426.4</v>
+      </c>
+      <c r="J220" s="45">
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+      <c r="K220" s="46">
         <f t="shared" si="51"/>
-        <v>426.4</v>
-      </c>
-      <c r="J220" s="45">
-        <f t="shared" si="52"/>
-        <v>0</v>
-      </c>
-      <c r="K220" s="46">
-        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="L220" s="46">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>0.1098169717138103</v>
       </c>
       <c r="M220" s="46">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>8.7773519594511046E-2</v>
       </c>
       <c r="N220" s="46">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="O220" s="48">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>9.0901145004807254E-2</v>
       </c>
     </row>
@@ -11387,31 +11429,31 @@
         <v>0</v>
       </c>
       <c r="I221" s="180">
+        <f t="shared" si="52"/>
+        <v>410</v>
+      </c>
+      <c r="J221" s="45">
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+      <c r="K221" s="46">
         <f t="shared" si="51"/>
-        <v>410</v>
-      </c>
-      <c r="J221" s="45">
-        <f t="shared" si="52"/>
-        <v>0</v>
-      </c>
-      <c r="K221" s="46">
-        <f t="shared" si="50"/>
         <v>0.1729106628242075</v>
       </c>
       <c r="L221" s="46">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>7.9866888519134774E-2</v>
       </c>
       <c r="M221" s="46">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>8.6537272839658785E-2</v>
       </c>
       <c r="N221" s="46">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="O221" s="48">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>8.7404947120006987E-2</v>
       </c>
     </row>
@@ -11438,31 +11480,31 @@
         <v>0</v>
       </c>
       <c r="I222" s="181">
+        <f t="shared" si="52"/>
+        <v>391.54999999999995</v>
+      </c>
+      <c r="J222" s="49">
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+      <c r="K222" s="50">
         <f t="shared" si="51"/>
-        <v>391.54999999999995</v>
-      </c>
-      <c r="J222" s="49">
-        <f t="shared" si="52"/>
-        <v>0</v>
-      </c>
-      <c r="K222" s="50">
-        <f t="shared" si="50"/>
         <v>0.1729106628242075</v>
       </c>
       <c r="L222" s="50">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>9.6505823627287851E-2</v>
       </c>
       <c r="M222" s="50">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>7.4792928668562228E-2</v>
       </c>
       <c r="N222" s="50">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="O222" s="51">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>8.3471724499606659E-2</v>
       </c>
     </row>
@@ -11925,7 +11967,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>

</xml_diff>